<commit_message>
nuevos casos, agurpar partidos en torta
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="264">
   <si>
     <t>Caso</t>
   </si>
@@ -1104,6 +1104,96 @@
   </si>
   <si>
     <t xml:space="preserve">Estación Central </t>
+  </si>
+  <si>
+    <t>Caso Main, alcaldesa de Antofagasta (Karen Rojo)</t>
+  </si>
+  <si>
+    <t>Karen Rojo</t>
+  </si>
+  <si>
+    <t>Independiente</t>
+  </si>
+  <si>
+    <t>Condenada</t>
+  </si>
+  <si>
+    <t>condenada a cinco años y un día de presidio mayor en su grado mínimo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Mostazal (Sergio Medel)</t>
+  </si>
+  <si>
+    <t>Sergio Medel</t>
+  </si>
+  <si>
+    <t>Mostazal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2435,7 +2525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V53"/>
+  <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -2836,10 +2926,10 @@
         <v>59</v>
       </c>
       <c r="G9" s="16">
+        <v>2017</v>
+      </c>
+      <c r="H9" s="16">
         <v>2020</v>
-      </c>
-      <c r="H9" s="16">
-        <v>2021</v>
       </c>
       <c r="I9" t="s" s="17">
         <v>60</v>
@@ -4828,8 +4918,116 @@
       <c r="U53" s="21"/>
       <c r="V53" s="21"/>
     </row>
+    <row r="54" ht="56.05" customHeight="1">
+      <c r="A54" t="s" s="14">
+        <v>250</v>
+      </c>
+      <c r="B54" s="15">
+        <v>24000000</v>
+      </c>
+      <c r="C54" s="16">
+        <v>2022</v>
+      </c>
+      <c r="D54" t="s" s="17">
+        <v>251</v>
+      </c>
+      <c r="E54" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="F54" t="s" s="17">
+        <v>252</v>
+      </c>
+      <c r="G54" s="16">
+        <v>2015</v>
+      </c>
+      <c r="H54" s="16">
+        <v>2016</v>
+      </c>
+      <c r="I54" t="s" s="17">
+        <v>162</v>
+      </c>
+      <c r="J54" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" t="s" s="19">
+        <v>143</v>
+      </c>
+      <c r="O54" s="21"/>
+      <c r="P54" t="s" s="19">
+        <v>253</v>
+      </c>
+      <c r="Q54" t="s" s="17">
+        <v>254</v>
+      </c>
+      <c r="R54" t="s" s="19">
+        <v>255</v>
+      </c>
+      <c r="S54" t="s" s="19">
+        <v>256</v>
+      </c>
+      <c r="T54" t="s" s="19">
+        <v>257</v>
+      </c>
+      <c r="U54" s="21"/>
+      <c r="V54" s="21"/>
+    </row>
+    <row r="55" ht="20.05" customHeight="1">
+      <c r="A55" t="s" s="14">
+        <v>258</v>
+      </c>
+      <c r="B55" s="15">
+        <v>200000000</v>
+      </c>
+      <c r="C55" s="16">
+        <v>2022</v>
+      </c>
+      <c r="D55" t="s" s="17">
+        <v>259</v>
+      </c>
+      <c r="E55" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="F55" t="s" s="17">
+        <v>30</v>
+      </c>
+      <c r="G55" s="16">
+        <v>2008</v>
+      </c>
+      <c r="H55" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I55" t="s" s="17">
+        <v>260</v>
+      </c>
+      <c r="J55" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K55" s="18"/>
+      <c r="L55" t="s" s="17">
+        <v>33</v>
+      </c>
+      <c r="M55" s="18"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="21"/>
+      <c r="Q55" s="18"/>
+      <c r="R55" t="s" s="19">
+        <v>261</v>
+      </c>
+      <c r="S55" t="s" s="19">
+        <v>262</v>
+      </c>
+      <c r="T55" t="s" s="19">
+        <v>263</v>
+      </c>
+      <c r="U55" s="21"/>
+      <c r="V55" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53 E53 G53:H53">
+  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53:C55 E53:E55 G53:H55">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -4897,6 +5095,12 @@
     <hyperlink ref="S50" r:id="rId57" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
     <hyperlink ref="R51" r:id="rId58" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
     <hyperlink ref="R53" r:id="rId59" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R54" r:id="rId60" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
+    <hyperlink ref="S54" r:id="rId61" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
+    <hyperlink ref="T54" r:id="rId62" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
+    <hyperlink ref="R55" r:id="rId63" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
+    <hyperlink ref="S55" r:id="rId64" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
+    <hyperlink ref="T55" r:id="rId65" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
fuente en caso la florida
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="265">
   <si>
     <t>Caso</t>
   </si>
@@ -406,6 +406,17 @@
   </si>
   <si>
     <t>La Florida</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.elmostrador.cl/destacado/2023/02/06/los-2-500-millones-de-la-corporacion-municipal-de-la-florida-que-carter-no-termina-de-explicar/</t>
+    </r>
   </si>
   <si>
     <t>Caso Fundaciones (Arica)</t>
@@ -3246,7 +3257,9 @@
       <c r="O16" s="20"/>
       <c r="P16" s="21"/>
       <c r="Q16" s="18"/>
-      <c r="R16" s="21"/>
+      <c r="R16" t="s" s="19">
+        <v>92</v>
+      </c>
       <c r="S16" s="21"/>
       <c r="T16" s="21"/>
       <c r="U16" s="21"/>
@@ -3254,7 +3267,7 @@
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="14">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B17" s="15">
         <v>2500000000</v>
@@ -3270,7 +3283,7 @@
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
       <c r="I17" t="s" s="17">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s" s="17">
         <v>14</v>
@@ -3280,7 +3293,7 @@
       <c r="M17" s="18"/>
       <c r="N17" s="21"/>
       <c r="O17" t="s" s="23">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P17" s="21"/>
       <c r="Q17" s="18"/>
@@ -3288,7 +3301,7 @@
         <v>76</v>
       </c>
       <c r="S17" t="s" s="19">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T17" s="21"/>
       <c r="U17" s="21"/>
@@ -3296,7 +3309,7 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="14">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B18" s="15">
         <v>2300000000</v>
@@ -3305,7 +3318,7 @@
         <v>2003</v>
       </c>
       <c r="D18" t="s" s="17">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E18" t="s" s="17">
         <v>29</v>
@@ -3316,7 +3329,7 @@
       <c r="G18" s="18"/>
       <c r="H18" s="18"/>
       <c r="I18" t="s" s="17">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J18" t="s" s="17">
         <v>32</v>
@@ -3327,7 +3340,7 @@
       </c>
       <c r="M18" s="18"/>
       <c r="N18" t="s" s="19">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O18" s="20"/>
       <c r="P18" s="21"/>
@@ -3335,22 +3348,22 @@
         <v>35</v>
       </c>
       <c r="R18" t="s" s="19">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S18" t="s" s="19">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T18" t="s" s="19">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U18" t="s" s="19">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="V18" s="21"/>
     </row>
     <row r="19" ht="32.05" customHeight="1">
       <c r="A19" t="s" s="14">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B19" s="15">
         <v>2113000000</v>
@@ -3359,18 +3372,18 @@
         <v>2023</v>
       </c>
       <c r="D19" t="s" s="17">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E19" t="s" s="17">
         <v>29</v>
       </c>
       <c r="F19" t="s" s="17">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" t="s" s="17">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J19" t="s" s="17">
         <v>14</v>
@@ -3380,15 +3393,15 @@
       <c r="M19" s="18"/>
       <c r="N19" s="21"/>
       <c r="O19" t="s" s="23">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P19" s="21"/>
       <c r="Q19" s="18"/>
       <c r="R19" t="s" s="19">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S19" t="s" s="19">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="T19" s="21"/>
       <c r="U19" s="21"/>
@@ -3396,7 +3409,7 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="14">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B20" s="15">
         <v>1700000000</v>
@@ -3418,20 +3431,20 @@
         <v>39</v>
       </c>
       <c r="K20" t="s" s="17">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" t="s" s="17">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N20" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O20" s="20"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="18"/>
       <c r="R20" t="s" s="19">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="S20" s="21"/>
       <c r="T20" s="21"/>
@@ -3440,7 +3453,7 @@
     </row>
     <row r="21" ht="32.05" customHeight="1">
       <c r="A21" t="s" s="14">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B21" s="15">
         <v>1673754000</v>
@@ -3449,7 +3462,7 @@
         <v>2019</v>
       </c>
       <c r="D21" t="s" s="17">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E21" t="s" s="17">
         <v>29</v>
@@ -3460,7 +3473,7 @@
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
       <c r="I21" t="s" s="17">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J21" t="s" s="17">
         <v>32</v>
@@ -3482,7 +3495,7 @@
     </row>
     <row r="22" ht="32.05" customHeight="1">
       <c r="A22" t="s" s="14">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B22" s="15">
         <v>1659000000</v>
@@ -3491,7 +3504,7 @@
         <v>2017</v>
       </c>
       <c r="D22" t="s" s="17">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s" s="17">
         <v>23</v>
@@ -3506,22 +3519,22 @@
         <v>39</v>
       </c>
       <c r="K22" t="s" s="17">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="L22" t="s" s="17">
         <v>33</v>
       </c>
       <c r="M22" t="s" s="17">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N22" t="s" s="19">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O22" s="20"/>
       <c r="P22" s="21"/>
       <c r="Q22" s="18"/>
       <c r="R22" t="s" s="19">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="S22" s="21"/>
       <c r="T22" s="21"/>
@@ -3530,7 +3543,7 @@
     </row>
     <row r="23" ht="32.05" customHeight="1">
       <c r="A23" t="s" s="14">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B23" s="15">
         <v>1500000000</v>
@@ -3539,7 +3552,7 @@
         <v>2018</v>
       </c>
       <c r="D23" t="s" s="17">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E23" t="s" s="17">
         <v>29</v>
@@ -3550,7 +3563,7 @@
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
       <c r="I23" t="s" s="17">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J23" t="s" s="17">
         <v>32</v>
@@ -3561,7 +3574,7 @@
       </c>
       <c r="M23" s="18"/>
       <c r="N23" t="s" s="19">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O23" s="20"/>
       <c r="P23" s="21"/>
@@ -3576,7 +3589,7 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="14">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B24" s="15">
         <v>1253000000</v>
@@ -3589,7 +3602,7 @@
         <v>58</v>
       </c>
       <c r="F24" t="s" s="17">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G24" s="16">
         <v>1997</v>
@@ -3610,7 +3623,7 @@
         <v>87</v>
       </c>
       <c r="S24" t="s" s="19">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="T24" s="21"/>
       <c r="U24" s="21"/>
@@ -3618,7 +3631,7 @@
     </row>
     <row r="25" ht="32.05" customHeight="1">
       <c r="A25" t="s" s="14">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B25" s="15">
         <v>1100000000</v>
@@ -3627,7 +3640,7 @@
         <v>2022</v>
       </c>
       <c r="D25" t="s" s="17">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E25" t="s" s="17">
         <v>29</v>
@@ -3642,7 +3655,7 @@
         <v>2023</v>
       </c>
       <c r="I25" t="s" s="17">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J25" t="s" s="17">
         <v>32</v>
@@ -3657,7 +3670,7 @@
       <c r="P25" s="21"/>
       <c r="Q25" s="18"/>
       <c r="R25" t="s" s="19">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="S25" s="21"/>
       <c r="T25" s="21"/>
@@ -3666,7 +3679,7 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="14">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B26" s="15">
         <v>1000000000</v>
@@ -3675,7 +3688,7 @@
         <v>2023</v>
       </c>
       <c r="D26" t="s" s="17">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E26" t="s" s="17">
         <v>29</v>
@@ -3686,7 +3699,7 @@
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
       <c r="I26" t="s" s="17">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J26" t="s" s="17">
         <v>32</v>
@@ -3701,7 +3714,7 @@
       <c r="P26" s="21"/>
       <c r="Q26" s="18"/>
       <c r="R26" t="s" s="19">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="S26" s="21"/>
       <c r="T26" s="21"/>
@@ -3710,7 +3723,7 @@
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="14">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B27" s="15">
         <v>946000000</v>
@@ -3723,7 +3736,7 @@
         <v>58</v>
       </c>
       <c r="F27" t="s" s="17">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G27" s="18"/>
       <c r="H27" s="18"/>
@@ -3746,7 +3759,7 @@
     </row>
     <row r="28" ht="32.05" customHeight="1">
       <c r="A28" t="s" s="14">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B28" s="15">
         <v>750000000</v>
@@ -3755,7 +3768,7 @@
         <v>2023</v>
       </c>
       <c r="D28" t="s" s="17">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E28" t="s" s="17">
         <v>29</v>
@@ -3770,7 +3783,7 @@
         <v>2015</v>
       </c>
       <c r="I28" t="s" s="17">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J28" t="s" s="17">
         <v>32</v>
@@ -3779,17 +3792,17 @@
       <c r="L28" s="18"/>
       <c r="M28" s="18"/>
       <c r="N28" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O28" s="20"/>
       <c r="P28" t="s" s="19">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Q28" t="s" s="19">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R28" t="s" s="19">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
@@ -3798,7 +3811,7 @@
     </row>
     <row r="29" ht="32.05" customHeight="1">
       <c r="A29" t="s" s="14">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B29" s="15">
         <v>680000000</v>
@@ -3807,7 +3820,7 @@
         <v>2018</v>
       </c>
       <c r="D29" t="s" s="17">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s" s="17">
         <v>29</v>
@@ -3818,7 +3831,7 @@
       <c r="G29" s="18"/>
       <c r="H29" s="18"/>
       <c r="I29" t="s" s="17">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J29" t="s" s="17">
         <v>32</v>
@@ -3829,26 +3842,26 @@
       </c>
       <c r="M29" s="18"/>
       <c r="N29" t="s" s="19">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O29" s="20"/>
       <c r="P29" s="21"/>
       <c r="Q29" s="18"/>
       <c r="R29" t="s" s="19">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="S29" t="s" s="19">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="T29" t="s" s="19">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
     </row>
     <row r="30" ht="32.05" customHeight="1">
       <c r="A30" t="s" s="14">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B30" s="15">
         <v>658000000</v>
@@ -3857,18 +3870,18 @@
         <v>2023</v>
       </c>
       <c r="D30" t="s" s="17">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s" s="17">
         <v>29</v>
       </c>
       <c r="F30" t="s" s="17">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" t="s" s="17">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J30" t="s" s="17">
         <v>14</v>
@@ -3877,10 +3890,10 @@
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
       <c r="N30" t="s" s="19">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O30" t="s" s="23">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="P30" s="21"/>
       <c r="Q30" s="18"/>
@@ -3888,7 +3901,7 @@
         <v>76</v>
       </c>
       <c r="S30" t="s" s="19">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="T30" s="21"/>
       <c r="U30" s="21"/>
@@ -3896,7 +3909,7 @@
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="14">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B31" s="15">
         <v>577000000</v>
@@ -3909,12 +3922,12 @@
         <v>58</v>
       </c>
       <c r="F31" t="s" s="17">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" t="s" s="17">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J31" t="s" s="17">
         <v>14</v>
@@ -3938,7 +3951,7 @@
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="14">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B32" s="15">
         <v>426000000</v>
@@ -3951,12 +3964,12 @@
         <v>58</v>
       </c>
       <c r="F32" t="s" s="17">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
       <c r="I32" t="s" s="17">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J32" t="s" s="17">
         <v>14</v>
@@ -3966,7 +3979,7 @@
       <c r="M32" s="18"/>
       <c r="N32" s="21"/>
       <c r="O32" t="s" s="23">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="P32" s="21"/>
       <c r="Q32" s="18"/>
@@ -3980,7 +3993,7 @@
     </row>
     <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="14">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B33" s="15">
         <v>293093681</v>
@@ -3989,13 +4002,13 @@
         <v>2023</v>
       </c>
       <c r="D33" t="s" s="17">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E33" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F33" t="s" s="17">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -4005,13 +4018,13 @@
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
       <c r="N33" t="s" s="19">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
       <c r="R33" t="s" s="19">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
@@ -4020,7 +4033,7 @@
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="14">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B34" s="15">
         <v>289350646</v>
@@ -4029,7 +4042,7 @@
         <v>2018</v>
       </c>
       <c r="D34" t="s" s="17">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E34" t="s" s="17">
         <v>29</v>
@@ -4040,7 +4053,7 @@
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" t="s" s="17">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J34" t="s" s="17">
         <v>32</v>
@@ -4062,7 +4075,7 @@
     </row>
     <row r="35" ht="32.05" customHeight="1">
       <c r="A35" t="s" s="14">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" s="15">
         <v>283000000</v>
@@ -4071,7 +4084,7 @@
         <v>2017</v>
       </c>
       <c r="D35" t="s" s="17">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E35" t="s" s="17">
         <v>58</v>
@@ -4086,28 +4099,28 @@
         <v>2017</v>
       </c>
       <c r="I35" t="s" s="17">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="J35" t="s" s="17">
         <v>32</v>
       </c>
       <c r="K35" t="s" s="17">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L35" t="s" s="17">
         <v>33</v>
       </c>
       <c r="M35" t="s" s="17">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="N35" t="s" s="19">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="O35" s="20"/>
       <c r="P35" s="21"/>
       <c r="Q35" s="18"/>
       <c r="R35" t="s" s="19">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
@@ -4116,7 +4129,7 @@
     </row>
     <row r="36" ht="32.05" customHeight="1">
       <c r="A36" t="s" s="14">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B36" s="15">
         <v>274000000</v>
@@ -4132,7 +4145,7 @@
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" t="s" s="17">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J36" t="s" s="17">
         <v>14</v>
@@ -4142,7 +4155,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="21"/>
       <c r="O36" t="s" s="23">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="P36" s="21"/>
       <c r="Q36" s="18"/>
@@ -4156,7 +4169,7 @@
     </row>
     <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="14">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B37" s="15">
         <v>262000000</v>
@@ -4165,19 +4178,19 @@
         <v>2006</v>
       </c>
       <c r="D37" t="s" s="17">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E37" t="s" s="17">
         <v>23</v>
       </c>
       <c r="F37" t="s" s="17">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
       <c r="J37" t="s" s="17">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
@@ -4194,7 +4207,7 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="14">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B38" s="15">
         <v>203000000</v>
@@ -4203,7 +4216,7 @@
         <v>2018</v>
       </c>
       <c r="D38" t="s" s="17">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E38" t="s" s="17">
         <v>29</v>
@@ -4214,7 +4227,7 @@
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" t="s" s="17">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J38" t="s" s="17">
         <v>32</v>
@@ -4229,7 +4242,7 @@
       <c r="P38" s="21"/>
       <c r="Q38" s="18"/>
       <c r="R38" t="s" s="19">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="S38" t="s" s="19">
         <v>68</v>
@@ -4240,7 +4253,7 @@
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="14">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B39" s="15">
         <v>200000000</v>
@@ -4249,7 +4262,7 @@
         <v>2012</v>
       </c>
       <c r="D39" t="s" s="17">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E39" t="s" s="17">
         <v>29</v>
@@ -4265,24 +4278,24 @@
       </c>
       <c r="I39" s="18"/>
       <c r="J39" t="s" s="17">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
       <c r="N39" t="s" s="19">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="21"/>
       <c r="Q39" t="s" s="17">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="R39" t="s" s="19">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="S39" t="s" s="19">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T39" s="21"/>
       <c r="U39" s="21"/>
@@ -4290,7 +4303,7 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="14">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B40" s="15">
         <v>190000000</v>
@@ -4299,7 +4312,7 @@
         <v>2024</v>
       </c>
       <c r="D40" t="s" s="17">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E40" t="s" s="17">
         <v>29</v>
@@ -4310,7 +4323,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" t="s" s="17">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="J40" t="s" s="17">
         <v>32</v>
@@ -4319,13 +4332,13 @@
       <c r="L40" s="18"/>
       <c r="M40" s="18"/>
       <c r="N40" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O40" s="20"/>
       <c r="P40" s="21"/>
       <c r="Q40" s="21"/>
       <c r="R40" t="s" s="19">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S40" s="21"/>
       <c r="T40" s="21"/>
@@ -4334,7 +4347,7 @@
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="14">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B41" s="15">
         <v>188000000</v>
@@ -4343,7 +4356,7 @@
         <v>2021</v>
       </c>
       <c r="D41" t="s" s="17">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s" s="17">
         <v>29</v>
@@ -4354,7 +4367,7 @@
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" t="s" s="17">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J41" t="s" s="17">
         <v>32</v>
@@ -4376,7 +4389,7 @@
     </row>
     <row r="42" ht="44.05" customHeight="1">
       <c r="A42" t="s" s="14">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B42" s="15">
         <v>176000000</v>
@@ -4385,7 +4398,7 @@
         <v>2024</v>
       </c>
       <c r="D42" t="s" s="17">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E42" t="s" s="17">
         <v>29</v>
@@ -4400,7 +4413,7 @@
         <v>2021</v>
       </c>
       <c r="I42" t="s" s="17">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J42" t="s" s="17">
         <v>32</v>
@@ -4411,20 +4424,20 @@
       </c>
       <c r="M42" s="18"/>
       <c r="N42" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O42" s="20"/>
       <c r="P42" t="s" s="19">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="Q42" t="s" s="17">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="R42" t="s" s="19">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="S42" t="s" s="19">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="T42" s="21"/>
       <c r="U42" s="21"/>
@@ -4432,7 +4445,7 @@
     </row>
     <row r="43" ht="32.05" customHeight="1">
       <c r="A43" t="s" s="14">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B43" s="15">
         <v>150000000</v>
@@ -4441,7 +4454,7 @@
         <v>2021</v>
       </c>
       <c r="D43" t="s" s="17">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E43" t="s" s="17">
         <v>29</v>
@@ -4452,7 +4465,7 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" t="s" s="17">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="J43" t="s" s="17">
         <v>32</v>
@@ -4467,10 +4480,10 @@
       <c r="P43" s="21"/>
       <c r="Q43" s="18"/>
       <c r="R43" t="s" s="19">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="S43" t="s" s="19">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="T43" s="21"/>
       <c r="U43" s="21"/>
@@ -4478,7 +4491,7 @@
     </row>
     <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="14">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B44" s="15">
         <v>148000000</v>
@@ -4494,7 +4507,7 @@
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
       <c r="I44" t="s" s="17">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="J44" t="s" s="17">
         <v>14</v>
@@ -4504,7 +4517,7 @@
       <c r="M44" s="18"/>
       <c r="N44" s="21"/>
       <c r="O44" t="s" s="23">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="P44" s="21"/>
       <c r="Q44" s="18"/>
@@ -4518,7 +4531,7 @@
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="14">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B45" s="15">
         <v>128000000</v>
@@ -4531,12 +4544,12 @@
         <v>58</v>
       </c>
       <c r="F45" t="s" s="17">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
       <c r="I45" t="s" s="17">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J45" t="s" s="17">
         <v>14</v>
@@ -4546,7 +4559,7 @@
       <c r="M45" s="18"/>
       <c r="N45" s="21"/>
       <c r="O45" t="s" s="23">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="P45" s="21"/>
       <c r="Q45" s="18"/>
@@ -4554,7 +4567,7 @@
         <v>76</v>
       </c>
       <c r="S45" t="s" s="19">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="T45" s="21"/>
       <c r="U45" s="21"/>
@@ -4562,7 +4575,7 @@
     </row>
     <row r="46" ht="32.05" customHeight="1">
       <c r="A46" t="s" s="14">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B46" s="15">
         <v>59595096</v>
@@ -4571,7 +4584,7 @@
         <v>2020</v>
       </c>
       <c r="D46" t="s" s="17">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E46" t="s" s="17">
         <v>29</v>
@@ -4604,7 +4617,7 @@
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="14">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B47" s="15">
         <v>40000000</v>
@@ -4624,7 +4637,7 @@
         <v>2013</v>
       </c>
       <c r="I47" t="s" s="17">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J47" t="s" s="17">
         <v>39</v>
@@ -4637,7 +4650,7 @@
       <c r="P47" s="21"/>
       <c r="Q47" s="18"/>
       <c r="R47" t="s" s="19">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="S47" s="21"/>
       <c r="T47" s="21"/>
@@ -4646,7 +4659,7 @@
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="14">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B48" s="15">
         <v>35000000</v>
@@ -4655,13 +4668,13 @@
         <v>2002</v>
       </c>
       <c r="D48" t="s" s="17">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E48" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F48" t="s" s="17">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -4671,18 +4684,18 @@
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
       <c r="N48" t="s" s="19">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="O48" s="21"/>
       <c r="P48" s="21"/>
       <c r="Q48" t="s" s="17">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="R48" t="s" s="19">
         <v>87</v>
       </c>
       <c r="S48" t="s" s="19">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="T48" s="21"/>
       <c r="U48" s="21"/>
@@ -4690,7 +4703,7 @@
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="14">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B49" s="15">
         <v>30000000</v>
@@ -4699,7 +4712,7 @@
         <v>2009</v>
       </c>
       <c r="D49" t="s" s="17">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E49" t="s" s="17">
         <v>29</v>
@@ -4713,7 +4726,7 @@
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" t="s" s="17">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
@@ -4723,7 +4736,7 @@
       <c r="P49" s="21"/>
       <c r="Q49" s="18"/>
       <c r="R49" t="s" s="19">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="S49" s="21"/>
       <c r="T49" s="21"/>
@@ -4732,7 +4745,7 @@
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="14">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B50" s="15">
         <v>23671000</v>
@@ -4741,13 +4754,13 @@
         <v>2008</v>
       </c>
       <c r="D50" t="s" s="17">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E50" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F50" t="s" s="17">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G50" s="16">
         <v>2004</v>
@@ -4761,7 +4774,7 @@
       <c r="L50" s="18"/>
       <c r="M50" s="18"/>
       <c r="N50" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O50" s="20"/>
       <c r="P50" s="21"/>
@@ -4770,7 +4783,7 @@
         <v>87</v>
       </c>
       <c r="S50" t="s" s="19">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="T50" s="21"/>
       <c r="U50" s="21"/>
@@ -4778,7 +4791,7 @@
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="14">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B51" s="15">
         <v>15700000</v>
@@ -4787,7 +4800,7 @@
         <v>2015</v>
       </c>
       <c r="D51" t="s" s="17">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E51" t="s" s="17">
         <v>29</v>
@@ -4798,7 +4811,7 @@
       <c r="G51" s="18"/>
       <c r="H51" s="18"/>
       <c r="I51" t="s" s="17">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J51" t="s" s="17">
         <v>32</v>
@@ -4812,7 +4825,7 @@
       <c r="O51" s="21"/>
       <c r="P51" s="21"/>
       <c r="Q51" t="s" s="17">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="R51" t="s" s="19">
         <v>68</v>
@@ -4824,7 +4837,7 @@
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="14">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B52" s="15">
         <v>10333332</v>
@@ -4833,7 +4846,7 @@
         <v>2024</v>
       </c>
       <c r="D52" t="s" s="17">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E52" t="s" s="17">
         <v>29</v>
@@ -4848,7 +4861,7 @@
         <v>2024</v>
       </c>
       <c r="I52" t="s" s="17">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J52" t="s" s="17">
         <v>32</v>
@@ -4859,7 +4872,7 @@
       </c>
       <c r="M52" s="18"/>
       <c r="N52" t="s" s="19">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O52" s="20"/>
       <c r="P52" t="s" s="19">
@@ -4867,10 +4880,10 @@
       </c>
       <c r="Q52" s="18"/>
       <c r="R52" t="s" s="19">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="S52" t="s" s="19">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="T52" s="21"/>
       <c r="U52" s="21"/>
@@ -4878,7 +4891,7 @@
     </row>
     <row r="53" ht="32.05" customHeight="1">
       <c r="A53" t="s" s="14">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B53" s="15">
         <v>10000000</v>
@@ -4887,7 +4900,7 @@
         <v>2015</v>
       </c>
       <c r="D53" t="s" s="17">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E53" t="s" s="17">
         <v>29</v>
@@ -4898,7 +4911,7 @@
       <c r="G53" s="18"/>
       <c r="H53" s="18"/>
       <c r="I53" t="s" s="17">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J53" t="s" s="17">
         <v>32</v>
@@ -4920,7 +4933,7 @@
     </row>
     <row r="54" ht="56.05" customHeight="1">
       <c r="A54" t="s" s="14">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B54" s="15">
         <v>24000000</v>
@@ -4929,13 +4942,13 @@
         <v>2022</v>
       </c>
       <c r="D54" t="s" s="17">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E54" t="s" s="17">
         <v>29</v>
       </c>
       <c r="F54" t="s" s="17">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G54" s="16">
         <v>2015</v>
@@ -4944,7 +4957,7 @@
         <v>2016</v>
       </c>
       <c r="I54" t="s" s="17">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J54" t="s" s="17">
         <v>32</v>
@@ -4953,30 +4966,30 @@
       <c r="L54" s="18"/>
       <c r="M54" s="18"/>
       <c r="N54" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="O54" s="21"/>
       <c r="P54" t="s" s="19">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="Q54" t="s" s="17">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="R54" t="s" s="19">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="S54" t="s" s="19">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="T54" t="s" s="19">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="U54" s="21"/>
       <c r="V54" s="21"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="14">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B55" s="15">
         <v>200000000</v>
@@ -4985,7 +4998,7 @@
         <v>2022</v>
       </c>
       <c r="D55" t="s" s="17">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E55" t="s" s="17">
         <v>29</v>
@@ -5000,7 +5013,7 @@
         <v>2021</v>
       </c>
       <c r="I55" t="s" s="17">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J55" t="s" s="17">
         <v>32</v>
@@ -5015,13 +5028,13 @@
       <c r="P55" s="21"/>
       <c r="Q55" s="18"/>
       <c r="R55" t="s" s="19">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="S55" t="s" s="19">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="T55" t="s" s="19">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
@@ -5048,59 +5061,60 @@
     <hyperlink ref="R14" r:id="rId10" location="" tooltip="" display="https://es.wikipedia.org/wiki/Milicogate"/>
     <hyperlink ref="R15" r:id="rId11" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
     <hyperlink ref="S15" r:id="rId12" location="" tooltip="" display="https://www.df.cl/aniversario/caso-inverlink-el-escandalo-que-amenazo-la-estabilidad-del-mercado"/>
-    <hyperlink ref="R17" r:id="rId13" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="S17" r:id="rId14" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/07/06/1100220/fundacion-el-desarrollo-de-organizaciones.html"/>
-    <hyperlink ref="R18" r:id="rId15" location="" tooltip="" display="https://www.latercera.com/la-tercera-sabado/noticia/cientos-de-depositos-en-efectivo-y-una-cuenta-con-2300-millones-las-pruebas-que-complican-al-tronco-torrealba/LH674LXDYVBR3J5IDIFUCMRIXE/"/>
-    <hyperlink ref="S18" r:id="rId16" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/20/caso-torrealba-detalles-de-gastos-de-campana-de-rn-que-fueron-financiados-con-dineros-de-vitacura/"/>
-    <hyperlink ref="T18" r:id="rId17" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2023/08/08/53-dias-tras-las-rejas-rechazan-solicitud-de-raul-torrealba-y-seguira-en-prision-preventiva/"/>
-    <hyperlink ref="U18" r:id="rId18" location="" tooltip="" display="https://radio.uchile.cl/2023/03/07/diputado-luis-cuello-apunta-a-felipe-guevara-es-sindicado-como-el-ideologo-del-mecanismo-que-permitio-desviar-y-triangular-dineros/"/>
-    <hyperlink ref="S19" r:id="rId19" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml"/>
-    <hyperlink ref="R20" r:id="rId20" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
-    <hyperlink ref="R21" r:id="rId21" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R22" r:id="rId22" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
-    <hyperlink ref="R23" r:id="rId23" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R24" r:id="rId24" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="S24" r:id="rId25" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
-    <hyperlink ref="R25" r:id="rId26" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
-    <hyperlink ref="R26" r:id="rId27" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
-    <hyperlink ref="R27" r:id="rId28" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="R29" r:id="rId29" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
-    <hyperlink ref="S29" r:id="rId30" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
-    <hyperlink ref="T29" r:id="rId31" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
-    <hyperlink ref="R30" r:id="rId32" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="S30" r:id="rId33" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
-    <hyperlink ref="R31" r:id="rId34" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="R32" r:id="rId35" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="R33" r:id="rId36" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
-    <hyperlink ref="R34" r:id="rId37" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R36" r:id="rId38" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="R38" r:id="rId39" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
-    <hyperlink ref="S38" r:id="rId40" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R39" r:id="rId41" location="" tooltip="" display="https://www.diarioconstitucional.cl/2021/04/17/detalles-del-caso-corpesca-tercer-tribunal-de-juicio-oral-en-lo-penal-de-santiago-condeno-al-exsenador-jaime-orpis-a-la-pena-unica-de-5-anos-y-un-dia-de-presidio-efectivo-en-calidad-de-autor-de-seis/"/>
-    <hyperlink ref="S39" r:id="rId42" location="" tooltip="" display="https://contracarga.cl/reportajes/caso-corpesca-explicado/"/>
-    <hyperlink ref="R40" r:id="rId43" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
-    <hyperlink ref="R41" r:id="rId44" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R42" r:id="rId45" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
-    <hyperlink ref="S42" r:id="rId46" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
-    <hyperlink ref="R43" r:id="rId47" location="" tooltip="" display="https://www.biobiochile.cl/especial/bbcl-investiga/noticias/cronicas/2022/02/02/los-millonarios-finiquitos-de-la-era-reginato-los-detalles-de-la-nueva-denuncia-de-ripamonti.shtml"/>
-    <hyperlink ref="S43" r:id="rId48" location="" tooltip="" display="https://www.publimetro.cl/noticias/2022/09/23/100-mil-millones-las-perdidas-de-virginia-reginato-en-municipalidad-de-vina-del-mar/"/>
-    <hyperlink ref="R44" r:id="rId49" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="R45" r:id="rId50" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="S45" r:id="rId51" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
-    <hyperlink ref="R46" r:id="rId52" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R47" r:id="rId53" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
-    <hyperlink ref="R48" r:id="rId54" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="S48" r:id="rId55" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
-    <hyperlink ref="R50" r:id="rId56" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="S50" r:id="rId57" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
-    <hyperlink ref="R51" r:id="rId58" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R53" r:id="rId59" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="R54" r:id="rId60" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
-    <hyperlink ref="S54" r:id="rId61" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
-    <hyperlink ref="T54" r:id="rId62" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
-    <hyperlink ref="R55" r:id="rId63" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
-    <hyperlink ref="S55" r:id="rId64" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
-    <hyperlink ref="T55" r:id="rId65" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
+    <hyperlink ref="R16" r:id="rId13" location="" tooltip="" display="https://www.elmostrador.cl/destacado/2023/02/06/los-2-500-millones-de-la-corporacion-municipal-de-la-florida-que-carter-no-termina-de-explicar/"/>
+    <hyperlink ref="R17" r:id="rId14" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="S17" r:id="rId15" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/07/06/1100220/fundacion-el-desarrollo-de-organizaciones.html"/>
+    <hyperlink ref="R18" r:id="rId16" location="" tooltip="" display="https://www.latercera.com/la-tercera-sabado/noticia/cientos-de-depositos-en-efectivo-y-una-cuenta-con-2300-millones-las-pruebas-que-complican-al-tronco-torrealba/LH674LXDYVBR3J5IDIFUCMRIXE/"/>
+    <hyperlink ref="S18" r:id="rId17" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/20/caso-torrealba-detalles-de-gastos-de-campana-de-rn-que-fueron-financiados-con-dineros-de-vitacura/"/>
+    <hyperlink ref="T18" r:id="rId18" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2023/08/08/53-dias-tras-las-rejas-rechazan-solicitud-de-raul-torrealba-y-seguira-en-prision-preventiva/"/>
+    <hyperlink ref="U18" r:id="rId19" location="" tooltip="" display="https://radio.uchile.cl/2023/03/07/diputado-luis-cuello-apunta-a-felipe-guevara-es-sindicado-como-el-ideologo-del-mecanismo-que-permitio-desviar-y-triangular-dineros/"/>
+    <hyperlink ref="S19" r:id="rId20" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml"/>
+    <hyperlink ref="R20" r:id="rId21" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
+    <hyperlink ref="R21" r:id="rId22" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R22" r:id="rId23" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
+    <hyperlink ref="R23" r:id="rId24" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R24" r:id="rId25" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="S24" r:id="rId26" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
+    <hyperlink ref="R25" r:id="rId27" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
+    <hyperlink ref="R26" r:id="rId28" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
+    <hyperlink ref="R27" r:id="rId29" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="R29" r:id="rId30" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
+    <hyperlink ref="S29" r:id="rId31" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
+    <hyperlink ref="T29" r:id="rId32" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
+    <hyperlink ref="R30" r:id="rId33" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="S30" r:id="rId34" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
+    <hyperlink ref="R31" r:id="rId35" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="R32" r:id="rId36" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="R33" r:id="rId37" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
+    <hyperlink ref="R34" r:id="rId38" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R36" r:id="rId39" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="R38" r:id="rId40" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
+    <hyperlink ref="S38" r:id="rId41" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R39" r:id="rId42" location="" tooltip="" display="https://www.diarioconstitucional.cl/2021/04/17/detalles-del-caso-corpesca-tercer-tribunal-de-juicio-oral-en-lo-penal-de-santiago-condeno-al-exsenador-jaime-orpis-a-la-pena-unica-de-5-anos-y-un-dia-de-presidio-efectivo-en-calidad-de-autor-de-seis/"/>
+    <hyperlink ref="S39" r:id="rId43" location="" tooltip="" display="https://contracarga.cl/reportajes/caso-corpesca-explicado/"/>
+    <hyperlink ref="R40" r:id="rId44" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
+    <hyperlink ref="R41" r:id="rId45" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R42" r:id="rId46" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
+    <hyperlink ref="S42" r:id="rId47" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
+    <hyperlink ref="R43" r:id="rId48" location="" tooltip="" display="https://www.biobiochile.cl/especial/bbcl-investiga/noticias/cronicas/2022/02/02/los-millonarios-finiquitos-de-la-era-reginato-los-detalles-de-la-nueva-denuncia-de-ripamonti.shtml"/>
+    <hyperlink ref="S43" r:id="rId49" location="" tooltip="" display="https://www.publimetro.cl/noticias/2022/09/23/100-mil-millones-las-perdidas-de-virginia-reginato-en-municipalidad-de-vina-del-mar/"/>
+    <hyperlink ref="R44" r:id="rId50" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="R45" r:id="rId51" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="S45" r:id="rId52" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
+    <hyperlink ref="R46" r:id="rId53" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R47" r:id="rId54" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
+    <hyperlink ref="R48" r:id="rId55" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="S48" r:id="rId56" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
+    <hyperlink ref="R50" r:id="rId57" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="S50" r:id="rId58" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
+    <hyperlink ref="R51" r:id="rId59" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R53" r:id="rId60" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="R54" r:id="rId61" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
+    <hyperlink ref="S54" r:id="rId62" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
+    <hyperlink ref="T54" r:id="rId63" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
+    <hyperlink ref="R55" r:id="rId64" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
+    <hyperlink ref="S55" r:id="rId65" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
+    <hyperlink ref="T55" r:id="rId66" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
nuevos casos, responsables, ubicaciones
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="276">
   <si>
     <t>Caso</t>
   </si>
@@ -749,6 +749,9 @@
     <t>Democracia Viva</t>
   </si>
   <si>
+    <t>Daniel Andrade, Carlos Contreras</t>
+  </si>
+  <si>
     <t>Antofagasta</t>
   </si>
   <si>
@@ -1204,6 +1207,60 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios, arista lencería (Camila Polizzi)</t>
+  </si>
+  <si>
+    <t>Camila Polizzi</t>
+  </si>
+  <si>
+    <t>estafa, falsificación de documento oficial, usurpación de identidad, lavado de activos</t>
+  </si>
+  <si>
+    <t>Fundación En tí</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://radio.uchile.cl/2023/11/28/755094/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Recoleta (Daniel Jadue)</t>
+  </si>
+  <si>
+    <t>Daniel Jadue</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html</t>
     </r>
   </si>
 </sst>
@@ -2536,7 +2593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V55"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -3949,7 +4006,7 @@
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
     </row>
-    <row r="32" ht="20.05" customHeight="1">
+    <row r="32" ht="32.05" customHeight="1">
       <c r="A32" t="s" s="14">
         <v>162</v>
       </c>
@@ -3959,7 +4016,9 @@
       <c r="C32" s="16">
         <v>2023</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" t="s" s="17">
+        <v>163</v>
+      </c>
       <c r="E32" t="s" s="17">
         <v>58</v>
       </c>
@@ -3969,7 +4028,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
       <c r="I32" t="s" s="17">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J32" t="s" s="17">
         <v>14</v>
@@ -3993,7 +4052,7 @@
     </row>
     <row r="33" ht="32.05" customHeight="1">
       <c r="A33" t="s" s="14">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B33" s="15">
         <v>293093681</v>
@@ -4002,13 +4061,13 @@
         <v>2023</v>
       </c>
       <c r="D33" t="s" s="17">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E33" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F33" t="s" s="17">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G33" s="18"/>
       <c r="H33" s="18"/>
@@ -4018,13 +4077,13 @@
       <c r="L33" s="18"/>
       <c r="M33" s="18"/>
       <c r="N33" t="s" s="19">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="21"/>
       <c r="Q33" s="21"/>
       <c r="R33" t="s" s="19">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
@@ -4033,7 +4092,7 @@
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="14">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B34" s="15">
         <v>289350646</v>
@@ -4042,7 +4101,7 @@
         <v>2018</v>
       </c>
       <c r="D34" t="s" s="17">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s" s="17">
         <v>29</v>
@@ -4053,7 +4112,7 @@
       <c r="G34" s="18"/>
       <c r="H34" s="18"/>
       <c r="I34" t="s" s="17">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="J34" t="s" s="17">
         <v>32</v>
@@ -4075,7 +4134,7 @@
     </row>
     <row r="35" ht="32.05" customHeight="1">
       <c r="A35" t="s" s="14">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B35" s="15">
         <v>283000000</v>
@@ -4084,7 +4143,7 @@
         <v>2017</v>
       </c>
       <c r="D35" t="s" s="17">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E35" t="s" s="17">
         <v>58</v>
@@ -4099,13 +4158,13 @@
         <v>2017</v>
       </c>
       <c r="I35" t="s" s="17">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J35" t="s" s="17">
         <v>32</v>
       </c>
       <c r="K35" t="s" s="17">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L35" t="s" s="17">
         <v>33</v>
@@ -4114,13 +4173,13 @@
         <v>114</v>
       </c>
       <c r="N35" t="s" s="19">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O35" s="20"/>
       <c r="P35" s="21"/>
       <c r="Q35" s="18"/>
       <c r="R35" t="s" s="19">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
@@ -4129,7 +4188,7 @@
     </row>
     <row r="36" ht="32.05" customHeight="1">
       <c r="A36" t="s" s="14">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B36" s="15">
         <v>274000000</v>
@@ -4145,7 +4204,7 @@
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" t="s" s="17">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J36" t="s" s="17">
         <v>14</v>
@@ -4155,7 +4214,7 @@
       <c r="M36" s="18"/>
       <c r="N36" s="21"/>
       <c r="O36" t="s" s="23">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="P36" s="21"/>
       <c r="Q36" s="18"/>
@@ -4169,7 +4228,7 @@
     </row>
     <row r="37" ht="32.05" customHeight="1">
       <c r="A37" t="s" s="14">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B37" s="15">
         <v>262000000</v>
@@ -4178,19 +4237,19 @@
         <v>2006</v>
       </c>
       <c r="D37" t="s" s="17">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E37" t="s" s="17">
         <v>23</v>
       </c>
       <c r="F37" t="s" s="17">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="18"/>
       <c r="J37" t="s" s="17">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="K37" s="18"/>
       <c r="L37" s="18"/>
@@ -4207,7 +4266,7 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="14">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B38" s="15">
         <v>203000000</v>
@@ -4216,7 +4275,7 @@
         <v>2018</v>
       </c>
       <c r="D38" t="s" s="17">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E38" t="s" s="17">
         <v>29</v>
@@ -4227,7 +4286,7 @@
       <c r="G38" s="18"/>
       <c r="H38" s="18"/>
       <c r="I38" t="s" s="17">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J38" t="s" s="17">
         <v>32</v>
@@ -4242,7 +4301,7 @@
       <c r="P38" s="21"/>
       <c r="Q38" s="18"/>
       <c r="R38" t="s" s="19">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="S38" t="s" s="19">
         <v>68</v>
@@ -4253,7 +4312,7 @@
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="14">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B39" s="15">
         <v>200000000</v>
@@ -4262,7 +4321,7 @@
         <v>2012</v>
       </c>
       <c r="D39" t="s" s="17">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E39" t="s" s="17">
         <v>29</v>
@@ -4278,24 +4337,24 @@
       </c>
       <c r="I39" s="18"/>
       <c r="J39" t="s" s="17">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="K39" s="18"/>
       <c r="L39" s="18"/>
       <c r="M39" s="18"/>
       <c r="N39" t="s" s="19">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="21"/>
       <c r="Q39" t="s" s="17">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="R39" t="s" s="19">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="S39" t="s" s="19">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="T39" s="21"/>
       <c r="U39" s="21"/>
@@ -4303,7 +4362,7 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="14">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" s="15">
         <v>190000000</v>
@@ -4312,7 +4371,7 @@
         <v>2024</v>
       </c>
       <c r="D40" t="s" s="17">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" t="s" s="17">
         <v>29</v>
@@ -4323,7 +4382,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" t="s" s="17">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="J40" t="s" s="17">
         <v>32</v>
@@ -4338,7 +4397,7 @@
       <c r="P40" s="21"/>
       <c r="Q40" s="21"/>
       <c r="R40" t="s" s="19">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="S40" s="21"/>
       <c r="T40" s="21"/>
@@ -4347,7 +4406,7 @@
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="14">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" s="15">
         <v>188000000</v>
@@ -4356,7 +4415,7 @@
         <v>2021</v>
       </c>
       <c r="D41" t="s" s="17">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E41" t="s" s="17">
         <v>29</v>
@@ -4367,7 +4426,7 @@
       <c r="G41" s="18"/>
       <c r="H41" s="18"/>
       <c r="I41" t="s" s="17">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="J41" t="s" s="17">
         <v>32</v>
@@ -4389,7 +4448,7 @@
     </row>
     <row r="42" ht="44.05" customHeight="1">
       <c r="A42" t="s" s="14">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B42" s="15">
         <v>176000000</v>
@@ -4398,7 +4457,7 @@
         <v>2024</v>
       </c>
       <c r="D42" t="s" s="17">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E42" t="s" s="17">
         <v>29</v>
@@ -4413,7 +4472,7 @@
         <v>2021</v>
       </c>
       <c r="I42" t="s" s="17">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J42" t="s" s="17">
         <v>32</v>
@@ -4428,16 +4487,16 @@
       </c>
       <c r="O42" s="20"/>
       <c r="P42" t="s" s="19">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q42" t="s" s="17">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="R42" t="s" s="19">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="S42" t="s" s="19">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="T42" s="21"/>
       <c r="U42" s="21"/>
@@ -4445,7 +4504,7 @@
     </row>
     <row r="43" ht="32.05" customHeight="1">
       <c r="A43" t="s" s="14">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B43" s="15">
         <v>150000000</v>
@@ -4454,7 +4513,7 @@
         <v>2021</v>
       </c>
       <c r="D43" t="s" s="17">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E43" t="s" s="17">
         <v>29</v>
@@ -4465,7 +4524,7 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" t="s" s="17">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J43" t="s" s="17">
         <v>32</v>
@@ -4480,10 +4539,10 @@
       <c r="P43" s="21"/>
       <c r="Q43" s="18"/>
       <c r="R43" t="s" s="19">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="S43" t="s" s="19">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="T43" s="21"/>
       <c r="U43" s="21"/>
@@ -4491,7 +4550,7 @@
     </row>
     <row r="44" ht="32.05" customHeight="1">
       <c r="A44" t="s" s="14">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B44" s="15">
         <v>148000000</v>
@@ -4507,7 +4566,7 @@
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
       <c r="I44" t="s" s="17">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J44" t="s" s="17">
         <v>14</v>
@@ -4517,7 +4576,7 @@
       <c r="M44" s="18"/>
       <c r="N44" s="21"/>
       <c r="O44" t="s" s="23">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="P44" s="21"/>
       <c r="Q44" s="18"/>
@@ -4531,7 +4590,7 @@
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="14">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B45" s="15">
         <v>128000000</v>
@@ -4544,12 +4603,12 @@
         <v>58</v>
       </c>
       <c r="F45" t="s" s="17">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
       <c r="I45" t="s" s="17">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="J45" t="s" s="17">
         <v>14</v>
@@ -4559,7 +4618,7 @@
       <c r="M45" s="18"/>
       <c r="N45" s="21"/>
       <c r="O45" t="s" s="23">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P45" s="21"/>
       <c r="Q45" s="18"/>
@@ -4567,7 +4626,7 @@
         <v>76</v>
       </c>
       <c r="S45" t="s" s="19">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T45" s="21"/>
       <c r="U45" s="21"/>
@@ -4575,7 +4634,7 @@
     </row>
     <row r="46" ht="32.05" customHeight="1">
       <c r="A46" t="s" s="14">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B46" s="15">
         <v>59595096</v>
@@ -4584,7 +4643,7 @@
         <v>2020</v>
       </c>
       <c r="D46" t="s" s="17">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E46" t="s" s="17">
         <v>29</v>
@@ -4617,7 +4676,7 @@
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="14">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B47" s="15">
         <v>40000000</v>
@@ -4637,7 +4696,7 @@
         <v>2013</v>
       </c>
       <c r="I47" t="s" s="17">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J47" t="s" s="17">
         <v>39</v>
@@ -4650,7 +4709,7 @@
       <c r="P47" s="21"/>
       <c r="Q47" s="18"/>
       <c r="R47" t="s" s="19">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="S47" s="21"/>
       <c r="T47" s="21"/>
@@ -4659,7 +4718,7 @@
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="14">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B48" s="15">
         <v>35000000</v>
@@ -4668,13 +4727,13 @@
         <v>2002</v>
       </c>
       <c r="D48" t="s" s="17">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E48" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F48" t="s" s="17">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
@@ -4684,18 +4743,18 @@
       <c r="L48" s="18"/>
       <c r="M48" s="18"/>
       <c r="N48" t="s" s="19">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="O48" s="21"/>
       <c r="P48" s="21"/>
       <c r="Q48" t="s" s="17">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="R48" t="s" s="19">
         <v>87</v>
       </c>
       <c r="S48" t="s" s="19">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="T48" s="21"/>
       <c r="U48" s="21"/>
@@ -4703,7 +4762,7 @@
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="14">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B49" s="15">
         <v>30000000</v>
@@ -4712,7 +4771,7 @@
         <v>2009</v>
       </c>
       <c r="D49" t="s" s="17">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E49" t="s" s="17">
         <v>29</v>
@@ -4726,7 +4785,7 @@
       <c r="H49" s="18"/>
       <c r="I49" s="18"/>
       <c r="J49" t="s" s="17">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="18"/>
@@ -4736,7 +4795,7 @@
       <c r="P49" s="21"/>
       <c r="Q49" s="18"/>
       <c r="R49" t="s" s="19">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="S49" s="21"/>
       <c r="T49" s="21"/>
@@ -4745,7 +4804,7 @@
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="14">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B50" s="15">
         <v>23671000</v>
@@ -4754,13 +4813,13 @@
         <v>2008</v>
       </c>
       <c r="D50" t="s" s="17">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E50" t="s" s="17">
         <v>58</v>
       </c>
       <c r="F50" t="s" s="17">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G50" s="16">
         <v>2004</v>
@@ -4783,7 +4842,7 @@
         <v>87</v>
       </c>
       <c r="S50" t="s" s="19">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="T50" s="21"/>
       <c r="U50" s="21"/>
@@ -4791,7 +4850,7 @@
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="14">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B51" s="15">
         <v>15700000</v>
@@ -4800,7 +4859,7 @@
         <v>2015</v>
       </c>
       <c r="D51" t="s" s="17">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E51" t="s" s="17">
         <v>29</v>
@@ -4811,7 +4870,7 @@
       <c r="G51" s="18"/>
       <c r="H51" s="18"/>
       <c r="I51" t="s" s="17">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J51" t="s" s="17">
         <v>32</v>
@@ -4825,7 +4884,7 @@
       <c r="O51" s="21"/>
       <c r="P51" s="21"/>
       <c r="Q51" t="s" s="17">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="R51" t="s" s="19">
         <v>68</v>
@@ -4837,7 +4896,7 @@
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="14">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B52" s="15">
         <v>10333332</v>
@@ -4846,7 +4905,7 @@
         <v>2024</v>
       </c>
       <c r="D52" t="s" s="17">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E52" t="s" s="17">
         <v>29</v>
@@ -4861,7 +4920,7 @@
         <v>2024</v>
       </c>
       <c r="I52" t="s" s="17">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J52" t="s" s="17">
         <v>32</v>
@@ -4872,7 +4931,7 @@
       </c>
       <c r="M52" s="18"/>
       <c r="N52" t="s" s="19">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O52" s="20"/>
       <c r="P52" t="s" s="19">
@@ -4880,10 +4939,10 @@
       </c>
       <c r="Q52" s="18"/>
       <c r="R52" t="s" s="19">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="S52" t="s" s="19">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="T52" s="21"/>
       <c r="U52" s="21"/>
@@ -4891,7 +4950,7 @@
     </row>
     <row r="53" ht="32.05" customHeight="1">
       <c r="A53" t="s" s="14">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B53" s="15">
         <v>10000000</v>
@@ -4900,7 +4959,7 @@
         <v>2015</v>
       </c>
       <c r="D53" t="s" s="17">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E53" t="s" s="17">
         <v>29</v>
@@ -4911,7 +4970,7 @@
       <c r="G53" s="18"/>
       <c r="H53" s="18"/>
       <c r="I53" t="s" s="17">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="J53" t="s" s="17">
         <v>32</v>
@@ -4933,7 +4992,7 @@
     </row>
     <row r="54" ht="56.05" customHeight="1">
       <c r="A54" t="s" s="14">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B54" s="15">
         <v>24000000</v>
@@ -4942,13 +5001,13 @@
         <v>2022</v>
       </c>
       <c r="D54" t="s" s="17">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E54" t="s" s="17">
         <v>29</v>
       </c>
       <c r="F54" t="s" s="17">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G54" s="16">
         <v>2015</v>
@@ -4957,7 +5016,7 @@
         <v>2016</v>
       </c>
       <c r="I54" t="s" s="17">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="J54" t="s" s="17">
         <v>32</v>
@@ -4970,26 +5029,26 @@
       </c>
       <c r="O54" s="21"/>
       <c r="P54" t="s" s="19">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Q54" t="s" s="17">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="R54" t="s" s="19">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="S54" t="s" s="19">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="T54" t="s" s="19">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="U54" s="21"/>
       <c r="V54" s="21"/>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="14">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B55" s="15">
         <v>200000000</v>
@@ -4998,7 +5057,7 @@
         <v>2022</v>
       </c>
       <c r="D55" t="s" s="17">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E55" t="s" s="17">
         <v>29</v>
@@ -5013,7 +5072,7 @@
         <v>2021</v>
       </c>
       <c r="I55" t="s" s="17">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J55" t="s" s="17">
         <v>32</v>
@@ -5028,19 +5087,119 @@
       <c r="P55" s="21"/>
       <c r="Q55" s="18"/>
       <c r="R55" t="s" s="19">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="S55" t="s" s="19">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="T55" t="s" s="19">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
     </row>
+    <row r="56" ht="32.05" customHeight="1">
+      <c r="A56" t="s" s="14">
+        <v>266</v>
+      </c>
+      <c r="B56" s="15">
+        <v>93500000</v>
+      </c>
+      <c r="C56" s="16">
+        <v>2023</v>
+      </c>
+      <c r="D56" t="s" s="17">
+        <v>267</v>
+      </c>
+      <c r="E56" t="s" s="17">
+        <v>58</v>
+      </c>
+      <c r="F56" t="s" s="17">
+        <v>254</v>
+      </c>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" t="s" s="17">
+        <v>180</v>
+      </c>
+      <c r="J56" t="s" s="17">
+        <v>14</v>
+      </c>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" t="s" s="19">
+        <v>268</v>
+      </c>
+      <c r="O56" t="s" s="19">
+        <v>269</v>
+      </c>
+      <c r="P56" s="21"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" t="s" s="19">
+        <v>270</v>
+      </c>
+      <c r="S56" t="s" s="19">
+        <v>271</v>
+      </c>
+      <c r="T56" s="21"/>
+      <c r="U56" s="21"/>
+      <c r="V56" s="21"/>
+    </row>
+    <row r="57" ht="20.05" customHeight="1">
+      <c r="A57" t="s" s="14">
+        <v>272</v>
+      </c>
+      <c r="B57" s="15">
+        <v>20000000</v>
+      </c>
+      <c r="C57" s="16">
+        <v>2023</v>
+      </c>
+      <c r="D57" t="s" s="17">
+        <v>273</v>
+      </c>
+      <c r="E57" t="s" s="17">
+        <v>58</v>
+      </c>
+      <c r="F57" t="s" s="17">
+        <v>274</v>
+      </c>
+      <c r="G57" s="16">
+        <v>2023</v>
+      </c>
+      <c r="H57" s="16">
+        <v>2024</v>
+      </c>
+      <c r="I57" t="s" s="17">
+        <v>226</v>
+      </c>
+      <c r="J57" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K57" t="s" s="17">
+        <v>5</v>
+      </c>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" t="s" s="19">
+        <v>231</v>
+      </c>
+      <c r="O57" s="21"/>
+      <c r="P57" t="s" s="19">
+        <v>62</v>
+      </c>
+      <c r="Q57" s="18"/>
+      <c r="R57" t="s" s="19">
+        <v>275</v>
+      </c>
+      <c r="S57" s="21"/>
+      <c r="T57" s="21"/>
+      <c r="U57" s="21"/>
+      <c r="V57" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53:C55 E53:E55 G53:H55">
+  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53:C57 E53:E57 G53:H57">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -5115,6 +5274,9 @@
     <hyperlink ref="R55" r:id="rId64" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
     <hyperlink ref="S55" r:id="rId65" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
     <hyperlink ref="T55" r:id="rId66" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
+    <hyperlink ref="R56" r:id="rId67" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
+    <hyperlink ref="S56" r:id="rId68" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
+    <hyperlink ref="R57" r:id="rId69" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
prueba de carga condicionada a scrolling
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="301">
   <si>
     <t>Caso</t>
   </si>
@@ -1261,6 +1261,145 @@
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de San Fernando (Luis Berwart)</t>
+  </si>
+  <si>
+    <t>Luis Berwart</t>
+  </si>
+  <si>
+    <t>San Fernando</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fraude al Fisco, uso malicioso de instrumento mercantil, soborno</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.elrancaguino.cl/2024/01/18/hasta-35-anos-de-carcel-y-el-pago-de-2-mil-millones-de-pesos-en-multas-arriesga-el-ex-alcalde-san-fernando-luis-berwart/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de San Fernando (Juan Paulo Molina)</t>
+  </si>
+  <si>
+    <t>Juan Paulo Molina</t>
+  </si>
+  <si>
+    <t>fraude al fisco reiterado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado</t>
+    </r>
+  </si>
+  <si>
+    <t>Municipalidad de Linares</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Guaitecas (Cristian Alvarado Oyarzo)</t>
+  </si>
+  <si>
+    <t>Cristian Alvarado Oyarzo</t>
+  </si>
+  <si>
+    <t>Guaitecas</t>
+  </si>
+  <si>
+    <t>malversación de fondos públicos</t>
+  </si>
+  <si>
+    <t>Sentencia</t>
+  </si>
+  <si>
+    <t>10 años de presidio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739#:~:text=Tras</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> un largo proceso, la,mes de diciembre del 2021.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Rancagua (Juan Ramón Godoy)</t>
+  </si>
+  <si>
+    <t>Juan Ramón Godoy</t>
+  </si>
+  <si>
+    <t>Rancagua</t>
+  </si>
+  <si>
+    <t>fraude al Fisco, negociación incompatible</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.latercera.com/earlyaccess/noticia/las-millonarias-transacciones-que-complican-al-alcalde-de-rancagua/GY4SPWLFPJDODKTTXDN7FR74B4/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://radio.uchile.cl/2023/03/04/tras-allanamiento-a-alcalde-de-rancagua-expertos-en-transparencia-llaman-a-fortalecer-los-mecanismos-para-perseguir-la-corrupcion/</t>
     </r>
   </si>
 </sst>
@@ -2593,7 +2732,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -5198,8 +5337,240 @@
       <c r="U57" s="21"/>
       <c r="V57" s="21"/>
     </row>
+    <row r="58" ht="32.05" customHeight="1">
+      <c r="A58" t="s" s="14">
+        <v>276</v>
+      </c>
+      <c r="B58" s="15">
+        <v>4000000000</v>
+      </c>
+      <c r="C58" s="16">
+        <v>2024</v>
+      </c>
+      <c r="D58" t="s" s="17">
+        <v>277</v>
+      </c>
+      <c r="E58" t="s" s="17">
+        <v>23</v>
+      </c>
+      <c r="F58" t="s" s="17">
+        <v>254</v>
+      </c>
+      <c r="G58" s="16">
+        <v>2012</v>
+      </c>
+      <c r="H58" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I58" t="s" s="17">
+        <v>278</v>
+      </c>
+      <c r="J58" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" t="s" s="19">
+        <v>279</v>
+      </c>
+      <c r="O58" s="21"/>
+      <c r="P58" s="21"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" t="s" s="19">
+        <v>280</v>
+      </c>
+      <c r="S58" s="21"/>
+      <c r="T58" s="21"/>
+      <c r="U58" s="21"/>
+      <c r="V58" s="21"/>
+    </row>
+    <row r="59" ht="32.05" customHeight="1">
+      <c r="A59" t="s" s="14">
+        <v>281</v>
+      </c>
+      <c r="B59" s="15">
+        <v>37550000</v>
+      </c>
+      <c r="C59" s="16">
+        <v>2023</v>
+      </c>
+      <c r="D59" t="s" s="17">
+        <v>282</v>
+      </c>
+      <c r="E59" t="s" s="17">
+        <v>23</v>
+      </c>
+      <c r="F59" t="s" s="17">
+        <v>184</v>
+      </c>
+      <c r="G59" s="16">
+        <v>2018</v>
+      </c>
+      <c r="H59" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I59" t="s" s="17">
+        <v>278</v>
+      </c>
+      <c r="J59" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" t="s" s="19">
+        <v>283</v>
+      </c>
+      <c r="O59" s="21"/>
+      <c r="P59" s="21"/>
+      <c r="Q59" s="18"/>
+      <c r="R59" t="s" s="19">
+        <v>284</v>
+      </c>
+      <c r="S59" s="21"/>
+      <c r="T59" s="21"/>
+      <c r="U59" s="21"/>
+      <c r="V59" s="21"/>
+    </row>
+    <row r="60" ht="20.05" customHeight="1">
+      <c r="A60" t="s" s="14">
+        <v>285</v>
+      </c>
+      <c r="B60" s="15">
+        <v>139739316</v>
+      </c>
+      <c r="C60" s="16">
+        <v>2020</v>
+      </c>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="21"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
+      <c r="Q60" s="18"/>
+      <c r="R60" t="s" s="19">
+        <v>286</v>
+      </c>
+      <c r="S60" s="21"/>
+      <c r="T60" s="21"/>
+      <c r="U60" s="21"/>
+      <c r="V60" s="21"/>
+    </row>
+    <row r="61" ht="32.05" customHeight="1">
+      <c r="A61" t="s" s="14">
+        <v>287</v>
+      </c>
+      <c r="B61" s="15">
+        <v>351000000</v>
+      </c>
+      <c r="C61" s="16">
+        <v>2021</v>
+      </c>
+      <c r="D61" t="s" s="17">
+        <v>288</v>
+      </c>
+      <c r="E61" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s" s="17">
+        <v>254</v>
+      </c>
+      <c r="G61" s="16">
+        <v>2013</v>
+      </c>
+      <c r="H61" s="16">
+        <v>2016</v>
+      </c>
+      <c r="I61" t="s" s="17">
+        <v>289</v>
+      </c>
+      <c r="J61" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" t="s" s="19">
+        <v>290</v>
+      </c>
+      <c r="O61" s="21"/>
+      <c r="P61" t="s" s="19">
+        <v>291</v>
+      </c>
+      <c r="Q61" t="s" s="17">
+        <v>292</v>
+      </c>
+      <c r="R61" t="s" s="19">
+        <v>293</v>
+      </c>
+      <c r="S61" t="s" s="19">
+        <v>294</v>
+      </c>
+      <c r="T61" s="21"/>
+      <c r="U61" s="21"/>
+      <c r="V61" s="21"/>
+    </row>
+    <row r="62" ht="32.05" customHeight="1">
+      <c r="A62" t="s" s="14">
+        <v>295</v>
+      </c>
+      <c r="B62" s="15">
+        <v>2492000000</v>
+      </c>
+      <c r="C62" s="16">
+        <v>2022</v>
+      </c>
+      <c r="D62" t="s" s="17">
+        <v>296</v>
+      </c>
+      <c r="E62" t="s" s="17">
+        <v>58</v>
+      </c>
+      <c r="F62" t="s" s="17">
+        <v>59</v>
+      </c>
+      <c r="G62" s="16">
+        <v>2020</v>
+      </c>
+      <c r="H62" s="16">
+        <v>2021</v>
+      </c>
+      <c r="I62" t="s" s="17">
+        <v>297</v>
+      </c>
+      <c r="J62" t="s" s="17">
+        <v>32</v>
+      </c>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" t="s" s="19">
+        <v>298</v>
+      </c>
+      <c r="O62" s="21"/>
+      <c r="P62" s="21"/>
+      <c r="Q62" s="18"/>
+      <c r="R62" t="s" s="19">
+        <v>299</v>
+      </c>
+      <c r="S62" t="s" s="19">
+        <v>300</v>
+      </c>
+      <c r="T62" s="21"/>
+      <c r="U62" s="21"/>
+      <c r="V62" s="21"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53:C57 E53:E57 G53:H57">
+  <conditionalFormatting sqref="C1:C9 E1:E9 G1:H8 H9 C10:C13 E10:E13 G10:H12 H13 C14:C28 E14:E28 G14:H27 H28 C29:C33 E29:E33 G29:H32 H33 C34:C35 E34:E35 G34:H34 H35 C36:C40 E36:E40 G36:H39 H40 C41:C42 E41:E42 G41:H41 H42 C43:C47 E43:E47 G43:H46 H47 C48:C49 E48:E49 G48:H48 H49 C50:C52 E50:E52 G50:H51 H52 C53:C62 E53:E62 G53:H62">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -5277,6 +5648,13 @@
     <hyperlink ref="R56" r:id="rId67" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
     <hyperlink ref="S56" r:id="rId68" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
     <hyperlink ref="R57" r:id="rId69" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
+    <hyperlink ref="R58" r:id="rId70" location="" tooltip="" display="https://www.elrancaguino.cl/2024/01/18/hasta-35-anos-de-carcel-y-el-pago-de-2-mil-millones-de-pesos-en-multas-arriesga-el-ex-alcalde-san-fernando-luis-berwart/"/>
+    <hyperlink ref="R59" r:id="rId71" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
+    <hyperlink ref="R60" r:id="rId72" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html"/>
+    <hyperlink ref="R61" r:id="rId73" location="" tooltip="" display="http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739#:~:text=Tras"/>
+    <hyperlink ref="S61" r:id="rId74" location="" tooltip="" display="https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica"/>
+    <hyperlink ref="R62" r:id="rId75" location="" tooltip="" display="https://www.latercera.com/earlyaccess/noticia/las-millonarias-transacciones-que-complican-al-alcalde-de-rancagua/GY4SPWLFPJDODKTTXDN7FR74B4/"/>
+    <hyperlink ref="S62" r:id="rId76" location="" tooltip="" display="https://radio.uchile.cl/2023/03/04/tras-allanamiento-a-alcalde-de-rancagua-expertos-en-transparencia-llaman-a-fortalecer-los-mecanismos-para-perseguir-la-corrupcion/"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
correcion en datos, graficos nuevos
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="386">
   <si>
     <t>Caso</t>
   </si>
@@ -1717,6 +1717,106 @@
   </si>
   <si>
     <t>https://estapasando.cl/reformalizan-por-nuevos-delitos-a-alcalde-de-buin-udi/</t>
+  </si>
+  <si>
+    <t>Corporación de Desarrollo Social de Providencia</t>
+  </si>
+  <si>
+    <t>Mariano Rosenzvaig</t>
+  </si>
+  <si>
+    <t>Funcionario municipal</t>
+  </si>
+  <si>
+    <t>malversación de caudales públicos, aplicación pública diferente</t>
+  </si>
+  <si>
+    <t>Suspensión condicional de la causa</t>
+  </si>
+  <si>
+    <t>firma mensual, fijación de domicilio y deberá ofrecer una charla</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde suplente de Tierra Amarilla (Mario Morales)</t>
+  </si>
+  <si>
+    <t>Mario Morales</t>
+  </si>
+  <si>
+    <t>Tierra Amarilla</t>
+  </si>
+  <si>
+    <t>fraude al fisco, cohecho, soborno</t>
+  </si>
+  <si>
+    <t>Prisión preventiva</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml</t>
+    </r>
+  </si>
+  <si>
+    <t>Ex administrador municipal de Tierra Amarilla</t>
+  </si>
+  <si>
+    <t>Jaime Bahamondes Cabrera</t>
+  </si>
+  <si>
+    <t>fraude al fisco</t>
+  </si>
+  <si>
+    <t>Condenado</t>
+  </si>
+  <si>
+    <t>presidio, prohibición de cargo público, multa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> El Tribunal,el marco del caso denominado</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3038,7 +3138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X71"/>
+  <dimension ref="A1:X74"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -3049,14 +3149,14 @@
     <col min="1" max="1" width="33.7266" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.22656" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.2266" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.4922" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.5469" style="1" customWidth="1"/>
     <col min="7" max="8" width="5.22656" style="1" customWidth="1"/>
     <col min="9" max="16" width="16.3516" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.4922" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.6875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="16.3516" style="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7344" style="1" customWidth="1"/>
     <col min="20" max="20" width="40.2734" style="1" customWidth="1"/>
     <col min="21" max="21" width="38.2188" style="1" customWidth="1"/>
     <col min="22" max="24" width="16.3516" style="1" customWidth="1"/>
@@ -3287,7 +3387,7 @@
       <c r="W4" s="20"/>
       <c r="X4" s="20"/>
     </row>
-    <row r="5" ht="44.05" customHeight="1">
+    <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="14">
         <v>46</v>
       </c>
@@ -3991,7 +4091,7 @@
         <v>4500000000</v>
       </c>
       <c r="C20" s="16">
-        <v>2003</v>
+        <v>2023</v>
       </c>
       <c r="D20" t="s" s="17">
         <v>122</v>
@@ -4465,7 +4565,7 @@
       <c r="W29" s="20"/>
       <c r="X29" s="20"/>
     </row>
-    <row r="30" ht="32.05" customHeight="1">
+    <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="14">
         <v>177</v>
       </c>
@@ -5267,7 +5367,7 @@
       <c r="W46" s="20"/>
       <c r="X46" s="20"/>
     </row>
-    <row r="47" ht="32.05" customHeight="1">
+    <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="14">
         <v>252</v>
       </c>
@@ -5603,7 +5703,7 @@
       <c r="W53" s="20"/>
       <c r="X53" s="20"/>
     </row>
-    <row r="54" ht="44.05" customHeight="1">
+    <row r="54" ht="32.05" customHeight="1">
       <c r="A54" t="s" s="14">
         <v>283</v>
       </c>
@@ -5703,7 +5803,7 @@
       <c r="W55" s="20"/>
       <c r="X55" s="20"/>
     </row>
-    <row r="56" ht="32.05" customHeight="1">
+    <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="14">
         <v>291</v>
       </c>
@@ -5891,7 +5991,7 @@
       <c r="W59" s="20"/>
       <c r="X59" s="20"/>
     </row>
-    <row r="60" ht="32.05" customHeight="1">
+    <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="14">
         <v>310</v>
       </c>
@@ -6089,7 +6189,7 @@
         <v>327</v>
       </c>
       <c r="E64" t="s" s="17">
-        <v>73</v>
+        <v>150</v>
       </c>
       <c r="F64" t="s" s="17">
         <v>74</v>
@@ -6179,7 +6279,7 @@
       <c r="W65" s="20"/>
       <c r="X65" s="20"/>
     </row>
-    <row r="66" ht="56.05" customHeight="1">
+    <row r="66" ht="44.05" customHeight="1">
       <c r="A66" t="s" s="14">
         <v>338</v>
       </c>
@@ -6319,7 +6419,9 @@
       <c r="K68" t="s" s="17">
         <v>350</v>
       </c>
-      <c r="L68" s="18"/>
+      <c r="L68" t="s" s="17">
+        <v>29</v>
+      </c>
       <c r="M68" t="s" s="17">
         <v>350</v>
       </c>
@@ -6373,7 +6475,9 @@
       <c r="K69" t="s" s="17">
         <v>5</v>
       </c>
-      <c r="L69" s="18"/>
+      <c r="L69" t="s" s="17">
+        <v>29</v>
+      </c>
       <c r="M69" s="18"/>
       <c r="N69" s="20"/>
       <c r="O69" t="s" s="21">
@@ -6497,8 +6601,182 @@
       <c r="W71" s="20"/>
       <c r="X71" s="20"/>
     </row>
+    <row r="72" ht="44.05" customHeight="1">
+      <c r="A72" t="s" s="14">
+        <v>366</v>
+      </c>
+      <c r="B72" s="15">
+        <v>1600000000</v>
+      </c>
+      <c r="C72" s="16">
+        <v>2020</v>
+      </c>
+      <c r="D72" t="s" s="17">
+        <v>367</v>
+      </c>
+      <c r="E72" t="s" s="17">
+        <v>150</v>
+      </c>
+      <c r="F72" t="s" s="17">
+        <v>212</v>
+      </c>
+      <c r="G72" s="16">
+        <v>2020</v>
+      </c>
+      <c r="H72" s="16">
+        <v>2022</v>
+      </c>
+      <c r="I72" t="s" s="17">
+        <v>328</v>
+      </c>
+      <c r="J72" t="s" s="17">
+        <v>368</v>
+      </c>
+      <c r="K72" s="18"/>
+      <c r="L72" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="M72" s="18"/>
+      <c r="N72" s="20"/>
+      <c r="O72" t="s" s="21">
+        <v>369</v>
+      </c>
+      <c r="P72" t="s" s="21">
+        <v>370</v>
+      </c>
+      <c r="Q72" s="18"/>
+      <c r="R72" s="18"/>
+      <c r="S72" t="s" s="17">
+        <v>371</v>
+      </c>
+      <c r="T72" t="s" s="21">
+        <v>372</v>
+      </c>
+      <c r="U72" s="20"/>
+      <c r="V72" s="20"/>
+      <c r="W72" s="20"/>
+      <c r="X72" s="20"/>
+    </row>
+    <row r="73" ht="32.05" customHeight="1">
+      <c r="A73" t="s" s="14">
+        <v>373</v>
+      </c>
+      <c r="B73" s="15">
+        <v>102000000</v>
+      </c>
+      <c r="C73" s="16">
+        <v>2020</v>
+      </c>
+      <c r="D73" t="s" s="17">
+        <v>374</v>
+      </c>
+      <c r="E73" t="s" s="17">
+        <v>150</v>
+      </c>
+      <c r="F73" t="s" s="17">
+        <v>151</v>
+      </c>
+      <c r="G73" s="16">
+        <v>2016</v>
+      </c>
+      <c r="H73" s="16">
+        <v>2020</v>
+      </c>
+      <c r="I73" t="s" s="17">
+        <v>375</v>
+      </c>
+      <c r="J73" t="s" s="17">
+        <v>28</v>
+      </c>
+      <c r="K73" s="18"/>
+      <c r="L73" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="M73" s="18"/>
+      <c r="N73" s="20"/>
+      <c r="O73" t="s" s="21">
+        <v>376</v>
+      </c>
+      <c r="P73" t="s" s="21">
+        <v>377</v>
+      </c>
+      <c r="Q73" s="18"/>
+      <c r="R73" s="18"/>
+      <c r="S73" s="18"/>
+      <c r="T73" t="s" s="21">
+        <v>378</v>
+      </c>
+      <c r="U73" s="20"/>
+      <c r="V73" s="20"/>
+      <c r="W73" s="20"/>
+      <c r="X73" s="20"/>
+    </row>
+    <row r="74" ht="32.05" customHeight="1">
+      <c r="A74" t="s" s="14">
+        <v>379</v>
+      </c>
+      <c r="B74" s="15">
+        <v>80069002</v>
+      </c>
+      <c r="C74" s="16">
+        <v>2023</v>
+      </c>
+      <c r="D74" t="s" s="17">
+        <v>380</v>
+      </c>
+      <c r="E74" t="s" s="17">
+        <v>73</v>
+      </c>
+      <c r="F74" t="s" s="17">
+        <v>317</v>
+      </c>
+      <c r="G74" s="16">
+        <v>2022</v>
+      </c>
+      <c r="H74" s="16">
+        <v>2023</v>
+      </c>
+      <c r="I74" t="s" s="17">
+        <v>375</v>
+      </c>
+      <c r="J74" t="s" s="17">
+        <v>368</v>
+      </c>
+      <c r="K74" t="s" s="17">
+        <v>28</v>
+      </c>
+      <c r="L74" t="s" s="17">
+        <v>29</v>
+      </c>
+      <c r="M74" s="18"/>
+      <c r="N74" s="20"/>
+      <c r="O74" t="s" s="21">
+        <v>381</v>
+      </c>
+      <c r="P74" t="s" s="21">
+        <v>382</v>
+      </c>
+      <c r="Q74" t="s" s="17">
+        <v>331</v>
+      </c>
+      <c r="R74" t="s" s="17">
+        <v>331</v>
+      </c>
+      <c r="S74" t="s" s="17">
+        <v>383</v>
+      </c>
+      <c r="T74" t="s" s="21">
+        <v>384</v>
+      </c>
+      <c r="U74" t="s" s="21">
+        <v>385</v>
+      </c>
+      <c r="V74" s="20"/>
+      <c r="W74" s="20"/>
+      <c r="X74" s="20"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C11 E1:E11 G1:H10 H11 C12:C15 E12:E15 G12:H14 H15 C16:C35 E16:E35 G16:H34 H35 C36:C44 E36:E44 G36:H43 H44 C45:C47 E45:E47 G45:H46 H47 C48:C52 E48:E52 G48:H51 H52 C53:C54 E53:E54 G53:H53 H54 C55:C61 E55:E61 G55:H60 H61 C62:C64 E62:E64 G62:H63 H64:H65 C65:C71 E65:E71 G66:H70 H71">
+  <conditionalFormatting sqref="C1:C11 E1:E11 G1:H10 H11 C12:C15 E12:E15 G12:H14 H15 C16:C35 E16:E35 G16:H34 H35 C36:C44 E36:E44 G36:H43 H44 C45:C47 E45:E47 G45:H46 H47 C48:C52 E48:E52 G48:H51 H52 C53:C54 E53:E54 G53:H53 H54 C55:C61 E55:E61 G55:H60 H61 C62:C64 E62:E64 G62:H63 H64:H65 C65:C71 E65:E71 G66:H70 H71:H74 C72:C74 E72:E74">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -6600,6 +6878,10 @@
     <hyperlink ref="T68" r:id="rId91" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
     <hyperlink ref="T69" r:id="rId92" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
     <hyperlink ref="T70" r:id="rId93" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T72" r:id="rId94" location="" tooltip="" display="https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022"/>
+    <hyperlink ref="T73" r:id="rId95" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
+    <hyperlink ref="T74" r:id="rId96" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
+    <hyperlink ref="U74" r:id="rId97" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
nuevos graficos, torta, datos
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="428">
   <si>
     <t>Caso</t>
   </si>
@@ -732,6 +732,9 @@
     <t>Fundación Local</t>
   </si>
   <si>
+    <t>negociaciones incompatibles, tráfico de influencia, fraude al fisco</t>
+  </si>
+  <si>
     <t>https://www.eldesconcierto.cl/opinion/2023/10/27/caso-convenios-corrupcion-en-la-derecha-supera-a-democracia-viva.html</t>
   </si>
   <si>
@@ -755,6 +758,9 @@
     <t>Rinconada</t>
   </si>
   <si>
+    <t>Malversación de Fondos Públicos</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -766,6 +772,25 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://munirinconada.cl/alcalde-juan-galdames-se-refiere-a-juicio-de-cuentas-que-ordena-la-restitucion-de-300-millones/#:~:text=Municipal-,Alcalde</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> Juan Galdames, se refiere a juicio de cuentas que,la restitución de 300 millones.&amp;text=Contraloría ordena la restitución de,por Malversación de Fondos Públicos.</t>
+    </r>
+  </si>
+  <si>
     <t>Caso LarrainVial</t>
   </si>
   <si>
@@ -936,6 +961,9 @@
     <t>Río Bueno</t>
   </si>
   <si>
+    <t>fraude de subvenciones estatales</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -1181,12 +1209,23 @@
     <t>Democracia Viva</t>
   </si>
   <si>
-    <t>Gobernador regional Araucanía, fundación Coigue</t>
+    <t>Caso Convenios (Fundación Coigue)</t>
+  </si>
+  <si>
+    <t>Luciano Rivas, Claudia
+Lillo, Sebastián
+Naveillán</t>
+  </si>
+  <si>
+    <t>Evópoli, UDI</t>
   </si>
   <si>
     <t>Fundación Coigue</t>
   </si>
   <si>
+    <t>Adjudicación de fondos a fundación sin experiencia ni giro adecuado</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <u val="single"/>
@@ -1194,819 +1233,861 @@
         <color indexed="8"/>
         <rFont val="Helvetica"/>
       </rPr>
+      <t>https://radionuevomundo.cl/2023/07/18/gobernador-rivas-suma-al-caso-fundacion-local-traspasos-arbitrarios-a-coihue-y-a-universidades-de-la-araucania/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://resumen.cl/articulos/la-derecha-de-la-araucania-en-el-caso-fundaciones-las-irregularidades-de-espacio-coigue-que-llevaron-al-ministerio-de-justicia-a-solicitar-su-cierre</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Motorola (Katherine Martorell)</t>
+  </si>
+  <si>
+    <t>Katherine Martorell</t>
+  </si>
+  <si>
+    <t>Subsecretario</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios (Bonhomía)</t>
+  </si>
+  <si>
+    <t>Republicanos</t>
+  </si>
+  <si>
+    <t>Biobío</t>
+  </si>
+  <si>
+    <t>Fundación Bonhomía</t>
+  </si>
+  <si>
+    <t>Ejecución incompleta de programa, facturas y boletas sin respaldo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-del-biobio/detienen-a-lider-de-empresa-en-allanamiento-por-caso-convenios-pdi/2024-03-13/123002.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Guaitecas (Cristian Alvarado Oyarzo)</t>
+  </si>
+  <si>
+    <t>Cristian Alvarado Oyarzo</t>
+  </si>
+  <si>
+    <t>Guaitecas</t>
+  </si>
+  <si>
+    <t>malversación de fondos públicos</t>
+  </si>
+  <si>
+    <t>10 años de presidio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica</t>
+    </r>
+  </si>
+  <si>
+    <t>Gastos electorales Comunes (Karina Oliva)</t>
+  </si>
+  <si>
+    <t>Karina Oliva</t>
+  </si>
+  <si>
+    <t>Comunes</t>
+  </si>
+  <si>
+    <t>fraude de subvenciones</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Subvenciones</t>
+  </si>
+  <si>
+    <t>Franka Grez</t>
+  </si>
+  <si>
+    <t>Ministro</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Valparaíso (Jorge Castro)</t>
+  </si>
+  <si>
+    <t>Jorge Castro</t>
+  </si>
+  <si>
+    <t>Valparaíso</t>
+  </si>
+  <si>
+    <t>Fraude al fisco, malversación de fondos</t>
+  </si>
+  <si>
+    <t>Caso San Ramón</t>
+  </si>
+  <si>
+    <t>Miguel Ángel Aguilera</t>
+  </si>
+  <si>
+    <t>San Ramón</t>
+  </si>
+  <si>
+    <t>Político</t>
+  </si>
+  <si>
+    <t>enriquecimiento ilícito, lavado de activos, cohecho, soborno</t>
+  </si>
+  <si>
+    <t>https://www.ciperchile.cl/2021/06/04/los-millonarios-pagos-al-alcalde-aguilera-y-los-testimonios-de-sus-subordinados-que-lo-tienen-al-borde-del-precipicio/</t>
+  </si>
+  <si>
+    <t>Caso Convenios (RedCultivarte)</t>
+  </si>
+  <si>
+    <t>ONG RedCultivarte</t>
+  </si>
+  <si>
+    <t>Caso Corpesca (Jaime Orpis)</t>
+  </si>
+  <si>
+    <t>Jaime Orpis</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios, arista lencería (Camila Polizzi)</t>
+  </si>
+  <si>
+    <t>Camila Polizzi, Diego Polanco</t>
+  </si>
+  <si>
+    <t>Fundación En tí</t>
+  </si>
+  <si>
+    <t>estafa, falsificación de documento oficial, usurpación de identidad, lavado de activos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://radio.uchile.cl/2023/11/28/755094/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Puente Alto (Germán Codina)</t>
+  </si>
+  <si>
+    <t>Germán Codina</t>
+  </si>
+  <si>
+    <t>Puente Alto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Mostazal (Sergio Medel)</t>
+  </si>
+  <si>
+    <t>Sergio Medel</t>
+  </si>
+  <si>
+    <t>Mostazal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Calama (Daniel Agusto Pérez)</t>
+  </si>
+  <si>
+    <t>Daniel Agusto Pérez</t>
+  </si>
+  <si>
+    <t>Calama</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Santiago (Felipe Alessandri)</t>
+  </si>
+  <si>
+    <t>Felipe Alessandri</t>
+  </si>
+  <si>
+    <t>Santiago</t>
+  </si>
+  <si>
+    <t>Pagos de horas extra, pagos de honorarios</t>
+  </si>
+  <si>
+    <t>Alcalde de Ñuñoa (Andrés Zarhi)</t>
+  </si>
+  <si>
+    <t>Andrés Zarhi</t>
+  </si>
+  <si>
+    <t>Ñuñoa</t>
+  </si>
+  <si>
+    <t>Formalizado</t>
+  </si>
+  <si>
+    <t>arresto domiciliario nocturno, arraigo nacional</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Municipalidad de Linares</t>
+  </si>
+  <si>
+    <t>Mario Meza Vásquez</t>
+  </si>
+  <si>
+    <t>Linares</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios (Atacama)</t>
+  </si>
+  <si>
+    <t>DC, PRO</t>
+  </si>
+  <si>
+    <t>Atacama</t>
+  </si>
+  <si>
+    <t>Fundación Comprometidos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Administrador municipal de Viña del Mar</t>
+  </si>
+  <si>
+    <t>Claudio Boisier</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde suplente de Tierra Amarilla (Mario Morales)</t>
+  </si>
+  <si>
+    <t>Mario Morales</t>
+  </si>
+  <si>
+    <t>Tierra Amarilla</t>
+  </si>
+  <si>
+    <t>fraude al fisco, cohecho, soborno</t>
+  </si>
+  <si>
+    <t>Prisión preventiva</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml</t>
+    </r>
+  </si>
+  <si>
+    <t>Ex administrador municipal de Tierra Amarilla</t>
+  </si>
+  <si>
+    <t>Jaime Bahamondes Cabrera</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>fraude al fisco</t>
+  </si>
+  <si>
+    <t>Condenado</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>presidio, prohibición de cargo público, multa</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> El Tribunal,el marco del caso denominado</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Penta (Pablo Wagner)</t>
+  </si>
+  <si>
+    <t>Pablo Wagner</t>
+  </si>
+  <si>
+    <t>Delitos tributarios, enriquecimiento ilícito</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Las Condes (Joaquín Lavín)</t>
+  </si>
+  <si>
+    <t>Joaquín Lavín Infante</t>
+  </si>
+  <si>
+    <t>Caso Ceresita</t>
+  </si>
+  <si>
+    <t>Recoleta</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.chiletransparente.cl/caso-ceresita/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de San Fernando (Juan Paulo Molina)</t>
+  </si>
+  <si>
+    <t>Juan Paulo Molina</t>
+  </si>
+  <si>
+    <t>fraude al fisco reiterado</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Coimas</t>
+  </si>
+  <si>
+    <t>Patricio Tombolini</t>
+  </si>
+  <si>
+    <t>PR, DC</t>
+  </si>
+  <si>
+    <t>cohecho</t>
+  </si>
+  <si>
+    <t>presidio</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://es.wikipedia.org/wiki/Caso_Coimas</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcaldesa de Providencia (Josefa Errázuriz)</t>
+  </si>
+  <si>
+    <t>Josefa Errázuriz</t>
+  </si>
+  <si>
+    <t>Pago de horas extra</t>
+  </si>
+  <si>
+    <t>Responsable pero sin condena</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sin condena por prescripción</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Claudia Nogueira </t>
+  </si>
+  <si>
+    <t>Diputado</t>
+  </si>
+  <si>
+    <t>https://www.ciperchile.cl/2009/06/12/fiscalia-decide-formalizar-a-diputada-nogueira-e-investiga-pagos-de-la-camara-a-asesores/</t>
+  </si>
+  <si>
+    <t>Caso Main, alcaldesa de Antofagasta (Karen Rojo)</t>
+  </si>
+  <si>
+    <t>Karen Rojo</t>
+  </si>
+  <si>
+    <t>Condenada</t>
+  </si>
+  <si>
+    <t>condenada a cinco años y un día de presidio mayor en su grado mínimo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso EFE</t>
+  </si>
+  <si>
+    <t>Luis Ajenjo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcaldesa de Recoleta (Sol Letelier)</t>
+  </si>
+  <si>
+    <t>Sol Letelier</t>
+  </si>
+  <si>
+    <t>Campaña política</t>
+  </si>
+  <si>
+    <t>Malversación de fondos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Recoleta (Daniel Jadue)</t>
+  </si>
+  <si>
+    <t>Daniel Jadue</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de Ñuñoa (Pedro Sabat)</t>
+  </si>
+  <si>
+    <t>Pedro Sabat</t>
+  </si>
+  <si>
+    <t>sentencia</t>
+  </si>
+  <si>
+    <t>Alcalde de Buin (Miguel Araya)</t>
+  </si>
+  <si>
+    <t>Miguel Araya</t>
+  </si>
+  <si>
+    <t>Buin</t>
+  </si>
+  <si>
+    <t>fraude al fisco, enriquecimiento ilícito, lavado de activos</t>
+  </si>
+  <si>
+    <t>https://www.elciudadano.com/actualidad/aumenta-la-lista-de-alcaldes-udi-vinculados-a-delitos-de-cuello-y-corbata-miguel-araya-sera-formalizado-el-proximo-6-de-marzo/02/21/</t>
+  </si>
+  <si>
+    <t>https://estapasando.cl/reformalizan-por-nuevos-delitos-a-alcalde-de-buin-udi/</t>
+  </si>
+  <si>
+    <t>Caso Convenios, División de Fomento e Industria (Araucanía)</t>
+  </si>
+  <si>
+    <t>Susan Alarcón</t>
+  </si>
+  <si>
+    <t>fraude al fisco reiterado, cohecho</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios (Enlace Urbano)</t>
+  </si>
+  <si>
+    <t>Fundación Enlace Urbano</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
       <t>https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.elciudadano.com/actualidad/gobernador-de-la-araucania-luciano-rivas-traspaso-mas-de-421-millones-a-fundacion-del-sobrino-apra-de-la-diputada-naveillan-para-capacitacion-a-dirigentes/07/12/</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Motorola (Katherine Martorell)</t>
-  </si>
-  <si>
-    <t>Katherine Martorell</t>
-  </si>
-  <si>
-    <t>Subsecretario</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Convenios (Bonhomía)</t>
-  </si>
-  <si>
-    <t>Republicanos</t>
-  </si>
-  <si>
-    <t>Biobío</t>
-  </si>
-  <si>
-    <t>Fundación Bonhomía</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Guaitecas (Cristian Alvarado Oyarzo)</t>
-  </si>
-  <si>
-    <t>Cristian Alvarado Oyarzo</t>
-  </si>
-  <si>
-    <t>Guaitecas</t>
-  </si>
-  <si>
-    <t>malversación de fondos públicos</t>
-  </si>
-  <si>
-    <t>10 años de presidio</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica</t>
-    </r>
-  </si>
-  <si>
-    <t>Gastos electorales Comunes (Karina Oliva)</t>
-  </si>
-  <si>
-    <t>Karina Oliva</t>
-  </si>
-  <si>
-    <t>Comunes</t>
-  </si>
-  <si>
-    <t>fraude de subvenciones</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Subvenciones</t>
-  </si>
-  <si>
-    <t>Franka Grez</t>
-  </si>
-  <si>
-    <t>Ministro</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Valparaíso (Jorge Castro)</t>
-  </si>
-  <si>
-    <t>Jorge Castro</t>
-  </si>
-  <si>
-    <t>Valparaíso</t>
-  </si>
-  <si>
-    <t>Caso San Ramón</t>
-  </si>
-  <si>
-    <t>Miguel Ángel Aguilera</t>
-  </si>
-  <si>
-    <t>San Ramón</t>
-  </si>
-  <si>
-    <t>Político</t>
-  </si>
-  <si>
-    <t>enriquecimiento ilícito, lavado de activos, cohecho, soborno</t>
-  </si>
-  <si>
-    <t>https://www.ciperchile.cl/2021/06/04/los-millonarios-pagos-al-alcalde-aguilera-y-los-testimonios-de-sus-subordinados-que-lo-tienen-al-borde-del-precipicio/</t>
-  </si>
-  <si>
-    <t>Caso Convenios (RedCultivarte)</t>
-  </si>
-  <si>
-    <t>ONG RedCultivarte</t>
-  </si>
-  <si>
-    <t>Caso Corpesca (Jaime Orpis)</t>
-  </si>
-  <si>
-    <t>Jaime Orpis</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Convenios, arista lencería (Camila Polizzi)</t>
-  </si>
-  <si>
-    <t>Camila Polizzi, Diego Polanco</t>
-  </si>
-  <si>
-    <t>Fundación En tí</t>
-  </si>
-  <si>
-    <t>estafa, falsificación de documento oficial, usurpación de identidad, lavado de activos</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://radio.uchile.cl/2023/11/28/755094/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Puente Alto (Germán Codina)</t>
-  </si>
-  <si>
-    <t>Germán Codina</t>
-  </si>
-  <si>
-    <t>Puente Alto</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Mostazal (Sergio Medel)</t>
-  </si>
-  <si>
-    <t>Sergio Medel</t>
-  </si>
-  <si>
-    <t>Mostazal</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Calama (Daniel Agusto Pérez)</t>
-  </si>
-  <si>
-    <t>Daniel Agusto Pérez</t>
-  </si>
-  <si>
-    <t>Calama</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Santiago (Felipe Alessandri)</t>
-  </si>
-  <si>
-    <t>Felipe Alessandri</t>
-  </si>
-  <si>
-    <t>Santiago</t>
-  </si>
-  <si>
-    <t>Pagos de horas extra, pagos de honorarios</t>
-  </si>
-  <si>
-    <t>Alcalde de Ñuñoa (Andrés Zarhi)</t>
-  </si>
-  <si>
-    <t>Andrés Zarhi</t>
-  </si>
-  <si>
-    <t>Ñuñoa</t>
-  </si>
-  <si>
-    <t>Formalizado</t>
-  </si>
-  <si>
-    <t>arresto domiciliario nocturno, arraigo nacional</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Municipalidad de Linares</t>
-  </si>
-  <si>
-    <t>Mario Meza Vásquez</t>
-  </si>
-  <si>
-    <t>Linares</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Convenios (Atacama)</t>
-  </si>
-  <si>
-    <t>DC, PRO</t>
-  </si>
-  <si>
-    <t>Atacama</t>
-  </si>
-  <si>
-    <t>Fundación Comprometidos</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Administrador municipal de Viña del Mar</t>
-  </si>
-  <si>
-    <t>Claudio Boisier</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde suplente de Tierra Amarilla (Mario Morales)</t>
-  </si>
-  <si>
-    <t>Mario Morales</t>
-  </si>
-  <si>
-    <t>Tierra Amarilla</t>
-  </si>
-  <si>
-    <t>fraude al fisco, cohecho, soborno</t>
-  </si>
-  <si>
-    <t>Prisión preventiva</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml</t>
-    </r>
-  </si>
-  <si>
-    <t>Ex administrador municipal de Tierra Amarilla</t>
-  </si>
-  <si>
-    <t>Jaime Bahamondes Cabrera</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <t>fraude al fisco</t>
-  </si>
-  <si>
-    <t>Condenado</t>
-  </si>
-  <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>presidio, prohibición de cargo público, multa</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> El Tribunal,el marco del caso denominado</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Penta (Pablo Wagner)</t>
-  </si>
-  <si>
-    <t>Pablo Wagner</t>
-  </si>
-  <si>
-    <t>Delitos tributarios, enriquecimiento ilícito</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Las Condes (Joaquín Lavín)</t>
-  </si>
-  <si>
-    <t>Joaquín Lavín Infante</t>
-  </si>
-  <si>
-    <t>Caso Ceresita</t>
-  </si>
-  <si>
-    <t>Recoleta</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.chiletransparente.cl/caso-ceresita/</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de San Fernando (Juan Paulo Molina)</t>
-  </si>
-  <si>
-    <t>Juan Paulo Molina</t>
-  </si>
-  <si>
-    <t>fraude al fisco reiterado</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso Coimas</t>
-  </si>
-  <si>
-    <t>Patricio Tombolini</t>
-  </si>
-  <si>
-    <t>PR, DC</t>
-  </si>
-  <si>
-    <t>cohecho</t>
-  </si>
-  <si>
-    <t>presidio</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://es.wikipedia.org/wiki/Caso_Coimas</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcaldesa de Providencia (Josefa Errázuriz)</t>
-  </si>
-  <si>
-    <t>Josefa Errázuriz</t>
-  </si>
-  <si>
-    <t>Pago de horas extra</t>
-  </si>
-  <si>
-    <t>Responsable pero sin condena</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Sin condena por prescripción</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Claudia Nogueira </t>
-  </si>
-  <si>
-    <t>Diputado</t>
-  </si>
-  <si>
-    <t>https://www.ciperchile.cl/2009/06/12/fiscalia-decide-formalizar-a-diputada-nogueira-e-investiga-pagos-de-la-camara-a-asesores/</t>
-  </si>
-  <si>
-    <t>Caso Main, alcaldesa de Antofagasta (Karen Rojo)</t>
-  </si>
-  <si>
-    <t>Karen Rojo</t>
-  </si>
-  <si>
-    <t>Condenada</t>
-  </si>
-  <si>
-    <t>condenada a cinco años y un día de presidio mayor en su grado mínimo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/</t>
-    </r>
-  </si>
-  <si>
-    <t>Caso EFE</t>
-  </si>
-  <si>
-    <t>Luis Ajenjo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcaldesa de Recoleta (Sol Letelier)</t>
-  </si>
-  <si>
-    <t>Sol Letelier</t>
-  </si>
-  <si>
-    <t>Campaña política</t>
-  </si>
-  <si>
-    <t>Malversación de fondos</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Recoleta (Daniel Jadue)</t>
-  </si>
-  <si>
-    <t>Daniel Jadue</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html</t>
-    </r>
-  </si>
-  <si>
-    <t>Alcalde de Ñuñoa (Pedro Sabat)</t>
-  </si>
-  <si>
-    <t>Pedro Sabat</t>
-  </si>
-  <si>
-    <t>sentencia</t>
-  </si>
-  <si>
-    <t>Alcalde de Buin (Miguel Araya)</t>
-  </si>
-  <si>
-    <t>Miguel Araya</t>
-  </si>
-  <si>
-    <t>Buin</t>
-  </si>
-  <si>
-    <t>fraude al fisco, enriquecimiento ilícito, lavado de activos</t>
-  </si>
-  <si>
-    <t>https://www.elciudadano.com/actualidad/aumenta-la-lista-de-alcaldes-udi-vinculados-a-delitos-de-cuello-y-corbata-miguel-araya-sera-formalizado-el-proximo-6-de-marzo/02/21/</t>
-  </si>
-  <si>
-    <t>https://estapasando.cl/reformalizan-por-nuevos-delitos-a-alcalde-de-buin-udi/</t>
-  </si>
-  <si>
-    <t>Caso Convenios, División de Fomento e Industria (Araucanía)</t>
-  </si>
-  <si>
-    <t>Susan Alarcón</t>
-  </si>
-  <si>
-    <t>Caso Convenios (Enlace Urbano)</t>
-  </si>
-  <si>
-    <t>Fundación Enlace Urbano</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica"/>
-      </rPr>
-      <t>https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html</t>
     </r>
   </si>
 </sst>
@@ -3394,7 +3475,9 @@
     <col min="5" max="5" width="16.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.5469" style="1" customWidth="1"/>
     <col min="7" max="8" width="5.22656" style="1" customWidth="1"/>
-    <col min="9" max="16" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="13" width="16.3516" style="1" customWidth="1"/>
+    <col min="14" max="14" width="23.9453" style="1" customWidth="1"/>
+    <col min="15" max="16" width="16.3516" style="1" customWidth="1"/>
     <col min="17" max="17" width="11.4922" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.6875" style="1" customWidth="1"/>
     <col min="19" max="19" width="22.7344" style="1" customWidth="1"/>
@@ -4609,16 +4692,18 @@
       <c r="N25" t="s" s="27">
         <v>156</v>
       </c>
-      <c r="O25" s="28"/>
+      <c r="O25" t="s" s="27">
+        <v>157</v>
+      </c>
       <c r="P25" s="28"/>
       <c r="Q25" s="25"/>
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
       <c r="T25" t="s" s="27">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="U25" t="s" s="27">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
@@ -4626,7 +4711,7 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="14">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B26" s="15">
         <v>2000000000</v>
@@ -4635,7 +4720,7 @@
         <v>2023</v>
       </c>
       <c r="D26" t="s" s="17">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s" s="17">
         <v>25</v>
@@ -4643,10 +4728,14 @@
       <c r="F26" t="s" s="17">
         <v>131</v>
       </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+      <c r="G26" s="16">
+        <v>2018</v>
+      </c>
+      <c r="H26" s="16">
+        <v>2019</v>
+      </c>
       <c r="I26" t="s" s="17">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J26" t="s" s="17">
         <v>28</v>
@@ -4655,22 +4744,26 @@
       <c r="L26" s="18"/>
       <c r="M26" s="18"/>
       <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
+      <c r="O26" t="s" s="21">
+        <v>163</v>
+      </c>
       <c r="P26" s="20"/>
       <c r="Q26" s="18"/>
       <c r="R26" s="18"/>
       <c r="S26" s="18"/>
       <c r="T26" t="s" s="21">
-        <v>162</v>
-      </c>
-      <c r="U26" s="20"/>
+        <v>164</v>
+      </c>
+      <c r="U26" t="s" s="21">
+        <v>165</v>
+      </c>
       <c r="V26" s="20"/>
       <c r="W26" s="20"/>
       <c r="X26" s="20"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="14">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B27" s="15">
         <v>1700000000</v>
@@ -4692,22 +4785,22 @@
         <v>48</v>
       </c>
       <c r="K27" t="s" s="17">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="L27" s="18"/>
       <c r="M27" t="s" s="17">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N27" s="20"/>
       <c r="O27" t="s" s="21">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="P27" s="20"/>
       <c r="Q27" s="18"/>
       <c r="R27" s="18"/>
       <c r="S27" s="18"/>
       <c r="T27" t="s" s="21">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="U27" s="20"/>
       <c r="V27" s="20"/>
@@ -4716,7 +4809,7 @@
     </row>
     <row r="28" ht="32.05" customHeight="1">
       <c r="A28" t="s" s="14">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B28" s="15">
         <v>1673754000</v>
@@ -4725,7 +4818,7 @@
         <v>2019</v>
       </c>
       <c r="D28" t="s" s="17">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E28" t="s" s="17">
         <v>25</v>
@@ -4736,7 +4829,7 @@
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
       <c r="I28" t="s" s="17">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="J28" t="s" s="17">
         <v>28</v>
@@ -4746,14 +4839,14 @@
       <c r="M28" s="18"/>
       <c r="N28" s="20"/>
       <c r="O28" t="s" s="21">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="P28" s="20"/>
       <c r="Q28" s="18"/>
       <c r="R28" s="18"/>
       <c r="S28" s="18"/>
       <c r="T28" t="s" s="21">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="U28" t="s" s="21">
         <v>83</v>
@@ -4764,7 +4857,7 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="14">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B29" s="15">
         <v>1659000000</v>
@@ -4773,7 +4866,7 @@
         <v>2017</v>
       </c>
       <c r="D29" t="s" s="17">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E29" t="s" s="17">
         <v>36</v>
@@ -4788,24 +4881,24 @@
         <v>48</v>
       </c>
       <c r="K29" t="s" s="17">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="L29" t="s" s="17">
         <v>29</v>
       </c>
       <c r="M29" t="s" s="17">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N29" s="20"/>
       <c r="O29" t="s" s="21">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="P29" s="20"/>
       <c r="Q29" s="18"/>
       <c r="R29" s="18"/>
       <c r="S29" s="18"/>
       <c r="T29" t="s" s="21">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="U29" s="20"/>
       <c r="V29" s="20"/>
@@ -4814,7 +4907,7 @@
     </row>
     <row r="30" ht="32.35" customHeight="1">
       <c r="A30" t="s" s="29">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B30" s="30">
         <v>1600000000</v>
@@ -4830,7 +4923,7 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" t="s" s="26">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J30" t="s" s="26">
         <v>13</v>
@@ -4839,7 +4932,7 @@
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
       <c r="N30" t="s" s="31">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="O30" s="28"/>
       <c r="P30" s="28"/>
@@ -4847,7 +4940,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
       <c r="T30" t="s" s="27">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="U30" s="28"/>
       <c r="V30" s="28"/>
@@ -4856,7 +4949,7 @@
     </row>
     <row r="31" ht="44.05" customHeight="1">
       <c r="A31" t="s" s="14">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B31" s="15">
         <v>1600000000</v>
@@ -4865,13 +4958,13 @@
         <v>2020</v>
       </c>
       <c r="D31" t="s" s="17">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E31" t="s" s="17">
         <v>146</v>
       </c>
       <c r="F31" t="s" s="17">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G31" s="16">
         <v>2020</v>
@@ -4880,10 +4973,10 @@
         <v>2022</v>
       </c>
       <c r="I31" t="s" s="17">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J31" t="s" s="17">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" t="s" s="17">
@@ -4892,18 +4985,18 @@
       <c r="M31" s="18"/>
       <c r="N31" s="20"/>
       <c r="O31" t="s" s="21">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="P31" t="s" s="21">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="Q31" s="18"/>
       <c r="R31" s="18"/>
       <c r="S31" t="s" s="17">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="T31" t="s" s="21">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="U31" s="20"/>
       <c r="V31" s="20"/>
@@ -4912,7 +5005,7 @@
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="14">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B32" s="15">
         <v>1253000000</v>
@@ -4925,7 +5018,7 @@
         <v>146</v>
       </c>
       <c r="F32" t="s" s="17">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G32" s="16">
         <v>1997</v>
@@ -4948,7 +5041,7 @@
         <v>137</v>
       </c>
       <c r="U32" t="s" s="21">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="V32" s="20"/>
       <c r="W32" s="20"/>
@@ -4956,7 +5049,7 @@
     </row>
     <row r="33" ht="32.35" customHeight="1">
       <c r="A33" t="s" s="29">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B33" s="30">
         <v>1200000000</v>
@@ -4970,7 +5063,7 @@
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
       <c r="I33" t="s" s="26">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J33" t="s" s="26">
         <v>13</v>
@@ -4979,7 +5072,7 @@
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
       <c r="N33" t="s" s="31">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="O33" s="28"/>
       <c r="P33" s="28"/>
@@ -4987,7 +5080,7 @@
       <c r="R33" s="25"/>
       <c r="S33" s="25"/>
       <c r="T33" t="s" s="27">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="U33" s="28"/>
       <c r="V33" s="28"/>
@@ -4996,7 +5089,7 @@
     </row>
     <row r="34" ht="20.35" customHeight="1">
       <c r="A34" t="s" s="29">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B34" s="30">
         <v>1200000000</v>
@@ -5012,7 +5105,7 @@
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
       <c r="I34" t="s" s="26">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="J34" t="s" s="26">
         <v>13</v>
@@ -5021,7 +5114,7 @@
       <c r="L34" s="25"/>
       <c r="M34" s="25"/>
       <c r="N34" t="s" s="27">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="O34" s="28"/>
       <c r="P34" s="28"/>
@@ -5029,10 +5122,10 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
       <c r="T34" t="s" s="27">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="U34" t="s" s="27">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="V34" s="28"/>
       <c r="W34" s="28"/>
@@ -5040,7 +5133,7 @@
     </row>
     <row r="35" ht="32.05" customHeight="1">
       <c r="A35" t="s" s="14">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B35" s="15">
         <v>1100000000</v>
@@ -5049,7 +5142,7 @@
         <v>2022</v>
       </c>
       <c r="D35" t="s" s="17">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E35" t="s" s="17">
         <v>25</v>
@@ -5064,7 +5157,7 @@
         <v>2023</v>
       </c>
       <c r="I35" t="s" s="17">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="J35" t="s" s="17">
         <v>28</v>
@@ -5075,13 +5168,15 @@
       </c>
       <c r="M35" s="18"/>
       <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
+      <c r="O35" t="s" s="21">
+        <v>204</v>
+      </c>
       <c r="P35" s="20"/>
       <c r="Q35" s="18"/>
       <c r="R35" s="18"/>
       <c r="S35" s="18"/>
       <c r="T35" t="s" s="21">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="U35" s="20"/>
       <c r="V35" s="20"/>
@@ -5090,7 +5185,7 @@
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" t="s" s="14">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="B36" s="15">
         <v>1000000000</v>
@@ -5099,7 +5194,7 @@
         <v>2023</v>
       </c>
       <c r="D36" t="s" s="17">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="E36" t="s" s="17">
         <v>25</v>
@@ -5110,7 +5205,7 @@
       <c r="G36" s="18"/>
       <c r="H36" s="18"/>
       <c r="I36" t="s" s="17">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="J36" t="s" s="17">
         <v>28</v>
@@ -5122,14 +5217,14 @@
       <c r="M36" s="18"/>
       <c r="N36" s="20"/>
       <c r="O36" t="s" s="21">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="P36" s="20"/>
       <c r="Q36" s="18"/>
       <c r="R36" s="18"/>
       <c r="S36" s="18"/>
       <c r="T36" t="s" s="21">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="U36" s="20"/>
       <c r="V36" s="20"/>
@@ -5138,7 +5233,7 @@
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="14">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B37" s="15">
         <v>946000000</v>
@@ -5176,7 +5271,7 @@
     </row>
     <row r="38" ht="44.05" customHeight="1">
       <c r="A38" t="s" s="14">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B38" s="15">
         <v>847807917</v>
@@ -5185,7 +5280,7 @@
         <v>2024</v>
       </c>
       <c r="D38" t="s" s="17">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
@@ -5203,7 +5298,7 @@
       <c r="R38" s="18"/>
       <c r="S38" s="18"/>
       <c r="T38" t="s" s="21">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="U38" s="20"/>
       <c r="V38" s="20"/>
@@ -5212,7 +5307,7 @@
     </row>
     <row r="39" ht="32.05" customHeight="1">
       <c r="A39" t="s" s="14">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B39" s="15">
         <v>750000000</v>
@@ -5221,7 +5316,7 @@
         <v>2023</v>
       </c>
       <c r="D39" t="s" s="17">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E39" t="s" s="17">
         <v>25</v>
@@ -5236,7 +5331,7 @@
         <v>2015</v>
       </c>
       <c r="I39" t="s" s="17">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="J39" t="s" s="17">
         <v>28</v>
@@ -5246,18 +5341,18 @@
       <c r="M39" s="18"/>
       <c r="N39" s="20"/>
       <c r="O39" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P39" t="s" s="21">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="Q39" s="18"/>
       <c r="R39" s="18"/>
       <c r="S39" t="s" s="21">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="T39" t="s" s="21">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="U39" s="20"/>
       <c r="V39" s="20"/>
@@ -5266,7 +5361,7 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="14">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="B40" s="15">
         <v>680000000</v>
@@ -5275,7 +5370,7 @@
         <v>2018</v>
       </c>
       <c r="D40" t="s" s="17">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E40" t="s" s="17">
         <v>25</v>
@@ -5286,7 +5381,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
       <c r="I40" t="s" s="17">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="J40" t="s" s="17">
         <v>28</v>
@@ -5305,20 +5400,20 @@
       <c r="R40" s="18"/>
       <c r="S40" s="18"/>
       <c r="T40" t="s" s="21">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="U40" t="s" s="21">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="V40" t="s" s="21">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="W40" s="20"/>
       <c r="X40" s="20"/>
     </row>
     <row r="41" ht="32.35" customHeight="1">
       <c r="A41" t="s" s="22">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="B41" s="23">
         <v>658000000</v>
@@ -5327,7 +5422,7 @@
         <v>2023</v>
       </c>
       <c r="D41" t="s" s="26">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E41" t="s" s="26">
         <v>25</v>
@@ -5347,10 +5442,10 @@
       <c r="L41" s="25"/>
       <c r="M41" s="25"/>
       <c r="N41" t="s" s="27">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="O41" t="s" s="27">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="P41" s="28"/>
       <c r="Q41" s="25"/>
@@ -5360,17 +5455,17 @@
         <v>142</v>
       </c>
       <c r="U41" t="s" s="27">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="V41" t="s" s="27">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="W41" s="28"/>
       <c r="X41" s="28"/>
     </row>
     <row r="42" ht="20.35" customHeight="1">
       <c r="A42" t="s" s="29">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="B42" s="23">
         <v>577000000</v>
@@ -5386,7 +5481,7 @@
       <c r="G42" s="25"/>
       <c r="H42" s="25"/>
       <c r="I42" t="s" s="26">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="J42" t="s" s="26">
         <v>13</v>
@@ -5395,10 +5490,10 @@
       <c r="L42" s="25"/>
       <c r="M42" s="25"/>
       <c r="N42" t="s" s="27">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="O42" t="s" s="27">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P42" t="s" s="27">
         <v>77</v>
@@ -5407,10 +5502,10 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
       <c r="T42" t="s" s="27">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="U42" t="s" s="27">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="V42" s="28"/>
       <c r="W42" s="28"/>
@@ -5418,7 +5513,7 @@
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="14">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="B43" s="15">
         <v>497000000</v>
@@ -5427,7 +5522,7 @@
         <v>2020</v>
       </c>
       <c r="D43" t="s" s="17">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="E43" t="s" s="17">
         <v>25</v>
@@ -5438,7 +5533,7 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" t="s" s="17">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J43" t="s" s="17">
         <v>28</v>
@@ -5448,17 +5543,17 @@
       <c r="M43" s="18"/>
       <c r="N43" s="20"/>
       <c r="O43" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P43" s="20"/>
       <c r="Q43" s="18"/>
       <c r="R43" s="18"/>
       <c r="S43" s="18"/>
       <c r="T43" t="s" s="21">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="U43" t="s" s="21">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="V43" s="20"/>
       <c r="W43" s="20"/>
@@ -5466,7 +5561,7 @@
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="14">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="B44" s="15">
         <v>465000000</v>
@@ -5475,7 +5570,7 @@
         <v>2019</v>
       </c>
       <c r="D44" t="s" s="17">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E44" t="s" s="17">
         <v>25</v>
@@ -5492,14 +5587,14 @@
       <c r="M44" s="18"/>
       <c r="N44" s="20"/>
       <c r="O44" t="s" s="21">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="P44" s="20"/>
       <c r="Q44" s="18"/>
       <c r="R44" s="18"/>
       <c r="S44" s="18"/>
       <c r="T44" t="s" s="21">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="U44" s="20"/>
       <c r="V44" s="20"/>
@@ -5508,7 +5603,7 @@
     </row>
     <row r="45" ht="32.35" customHeight="1">
       <c r="A45" t="s" s="22">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="B45" s="23">
         <v>426000000</v>
@@ -5517,18 +5612,18 @@
         <v>2023</v>
       </c>
       <c r="D45" t="s" s="26">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="E45" t="s" s="26">
         <v>146</v>
       </c>
       <c r="F45" t="s" s="26">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G45" s="25"/>
       <c r="H45" s="25"/>
       <c r="I45" t="s" s="26">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="J45" t="s" s="26">
         <v>13</v>
@@ -5537,10 +5632,10 @@
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
       <c r="N45" t="s" s="27">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="O45" t="s" s="27">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P45" s="28"/>
       <c r="Q45" s="25"/>
@@ -5554,9 +5649,9 @@
       <c r="W45" s="28"/>
       <c r="X45" s="28"/>
     </row>
-    <row r="46" ht="32.35" customHeight="1">
+    <row r="46" ht="44.35" customHeight="1">
       <c r="A46" t="s" s="29">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="B46" s="30">
         <v>421000000</v>
@@ -5565,13 +5660,13 @@
         <v>2023</v>
       </c>
       <c r="D46" t="s" s="26">
-        <v>153</v>
+        <v>253</v>
       </c>
       <c r="E46" t="s" s="26">
         <v>25</v>
       </c>
       <c r="F46" t="s" s="26">
-        <v>154</v>
+        <v>254</v>
       </c>
       <c r="G46" s="25"/>
       <c r="H46" s="25"/>
@@ -5585,28 +5680,30 @@
       <c r="L46" s="25"/>
       <c r="M46" s="25"/>
       <c r="N46" t="s" s="27">
-        <v>249</v>
-      </c>
-      <c r="O46" s="28"/>
+        <v>255</v>
+      </c>
+      <c r="O46" t="s" s="27">
+        <v>256</v>
+      </c>
       <c r="P46" s="28"/>
       <c r="Q46" s="25"/>
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
       <c r="T46" t="s" s="27">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="U46" t="s" s="27">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="V46" t="s" s="27">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="W46" s="28"/>
       <c r="X46" s="28"/>
     </row>
     <row r="47" ht="44.05" customHeight="1">
       <c r="A47" t="s" s="14">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="B47" s="15">
         <v>400000000</v>
@@ -5615,7 +5712,7 @@
         <v>2023</v>
       </c>
       <c r="D47" t="s" s="17">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E47" t="s" s="17">
         <v>25</v>
@@ -5625,23 +5722,23 @@
       </c>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
+      <c r="I47" s="25"/>
       <c r="J47" t="s" s="17">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18"/>
       <c r="N47" s="20"/>
       <c r="O47" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P47" s="20"/>
       <c r="Q47" s="18"/>
       <c r="R47" s="18"/>
       <c r="S47" s="18"/>
       <c r="T47" t="s" s="17">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="U47" s="20"/>
       <c r="V47" s="20"/>
@@ -5650,7 +5747,7 @@
     </row>
     <row r="48" ht="20.35" customHeight="1">
       <c r="A48" t="s" s="29">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="B48" s="30">
         <v>356000000</v>
@@ -5663,12 +5760,12 @@
         <v>25</v>
       </c>
       <c r="F48" t="s" s="26">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="G48" s="25"/>
       <c r="H48" s="25"/>
       <c r="I48" t="s" s="26">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="J48" t="s" s="26">
         <v>13</v>
@@ -5677,26 +5774,30 @@
       <c r="L48" s="25"/>
       <c r="M48" s="25"/>
       <c r="N48" t="s" s="27">
-        <v>260</v>
-      </c>
-      <c r="O48" s="28"/>
+        <v>267</v>
+      </c>
+      <c r="O48" t="s" s="27">
+        <v>268</v>
+      </c>
       <c r="P48" s="28"/>
       <c r="Q48" s="25"/>
       <c r="R48" s="25"/>
       <c r="S48" s="25"/>
       <c r="T48" t="s" s="27">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="U48" t="s" s="27">
-        <v>262</v>
-      </c>
-      <c r="V48" s="25"/>
+        <v>270</v>
+      </c>
+      <c r="V48" t="s" s="27">
+        <v>271</v>
+      </c>
       <c r="W48" s="28"/>
       <c r="X48" s="28"/>
     </row>
     <row r="49" ht="32.05" customHeight="1">
       <c r="A49" t="s" s="14">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="B49" s="15">
         <v>351000000</v>
@@ -5705,7 +5806,7 @@
         <v>2021</v>
       </c>
       <c r="D49" t="s" s="17">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="E49" t="s" s="17">
         <v>25</v>
@@ -5720,7 +5821,7 @@
         <v>2016</v>
       </c>
       <c r="I49" t="s" s="17">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="J49" t="s" s="17">
         <v>28</v>
@@ -5730,7 +5831,7 @@
       <c r="M49" s="18"/>
       <c r="N49" s="20"/>
       <c r="O49" t="s" s="21">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="P49" t="s" s="21">
         <v>16</v>
@@ -5738,13 +5839,13 @@
       <c r="Q49" s="18"/>
       <c r="R49" s="18"/>
       <c r="S49" t="s" s="17">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="T49" t="s" s="17">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="U49" t="s" s="21">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="V49" s="20"/>
       <c r="W49" s="20"/>
@@ -5752,7 +5853,7 @@
     </row>
     <row r="50" ht="32.05" customHeight="1">
       <c r="A50" t="s" s="14">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B50" s="15">
         <v>293093681</v>
@@ -5761,13 +5862,13 @@
         <v>2023</v>
       </c>
       <c r="D50" t="s" s="17">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="E50" t="s" s="17">
         <v>146</v>
       </c>
       <c r="F50" t="s" s="17">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
@@ -5778,14 +5879,14 @@
       <c r="M50" s="18"/>
       <c r="N50" s="20"/>
       <c r="O50" t="s" s="21">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="P50" s="20"/>
       <c r="Q50" s="18"/>
       <c r="R50" s="18"/>
       <c r="S50" s="20"/>
       <c r="T50" t="s" s="21">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="U50" s="20"/>
       <c r="V50" s="20"/>
@@ -5794,7 +5895,7 @@
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="14">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B51" s="15">
         <v>290000000</v>
@@ -5803,7 +5904,7 @@
         <v>2006</v>
       </c>
       <c r="D51" t="s" s="17">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E51" t="s" s="17">
         <v>36</v>
@@ -5813,21 +5914,21 @@
       <c r="H51" s="18"/>
       <c r="I51" s="18"/>
       <c r="J51" t="s" s="17">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="K51" s="18"/>
       <c r="L51" s="18"/>
       <c r="M51" s="18"/>
       <c r="N51" s="20"/>
       <c r="O51" t="s" s="21">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="P51" s="20"/>
       <c r="Q51" s="18"/>
       <c r="R51" s="18"/>
       <c r="S51" s="18"/>
       <c r="T51" t="s" s="21">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="U51" s="20"/>
       <c r="V51" s="20"/>
@@ -5836,7 +5937,7 @@
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="14">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="B52" s="15">
         <v>289350646</v>
@@ -5845,7 +5946,7 @@
         <v>2018</v>
       </c>
       <c r="D52" t="s" s="17">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="E52" t="s" s="17">
         <v>25</v>
@@ -5856,7 +5957,7 @@
       <c r="G52" s="18"/>
       <c r="H52" s="18"/>
       <c r="I52" t="s" s="17">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="J52" t="s" s="17">
         <v>28</v>
@@ -5865,7 +5966,9 @@
       <c r="L52" s="18"/>
       <c r="M52" s="18"/>
       <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
+      <c r="O52" t="s" s="21">
+        <v>291</v>
+      </c>
       <c r="P52" s="20"/>
       <c r="Q52" s="18"/>
       <c r="R52" s="18"/>
@@ -5880,7 +5983,7 @@
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="14">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="B53" s="15">
         <v>283000000</v>
@@ -5889,7 +5992,7 @@
         <v>2017</v>
       </c>
       <c r="D53" t="s" s="17">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="E53" t="s" s="17">
         <v>146</v>
@@ -5904,30 +6007,30 @@
         <v>2017</v>
       </c>
       <c r="I53" t="s" s="17">
-        <v>284</v>
+        <v>294</v>
       </c>
       <c r="J53" t="s" s="17">
         <v>28</v>
       </c>
       <c r="K53" t="s" s="17">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="L53" t="s" s="17">
         <v>29</v>
       </c>
       <c r="M53" t="s" s="17">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="N53" s="20"/>
       <c r="O53" t="s" s="21">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="P53" s="20"/>
       <c r="Q53" s="18"/>
       <c r="R53" s="18"/>
       <c r="S53" s="18"/>
       <c r="T53" t="s" s="21">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="U53" s="20"/>
       <c r="V53" s="20"/>
@@ -5936,7 +6039,7 @@
     </row>
     <row r="54" ht="20.35" customHeight="1">
       <c r="A54" t="s" s="22">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B54" s="23">
         <v>274000000</v>
@@ -5952,7 +6055,7 @@
       <c r="G54" s="25"/>
       <c r="H54" s="25"/>
       <c r="I54" t="s" s="26">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="J54" t="s" s="26">
         <v>13</v>
@@ -5961,7 +6064,7 @@
       <c r="L54" s="25"/>
       <c r="M54" s="25"/>
       <c r="N54" t="s" s="27">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="O54" s="28"/>
       <c r="P54" s="28"/>
@@ -5978,7 +6081,7 @@
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="14">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="B55" s="15">
         <v>264254000</v>
@@ -5987,7 +6090,7 @@
         <v>2021</v>
       </c>
       <c r="D55" t="s" s="17">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="E55" t="s" s="17">
         <v>25</v>
@@ -6011,7 +6114,7 @@
       <c r="R55" s="18"/>
       <c r="S55" s="18"/>
       <c r="T55" t="s" s="21">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="U55" s="20"/>
       <c r="V55" s="20"/>
@@ -6020,7 +6123,7 @@
     </row>
     <row r="56" ht="32.35" customHeight="1">
       <c r="A56" t="s" s="22">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="B56" s="23">
         <v>250000000</v>
@@ -6029,7 +6132,7 @@
         <v>2023</v>
       </c>
       <c r="D56" t="s" s="26">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="E56" t="s" s="26">
         <v>146</v>
@@ -6040,7 +6143,7 @@
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
       <c r="I56" t="s" s="26">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="J56" t="s" s="26">
         <v>13</v>
@@ -6049,30 +6152,30 @@
       <c r="L56" s="25"/>
       <c r="M56" s="25"/>
       <c r="N56" t="s" s="27">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="O56" t="s" s="27">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="P56" s="28"/>
       <c r="Q56" s="25"/>
       <c r="R56" s="25"/>
       <c r="S56" s="25"/>
       <c r="T56" t="s" s="27">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="U56" t="s" s="27">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="V56" t="s" s="27">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="W56" s="28"/>
       <c r="X56" s="28"/>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="14">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B57" s="15">
         <v>203000000</v>
@@ -6081,7 +6184,7 @@
         <v>2018</v>
       </c>
       <c r="D57" t="s" s="17">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="E57" t="s" s="17">
         <v>25</v>
@@ -6092,7 +6195,7 @@
       <c r="G57" s="18"/>
       <c r="H57" s="18"/>
       <c r="I57" t="s" s="17">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="J57" t="s" s="17">
         <v>28</v>
@@ -6109,7 +6212,7 @@
       <c r="R57" s="18"/>
       <c r="S57" s="18"/>
       <c r="T57" t="s" s="21">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="U57" t="s" s="21">
         <v>83</v>
@@ -6120,7 +6223,7 @@
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="14">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="B58" s="15">
         <v>200000000</v>
@@ -6129,7 +6232,7 @@
         <v>2022</v>
       </c>
       <c r="D58" t="s" s="17">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="E58" t="s" s="17">
         <v>25</v>
@@ -6144,7 +6247,7 @@
         <v>2021</v>
       </c>
       <c r="I58" t="s" s="17">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="J58" t="s" s="17">
         <v>28</v>
@@ -6161,20 +6264,20 @@
       <c r="R58" s="18"/>
       <c r="S58" s="18"/>
       <c r="T58" t="s" s="21">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="U58" t="s" s="21">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="V58" t="s" s="21">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="W58" s="20"/>
       <c r="X58" s="20"/>
     </row>
     <row r="59" ht="32.05" customHeight="1">
       <c r="A59" t="s" s="14">
-        <v>309</v>
+        <v>319</v>
       </c>
       <c r="B59" s="15">
         <v>190000000</v>
@@ -6183,7 +6286,7 @@
         <v>2024</v>
       </c>
       <c r="D59" t="s" s="17">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="E59" t="s" s="17">
         <v>25</v>
@@ -6194,7 +6297,7 @@
       <c r="G59" s="18"/>
       <c r="H59" s="18"/>
       <c r="I59" t="s" s="17">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="J59" t="s" s="17">
         <v>28</v>
@@ -6204,17 +6307,17 @@
       <c r="M59" s="18"/>
       <c r="N59" s="20"/>
       <c r="O59" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P59" s="20"/>
       <c r="Q59" s="18"/>
       <c r="R59" s="18"/>
       <c r="S59" s="20"/>
       <c r="T59" t="s" s="21">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="U59" t="s" s="21">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="V59" s="20"/>
       <c r="W59" s="20"/>
@@ -6222,7 +6325,7 @@
     </row>
     <row r="60" ht="20.05" customHeight="1">
       <c r="A60" t="s" s="14">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="B60" s="15">
         <v>188000000</v>
@@ -6231,7 +6334,7 @@
         <v>2021</v>
       </c>
       <c r="D60" t="s" s="17">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="E60" t="s" s="17">
         <v>25</v>
@@ -6242,7 +6345,7 @@
       <c r="G60" s="18"/>
       <c r="H60" s="18"/>
       <c r="I60" t="s" s="17">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="J60" t="s" s="17">
         <v>28</v>
@@ -6252,7 +6355,7 @@
       <c r="M60" s="18"/>
       <c r="N60" s="20"/>
       <c r="O60" t="s" s="21">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="P60" s="20"/>
       <c r="Q60" s="18"/>
@@ -6268,7 +6371,7 @@
     </row>
     <row r="61" ht="32.05" customHeight="1">
       <c r="A61" t="s" s="14">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="B61" s="15">
         <v>176000000</v>
@@ -6277,7 +6380,7 @@
         <v>2024</v>
       </c>
       <c r="D61" t="s" s="17">
-        <v>319</v>
+        <v>329</v>
       </c>
       <c r="E61" t="s" s="17">
         <v>25</v>
@@ -6292,7 +6395,7 @@
         <v>2021</v>
       </c>
       <c r="I61" t="s" s="17">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="J61" t="s" s="17">
         <v>28</v>
@@ -6304,21 +6407,21 @@
       <c r="M61" s="18"/>
       <c r="N61" s="20"/>
       <c r="O61" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P61" t="s" s="21">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="Q61" s="18"/>
       <c r="R61" s="18"/>
       <c r="S61" t="s" s="17">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="T61" t="s" s="21">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="U61" t="s" s="21">
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="V61" s="20"/>
       <c r="W61" s="20"/>
@@ -6326,7 +6429,7 @@
     </row>
     <row r="62" ht="20.05" customHeight="1">
       <c r="A62" t="s" s="14">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="B62" s="15">
         <v>139739316</v>
@@ -6335,7 +6438,7 @@
         <v>2020</v>
       </c>
       <c r="D62" t="s" s="17">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="E62" t="s" s="17">
         <v>25</v>
@@ -6350,7 +6453,7 @@
         <v>2020</v>
       </c>
       <c r="I62" t="s" s="17">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="J62" t="s" s="17">
         <v>28</v>
@@ -6365,7 +6468,7 @@
       <c r="R62" s="18"/>
       <c r="S62" s="18"/>
       <c r="T62" t="s" s="21">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="U62" s="20"/>
       <c r="V62" s="20"/>
@@ -6374,7 +6477,7 @@
     </row>
     <row r="63" ht="20.35" customHeight="1">
       <c r="A63" t="s" s="22">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="B63" s="23">
         <v>128000000</v>
@@ -6387,12 +6490,12 @@
         <v>146</v>
       </c>
       <c r="F63" t="s" s="26">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="G63" s="25"/>
       <c r="H63" s="25"/>
       <c r="I63" t="s" s="26">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="J63" t="s" s="26">
         <v>13</v>
@@ -6401,7 +6504,7 @@
       <c r="L63" s="25"/>
       <c r="M63" s="25"/>
       <c r="N63" t="s" s="27">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="O63" s="28"/>
       <c r="P63" s="28"/>
@@ -6412,7 +6515,7 @@
         <v>142</v>
       </c>
       <c r="U63" t="s" s="27">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="V63" s="28"/>
       <c r="W63" s="28"/>
@@ -6420,7 +6523,7 @@
     </row>
     <row r="64" ht="32.05" customHeight="1">
       <c r="A64" t="s" s="14">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="B64" s="15">
         <v>104000000</v>
@@ -6429,7 +6532,7 @@
         <v>2024</v>
       </c>
       <c r="D64" t="s" s="17">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="E64" t="s" s="17">
         <v>25</v>
@@ -6447,24 +6550,24 @@
         <v>27</v>
       </c>
       <c r="J64" t="s" s="17">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K64" s="18"/>
       <c r="L64" s="18"/>
       <c r="M64" s="18"/>
       <c r="N64" s="20"/>
       <c r="O64" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P64" s="20"/>
       <c r="Q64" s="18"/>
       <c r="R64" s="18"/>
       <c r="S64" s="18"/>
       <c r="T64" t="s" s="21">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="U64" t="s" s="21">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="V64" s="20"/>
       <c r="W64" s="20"/>
@@ -6472,7 +6575,7 @@
     </row>
     <row r="65" ht="32.05" customHeight="1">
       <c r="A65" t="s" s="14">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B65" s="15">
         <v>102000000</v>
@@ -6481,7 +6584,7 @@
         <v>2020</v>
       </c>
       <c r="D65" t="s" s="17">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="E65" t="s" s="17">
         <v>146</v>
@@ -6496,7 +6599,7 @@
         <v>2020</v>
       </c>
       <c r="I65" t="s" s="17">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="J65" t="s" s="17">
         <v>28</v>
@@ -6508,16 +6611,16 @@
       <c r="M65" s="18"/>
       <c r="N65" s="20"/>
       <c r="O65" t="s" s="21">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="P65" t="s" s="21">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="Q65" s="18"/>
       <c r="R65" s="18"/>
       <c r="S65" s="18"/>
       <c r="T65" t="s" s="21">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="U65" s="20"/>
       <c r="V65" s="20"/>
@@ -6526,7 +6629,7 @@
     </row>
     <row r="66" ht="32.05" customHeight="1">
       <c r="A66" t="s" s="14">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="B66" s="15">
         <v>80069002</v>
@@ -6535,13 +6638,13 @@
         <v>2023</v>
       </c>
       <c r="D66" t="s" s="17">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="E66" t="s" s="17">
         <v>73</v>
       </c>
       <c r="F66" t="s" s="17">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="G66" s="16">
         <v>2022</v>
@@ -6550,10 +6653,10 @@
         <v>2023</v>
       </c>
       <c r="I66" t="s" s="17">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="J66" t="s" s="17">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K66" t="s" s="17">
         <v>28</v>
@@ -6564,25 +6667,25 @@
       <c r="M66" s="18"/>
       <c r="N66" s="20"/>
       <c r="O66" t="s" s="21">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="P66" t="s" s="21">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="Q66" t="s" s="17">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="R66" t="s" s="17">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="S66" t="s" s="17">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="T66" t="s" s="21">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="U66" t="s" s="21">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="V66" s="20"/>
       <c r="W66" s="20"/>
@@ -6590,7 +6693,7 @@
     </row>
     <row r="67" ht="20.05" customHeight="1">
       <c r="A67" t="s" s="14">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="B67" s="15">
         <v>66000000</v>
@@ -6599,7 +6702,7 @@
         <v>2018</v>
       </c>
       <c r="D67" t="s" s="17">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="E67" t="s" s="17">
         <v>25</v>
@@ -6611,21 +6714,21 @@
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
       <c r="J67" t="s" s="17">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18"/>
       <c r="N67" s="20"/>
       <c r="O67" t="s" s="21">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="P67" s="20"/>
       <c r="Q67" s="18"/>
       <c r="R67" s="18"/>
       <c r="S67" s="18"/>
       <c r="T67" t="s" s="21">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="U67" s="20"/>
       <c r="V67" s="20"/>
@@ -6634,7 +6737,7 @@
     </row>
     <row r="68" ht="20.05" customHeight="1">
       <c r="A68" t="s" s="14">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="B68" s="15">
         <v>59595096</v>
@@ -6643,7 +6746,7 @@
         <v>2020</v>
       </c>
       <c r="D68" t="s" s="17">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="E68" t="s" s="17">
         <v>25</v>
@@ -6678,7 +6781,7 @@
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="14">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="B69" s="15">
         <v>40000000</v>
@@ -6698,7 +6801,7 @@
         <v>2013</v>
       </c>
       <c r="I69" t="s" s="17">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="J69" t="s" s="17">
         <v>48</v>
@@ -6713,7 +6816,7 @@
       <c r="R69" s="18"/>
       <c r="S69" s="18"/>
       <c r="T69" t="s" s="21">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="U69" s="20"/>
       <c r="V69" s="20"/>
@@ -6722,7 +6825,7 @@
     </row>
     <row r="70" ht="32.05" customHeight="1">
       <c r="A70" t="s" s="14">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="B70" s="15">
         <v>37550000</v>
@@ -6731,13 +6834,13 @@
         <v>2023</v>
       </c>
       <c r="D70" t="s" s="17">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="E70" t="s" s="17">
         <v>36</v>
       </c>
       <c r="F70" t="s" s="17">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="G70" s="16">
         <v>2018</v>
@@ -6756,14 +6859,14 @@
       <c r="M70" s="18"/>
       <c r="N70" s="20"/>
       <c r="O70" t="s" s="21">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="P70" s="20"/>
       <c r="Q70" s="18"/>
       <c r="R70" s="18"/>
       <c r="S70" s="18"/>
       <c r="T70" t="s" s="21">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="U70" s="20"/>
       <c r="V70" s="20"/>
@@ -6772,7 +6875,7 @@
     </row>
     <row r="71" ht="20.05" customHeight="1">
       <c r="A71" t="s" s="14">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B71" s="15">
         <v>35000000</v>
@@ -6781,13 +6884,13 @@
         <v>2002</v>
       </c>
       <c r="D71" t="s" s="17">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="E71" t="s" s="17">
         <v>146</v>
       </c>
       <c r="F71" t="s" s="17">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="18"/>
@@ -6798,19 +6901,19 @@
       <c r="M71" s="18"/>
       <c r="N71" s="20"/>
       <c r="O71" t="s" s="21">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="P71" s="20"/>
       <c r="Q71" s="18"/>
       <c r="R71" s="18"/>
       <c r="S71" t="s" s="17">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="T71" t="s" s="21">
         <v>137</v>
       </c>
       <c r="U71" t="s" s="21">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="V71" s="20"/>
       <c r="W71" s="20"/>
@@ -6818,7 +6921,7 @@
     </row>
     <row r="72" ht="32.05" customHeight="1">
       <c r="A72" t="s" s="14">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="B72" s="15">
         <v>31000000</v>
@@ -6827,7 +6930,7 @@
         <v>2019</v>
       </c>
       <c r="D72" t="s" s="17">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="E72" t="s" s="17">
         <v>146</v>
@@ -6842,7 +6945,7 @@
         <v>2019</v>
       </c>
       <c r="I72" t="s" s="17">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="J72" t="s" s="17">
         <v>28</v>
@@ -6854,22 +6957,22 @@
       <c r="M72" s="18"/>
       <c r="N72" s="20"/>
       <c r="O72" t="s" s="21">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="P72" t="s" s="21">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="Q72" t="s" s="17">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="R72" t="s" s="17">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="S72" t="s" s="17">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="T72" t="s" s="21">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="U72" s="20"/>
       <c r="V72" s="20"/>
@@ -6878,7 +6981,7 @@
     </row>
     <row r="73" ht="20.05" customHeight="1">
       <c r="A73" t="s" s="14">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="B73" s="15">
         <v>30000000</v>
@@ -6887,7 +6990,7 @@
         <v>2009</v>
       </c>
       <c r="D73" t="s" s="17">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="E73" t="s" s="17">
         <v>25</v>
@@ -6901,7 +7004,7 @@
       <c r="H73" s="18"/>
       <c r="I73" s="18"/>
       <c r="J73" t="s" s="17">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="K73" s="18"/>
       <c r="L73" s="18"/>
@@ -6913,7 +7016,7 @@
       <c r="R73" s="18"/>
       <c r="S73" s="18"/>
       <c r="T73" t="s" s="21">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="U73" s="20"/>
       <c r="V73" s="20"/>
@@ -6922,7 +7025,7 @@
     </row>
     <row r="74" ht="44.05" customHeight="1">
       <c r="A74" t="s" s="14">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="B74" s="15">
         <v>24000000</v>
@@ -6931,7 +7034,7 @@
         <v>2022</v>
       </c>
       <c r="D74" t="s" s="17">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="E74" t="s" s="17">
         <v>25</v>
@@ -6946,7 +7049,7 @@
         <v>2016</v>
       </c>
       <c r="I74" t="s" s="17">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="J74" t="s" s="17">
         <v>28</v>
@@ -6956,31 +7059,31 @@
       <c r="M74" s="18"/>
       <c r="N74" s="20"/>
       <c r="O74" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P74" t="s" s="21">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="Q74" s="18"/>
       <c r="R74" s="18"/>
       <c r="S74" t="s" s="17">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="T74" t="s" s="21">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="U74" t="s" s="21">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="V74" t="s" s="21">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="W74" s="20"/>
       <c r="X74" s="20"/>
     </row>
     <row r="75" ht="20.05" customHeight="1">
       <c r="A75" t="s" s="14">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="B75" s="15">
         <v>23671000</v>
@@ -6989,13 +7092,13 @@
         <v>2008</v>
       </c>
       <c r="D75" t="s" s="17">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="E75" t="s" s="17">
         <v>73</v>
       </c>
       <c r="F75" t="s" s="17">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="G75" s="16">
         <v>2004</v>
@@ -7010,7 +7113,7 @@
       <c r="M75" s="18"/>
       <c r="N75" s="20"/>
       <c r="O75" t="s" s="21">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="P75" s="20"/>
       <c r="Q75" s="18"/>
@@ -7020,7 +7123,7 @@
         <v>137</v>
       </c>
       <c r="U75" t="s" s="21">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="V75" s="20"/>
       <c r="W75" s="20"/>
@@ -7028,7 +7131,7 @@
     </row>
     <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="14">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B76" s="15">
         <v>22917478</v>
@@ -7037,7 +7140,7 @@
         <v>2013</v>
       </c>
       <c r="D76" t="s" s="17">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="E76" t="s" s="17">
         <v>25</v>
@@ -7052,30 +7155,30 @@
         <v>2012</v>
       </c>
       <c r="I76" t="s" s="17">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="J76" t="s" s="17">
         <v>28</v>
       </c>
       <c r="K76" t="s" s="17">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="L76" t="s" s="17">
         <v>29</v>
       </c>
       <c r="M76" t="s" s="17">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="N76" s="20"/>
       <c r="O76" t="s" s="21">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="P76" s="20"/>
       <c r="Q76" s="18"/>
       <c r="R76" s="18"/>
       <c r="S76" s="18"/>
       <c r="T76" t="s" s="21">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="U76" s="20"/>
       <c r="V76" s="20"/>
@@ -7084,7 +7187,7 @@
     </row>
     <row r="77" ht="20.05" customHeight="1">
       <c r="A77" t="s" s="14">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="B77" s="15">
         <v>20000000</v>
@@ -7093,13 +7196,13 @@
         <v>2023</v>
       </c>
       <c r="D77" t="s" s="17">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="E77" t="s" s="17">
         <v>146</v>
       </c>
       <c r="F77" t="s" s="17">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="G77" s="16">
         <v>2023</v>
@@ -7108,7 +7211,7 @@
         <v>2024</v>
       </c>
       <c r="I77" t="s" s="17">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="J77" t="s" s="17">
         <v>28</v>
@@ -7122,7 +7225,7 @@
       <c r="M77" s="18"/>
       <c r="N77" s="20"/>
       <c r="O77" t="s" s="21">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="P77" t="s" s="21">
         <v>77</v>
@@ -7131,7 +7234,7 @@
       <c r="R77" s="18"/>
       <c r="S77" s="18"/>
       <c r="T77" t="s" s="21">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="U77" s="20"/>
       <c r="V77" s="20"/>
@@ -7140,7 +7243,7 @@
     </row>
     <row r="78" ht="20.05" customHeight="1">
       <c r="A78" t="s" s="14">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="B78" s="15">
         <v>15700000</v>
@@ -7149,7 +7252,7 @@
         <v>2015</v>
       </c>
       <c r="D78" t="s" s="17">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="E78" t="s" s="17">
         <v>25</v>
@@ -7160,7 +7263,7 @@
       <c r="G78" s="18"/>
       <c r="H78" s="18"/>
       <c r="I78" t="s" s="17">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="J78" t="s" s="17">
         <v>28</v>
@@ -7176,7 +7279,7 @@
       <c r="Q78" s="18"/>
       <c r="R78" s="18"/>
       <c r="S78" t="s" s="17">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="T78" t="s" s="21">
         <v>83</v>
@@ -7188,7 +7291,7 @@
     </row>
     <row r="79" ht="20.05" customHeight="1">
       <c r="A79" t="s" s="14">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B79" s="15">
         <v>10333332</v>
@@ -7197,7 +7300,7 @@
         <v>2024</v>
       </c>
       <c r="D79" t="s" s="17">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="E79" t="s" s="17">
         <v>25</v>
@@ -7212,7 +7315,7 @@
         <v>2024</v>
       </c>
       <c r="I79" t="s" s="17">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="J79" t="s" s="17">
         <v>28</v>
@@ -7224,7 +7327,7 @@
       <c r="M79" s="18"/>
       <c r="N79" s="20"/>
       <c r="O79" t="s" s="21">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="P79" t="s" s="21">
         <v>77</v>
@@ -7233,10 +7336,10 @@
       <c r="R79" s="18"/>
       <c r="S79" s="18"/>
       <c r="T79" t="s" s="21">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="U79" t="s" s="21">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="V79" s="20"/>
       <c r="W79" s="20"/>
@@ -7244,7 +7347,7 @@
     </row>
     <row r="80" ht="32.35" customHeight="1">
       <c r="A80" t="s" s="29">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="B80" s="23">
         <v>9000000</v>
@@ -7253,7 +7356,7 @@
         <v>2023</v>
       </c>
       <c r="D80" t="s" s="32">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="E80" t="s" s="26">
         <v>25</v>
@@ -7273,26 +7376,30 @@
       <c r="L80" s="25"/>
       <c r="M80" s="25"/>
       <c r="N80" t="s" s="27">
-        <v>226</v>
-      </c>
-      <c r="O80" s="28"/>
+        <v>230</v>
+      </c>
+      <c r="O80" t="s" s="27">
+        <v>422</v>
+      </c>
       <c r="P80" s="28"/>
       <c r="Q80" s="25"/>
       <c r="R80" s="25"/>
       <c r="S80" s="25"/>
       <c r="T80" t="s" s="27">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="U80" t="s" s="27">
-        <v>251</v>
-      </c>
-      <c r="V80" s="28"/>
+        <v>258</v>
+      </c>
+      <c r="V80" t="s" s="27">
+        <v>423</v>
+      </c>
       <c r="W80" s="28"/>
       <c r="X80" s="28"/>
     </row>
     <row r="81" ht="20.35" customHeight="1">
       <c r="A81" t="s" s="29">
-        <v>412</v>
+        <v>424</v>
       </c>
       <c r="B81" s="30">
         <v>1022000</v>
@@ -7308,7 +7415,7 @@
       <c r="G81" s="25"/>
       <c r="H81" s="25"/>
       <c r="I81" t="s" s="26">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="J81" t="s" s="26">
         <v>13</v>
@@ -7317,7 +7424,7 @@
       <c r="L81" s="25"/>
       <c r="M81" s="25"/>
       <c r="N81" t="s" s="27">
-        <v>413</v>
+        <v>425</v>
       </c>
       <c r="O81" s="28"/>
       <c r="P81" s="28"/>
@@ -7325,10 +7432,10 @@
       <c r="R81" s="25"/>
       <c r="S81" s="25"/>
       <c r="T81" t="s" s="27">
-        <v>414</v>
+        <v>426</v>
       </c>
       <c r="U81" t="s" s="27">
-        <v>250</v>
+        <v>427</v>
       </c>
       <c r="V81" s="28"/>
       <c r="W81" s="28"/>
@@ -7377,86 +7484,89 @@
     <hyperlink ref="U24" r:id="rId31" location="" tooltip="" display="https://radio.uchile.cl/2023/03/04/tras-allanamiento-a-alcalde-de-rancagua-expertos-en-transparencia-llaman-a-fortalecer-los-mecanismos-para-perseguir-la-corrupcion/"/>
     <hyperlink ref="U25" r:id="rId32" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml"/>
     <hyperlink ref="T26" r:id="rId33" location="" tooltip="" display="https://www.cnnchile.com/pais/destitucion-alcalde-rinconada-contraloria-irregularidades_20230606/"/>
-    <hyperlink ref="T27" r:id="rId34" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
-    <hyperlink ref="T28" r:id="rId35" location="" tooltip="" display="https://www.ovejeronoticias.cl/2023/12/puerto-natales-ex-alcalde-udi-fernando-paredes-continua-con-reclusion-domiciliaria-total/"/>
-    <hyperlink ref="U28" r:id="rId36" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T29" r:id="rId37" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
-    <hyperlink ref="T30" r:id="rId38" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T31" r:id="rId39" location="" tooltip="" display="https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022"/>
-    <hyperlink ref="T32" r:id="rId40" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U32" r:id="rId41" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
-    <hyperlink ref="T33" r:id="rId42" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T34" r:id="rId43" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="U34" r:id="rId44" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T35" r:id="rId45" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
-    <hyperlink ref="T36" r:id="rId46" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
-    <hyperlink ref="T37" r:id="rId47" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="T38" r:id="rId48" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/03/19/milicogate-dictan-procesamiento-contra-general-y-coroneles-r-por-presunto-fraude-de-519-millones.shtml"/>
-    <hyperlink ref="T40" r:id="rId49" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
-    <hyperlink ref="U40" r:id="rId50" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
-    <hyperlink ref="V40" r:id="rId51" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
-    <hyperlink ref="T41" r:id="rId52" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="U41" r:id="rId53" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
-    <hyperlink ref="V41" r:id="rId54" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/12/29/caso-manicure/"/>
-    <hyperlink ref="T42" r:id="rId55" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/11/pdi-allano-gobernacion-del-maule-en-medio-de-investigaciones-por-traspasos-a-urbanismo-social.shtml"/>
-    <hyperlink ref="U42" r:id="rId56" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/12/caso-convenios-jefe-de-control-interno-del-gore-maule-declaro-por-traspasos-a-urbanismo-social.shtml"/>
-    <hyperlink ref="T43" r:id="rId57" location="" tooltip="" display="https://www.eldesconcierto.cl/reportajes/2024/01/23/municipio-se-querella-por-multa-de-500-millones-acusan-a-exalcalde-de-melipilla-por-fraude-al-fisco.html"/>
-    <hyperlink ref="U43" r:id="rId58" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/municipalidad-de-melipilla-presenta-querella-por-fraude-al-fisco-contra-el-exalcalde-ivan-campos/P6XRT2X73NAHJIEMIZWPRX6VEU/"/>
-    <hyperlink ref="T44" r:id="rId59" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2019/05/05/las-vueltas-de-la-vida-rn-elige-a-claudio-eguiluz-condenado-por-caso-sqm-como-su-presidente-regional-en-el-biobio/"/>
-    <hyperlink ref="T45" r:id="rId60" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="T46" r:id="rId61" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
-    <hyperlink ref="U46" r:id="rId62" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
-    <hyperlink ref="V46" r:id="rId63" location="" tooltip="" display="https://www.elciudadano.com/actualidad/gobernador-de-la-araucania-luciano-rivas-traspaso-mas-de-421-millones-a-fundacion-del-sobrino-apra-de-la-diputada-naveillan-para-capacitacion-a-dirigentes/07/12/"/>
-    <hyperlink ref="T47" r:id="rId64" location="" tooltip="" display="https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/"/>
-    <hyperlink ref="T48" r:id="rId65" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml"/>
-    <hyperlink ref="U48" r:id="rId66" location="" tooltip="" display="https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana"/>
-    <hyperlink ref="T49" r:id="rId67" location="" tooltip="" display="http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739"/>
-    <hyperlink ref="U49" r:id="rId68" location="" tooltip="" display="https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica"/>
-    <hyperlink ref="T50" r:id="rId69" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
-    <hyperlink ref="T51" r:id="rId70" location="" tooltip="" display="https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/"/>
-    <hyperlink ref="T52" r:id="rId71" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T54" r:id="rId72" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="T55" r:id="rId73" location="" tooltip="" display="https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/"/>
-    <hyperlink ref="T56" r:id="rId74" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
-    <hyperlink ref="U56" r:id="rId75" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
-    <hyperlink ref="V56" r:id="rId76" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="T57" r:id="rId77" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
-    <hyperlink ref="U57" r:id="rId78" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T58" r:id="rId79" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
-    <hyperlink ref="U58" r:id="rId80" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
-    <hyperlink ref="V58" r:id="rId81" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
-    <hyperlink ref="T59" r:id="rId82" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
-    <hyperlink ref="U59" r:id="rId83" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml"/>
-    <hyperlink ref="T60" r:id="rId84" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T61" r:id="rId85" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
-    <hyperlink ref="U61" r:id="rId86" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
-    <hyperlink ref="T62" r:id="rId87" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html"/>
-    <hyperlink ref="T63" r:id="rId88" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="U63" r:id="rId89" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
-    <hyperlink ref="T64" r:id="rId90" location="" tooltip="" display="https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/"/>
-    <hyperlink ref="U64" r:id="rId91" location="" tooltip="" display="https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html"/>
-    <hyperlink ref="T65" r:id="rId92" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
-    <hyperlink ref="T66" r:id="rId93" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
-    <hyperlink ref="U66" r:id="rId94" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
-    <hyperlink ref="T67" r:id="rId95" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
-    <hyperlink ref="T68" r:id="rId96" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T69" r:id="rId97" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
-    <hyperlink ref="T70" r:id="rId98" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
-    <hyperlink ref="T71" r:id="rId99" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U71" r:id="rId100" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
-    <hyperlink ref="T72" r:id="rId101" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
-    <hyperlink ref="T74" r:id="rId102" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
-    <hyperlink ref="U74" r:id="rId103" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
-    <hyperlink ref="V74" r:id="rId104" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
-    <hyperlink ref="T75" r:id="rId105" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U75" r:id="rId106" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
-    <hyperlink ref="T76" r:id="rId107" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
-    <hyperlink ref="T77" r:id="rId108" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
-    <hyperlink ref="T78" r:id="rId109" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T80" r:id="rId110" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="U80" r:id="rId111" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
-    <hyperlink ref="T81" r:id="rId112" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
-    <hyperlink ref="U81" r:id="rId113" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
+    <hyperlink ref="U26" r:id="rId34" location="" tooltip="" display="https://munirinconada.cl/alcalde-juan-galdames-se-refiere-a-juicio-de-cuentas-que-ordena-la-restitucion-de-300-millones/#:~:text=Municipal-,Alcalde"/>
+    <hyperlink ref="T27" r:id="rId35" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
+    <hyperlink ref="T28" r:id="rId36" location="" tooltip="" display="https://www.ovejeronoticias.cl/2023/12/puerto-natales-ex-alcalde-udi-fernando-paredes-continua-con-reclusion-domiciliaria-total/"/>
+    <hyperlink ref="U28" r:id="rId37" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T29" r:id="rId38" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
+    <hyperlink ref="T30" r:id="rId39" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T31" r:id="rId40" location="" tooltip="" display="https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022"/>
+    <hyperlink ref="T32" r:id="rId41" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U32" r:id="rId42" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
+    <hyperlink ref="T33" r:id="rId43" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T34" r:id="rId44" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="U34" r:id="rId45" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T35" r:id="rId46" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
+    <hyperlink ref="T36" r:id="rId47" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
+    <hyperlink ref="T37" r:id="rId48" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="T38" r:id="rId49" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/03/19/milicogate-dictan-procesamiento-contra-general-y-coroneles-r-por-presunto-fraude-de-519-millones.shtml"/>
+    <hyperlink ref="T40" r:id="rId50" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
+    <hyperlink ref="U40" r:id="rId51" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
+    <hyperlink ref="V40" r:id="rId52" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
+    <hyperlink ref="T41" r:id="rId53" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="U41" r:id="rId54" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
+    <hyperlink ref="V41" r:id="rId55" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/12/29/caso-manicure/"/>
+    <hyperlink ref="T42" r:id="rId56" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/11/pdi-allano-gobernacion-del-maule-en-medio-de-investigaciones-por-traspasos-a-urbanismo-social.shtml"/>
+    <hyperlink ref="U42" r:id="rId57" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/12/caso-convenios-jefe-de-control-interno-del-gore-maule-declaro-por-traspasos-a-urbanismo-social.shtml"/>
+    <hyperlink ref="T43" r:id="rId58" location="" tooltip="" display="https://www.eldesconcierto.cl/reportajes/2024/01/23/municipio-se-querella-por-multa-de-500-millones-acusan-a-exalcalde-de-melipilla-por-fraude-al-fisco.html"/>
+    <hyperlink ref="U43" r:id="rId59" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/municipalidad-de-melipilla-presenta-querella-por-fraude-al-fisco-contra-el-exalcalde-ivan-campos/P6XRT2X73NAHJIEMIZWPRX6VEU/"/>
+    <hyperlink ref="T44" r:id="rId60" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2019/05/05/las-vueltas-de-la-vida-rn-elige-a-claudio-eguiluz-condenado-por-caso-sqm-como-su-presidente-regional-en-el-biobio/"/>
+    <hyperlink ref="T45" r:id="rId61" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="T46" r:id="rId62" location="" tooltip="" display="https://radionuevomundo.cl/2023/07/18/gobernador-rivas-suma-al-caso-fundacion-local-traspasos-arbitrarios-a-coihue-y-a-universidades-de-la-araucania/"/>
+    <hyperlink ref="U46" r:id="rId63" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
+    <hyperlink ref="V46" r:id="rId64" location="" tooltip="" display="https://resumen.cl/articulos/la-derecha-de-la-araucania-en-el-caso-fundaciones-las-irregularidades-de-espacio-coigue-que-llevaron-al-ministerio-de-justicia-a-solicitar-su-cierre"/>
+    <hyperlink ref="T47" r:id="rId65" location="" tooltip="" display="https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/"/>
+    <hyperlink ref="T48" r:id="rId66" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml"/>
+    <hyperlink ref="U48" r:id="rId67" location="" tooltip="" display="https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana"/>
+    <hyperlink ref="V48" r:id="rId68" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-biobio/detienen-a-lider-de-empresa-en-allanamiento-por-caso-convenios-pdi/2024-03-13/123002.html"/>
+    <hyperlink ref="T49" r:id="rId69" location="" tooltip="" display="http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739"/>
+    <hyperlink ref="U49" r:id="rId70" location="" tooltip="" display="https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica"/>
+    <hyperlink ref="T50" r:id="rId71" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
+    <hyperlink ref="T51" r:id="rId72" location="" tooltip="" display="https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/"/>
+    <hyperlink ref="T52" r:id="rId73" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T54" r:id="rId74" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="T55" r:id="rId75" location="" tooltip="" display="https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/"/>
+    <hyperlink ref="T56" r:id="rId76" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
+    <hyperlink ref="U56" r:id="rId77" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
+    <hyperlink ref="V56" r:id="rId78" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="T57" r:id="rId79" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
+    <hyperlink ref="U57" r:id="rId80" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T58" r:id="rId81" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
+    <hyperlink ref="U58" r:id="rId82" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
+    <hyperlink ref="V58" r:id="rId83" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
+    <hyperlink ref="T59" r:id="rId84" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
+    <hyperlink ref="U59" r:id="rId85" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml"/>
+    <hyperlink ref="T60" r:id="rId86" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T61" r:id="rId87" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
+    <hyperlink ref="U61" r:id="rId88" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
+    <hyperlink ref="T62" r:id="rId89" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html"/>
+    <hyperlink ref="T63" r:id="rId90" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="U63" r:id="rId91" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
+    <hyperlink ref="T64" r:id="rId92" location="" tooltip="" display="https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/"/>
+    <hyperlink ref="U64" r:id="rId93" location="" tooltip="" display="https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html"/>
+    <hyperlink ref="T65" r:id="rId94" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
+    <hyperlink ref="T66" r:id="rId95" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
+    <hyperlink ref="U66" r:id="rId96" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
+    <hyperlink ref="T67" r:id="rId97" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
+    <hyperlink ref="T68" r:id="rId98" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T69" r:id="rId99" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
+    <hyperlink ref="T70" r:id="rId100" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
+    <hyperlink ref="T71" r:id="rId101" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U71" r:id="rId102" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
+    <hyperlink ref="T72" r:id="rId103" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
+    <hyperlink ref="T74" r:id="rId104" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
+    <hyperlink ref="U74" r:id="rId105" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
+    <hyperlink ref="V74" r:id="rId106" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
+    <hyperlink ref="T75" r:id="rId107" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U75" r:id="rId108" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
+    <hyperlink ref="T76" r:id="rId109" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
+    <hyperlink ref="T77" r:id="rId110" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
+    <hyperlink ref="T78" r:id="rId111" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T80" r:id="rId112" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="U80" r:id="rId113" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
+    <hyperlink ref="V80" r:id="rId114" location="" tooltip="" display="https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/"/>
+    <hyperlink ref="T81" r:id="rId115" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
+    <hyperlink ref="U81" r:id="rId116" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
entorno reproducible usando renv
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="458">
   <si>
     <t>Caso</t>
   </si>
@@ -2223,6 +2223,49 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t>https://www.chvnoticias.cl/exclusivo-chv/todas-las-pruebas-fiscalia-hector-espinosa-pdi_20220828/</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Luminarias: concejal de Iquique (Felipe Arenas)</t>
+  </si>
+  <si>
+    <t>Felipe Arenas</t>
+  </si>
+  <si>
+    <t>Iquique</t>
+  </si>
+  <si>
+    <t>Concejal</t>
+  </si>
+  <si>
+    <t>Personal</t>
+  </si>
+  <si>
+    <t>Fraude al fisco, cohecho reiterado</t>
+  </si>
+  <si>
+    <t>3 años y un día y 718 días de presidio, con el beneficio de la libertad vigilada intensiva</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.latercera.com/campuslt/noticia/luminarias-juzgado-de-garantia-de-iquique-condena-a-exconcejal-felipe-arenas-por-fraude-al-fisco-y-cohecho/OR3BBHZLARCULI7J5A22A66CSU/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://iquiquetv.cl/2024/07/02/caso-luminarias-led-condenan-a-ex-concejal-felipe-arenas-por-cohecho-y-fraude-al-fisco/</t>
     </r>
   </si>
 </sst>
@@ -3592,7 +3635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X84"/>
+  <dimension ref="A1:X85"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -7731,8 +7774,74 @@
       <c r="W84" s="27"/>
       <c r="X84" s="27"/>
     </row>
+    <row r="85" ht="56.35" customHeight="1">
+      <c r="A85" t="s" s="28">
+        <v>449</v>
+      </c>
+      <c r="B85" s="29">
+        <v>500000000</v>
+      </c>
+      <c r="C85" s="23">
+        <v>2024</v>
+      </c>
+      <c r="D85" t="s" s="25">
+        <v>450</v>
+      </c>
+      <c r="E85" t="s" s="25">
+        <v>26</v>
+      </c>
+      <c r="F85" t="s" s="25">
+        <v>27</v>
+      </c>
+      <c r="G85" s="23">
+        <v>2016</v>
+      </c>
+      <c r="H85" s="23">
+        <v>2018</v>
+      </c>
+      <c r="I85" t="s" s="25">
+        <v>451</v>
+      </c>
+      <c r="J85" t="s" s="25">
+        <v>452</v>
+      </c>
+      <c r="K85" t="s" s="25">
+        <v>453</v>
+      </c>
+      <c r="L85" t="s" s="25">
+        <v>30</v>
+      </c>
+      <c r="M85" t="s" s="25">
+        <v>177</v>
+      </c>
+      <c r="N85" s="27"/>
+      <c r="O85" t="s" s="26">
+        <v>454</v>
+      </c>
+      <c r="P85" t="s" s="26">
+        <v>367</v>
+      </c>
+      <c r="Q85" t="s" s="25">
+        <v>368</v>
+      </c>
+      <c r="R85" t="s" s="16">
+        <v>368</v>
+      </c>
+      <c r="S85" t="s" s="25">
+        <v>455</v>
+      </c>
+      <c r="T85" t="s" s="26">
+        <v>456</v>
+      </c>
+      <c r="U85" t="s" s="26">
+        <v>457</v>
+      </c>
+      <c r="V85" s="27"/>
+      <c r="W85" s="27"/>
+      <c r="X85" s="27"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C11 E1:E11 G1:H10 H11 C12:C14 E12:E14 G12:H13 H14 C15:C32 E15:E32 G15:H31 H32 C33:C40 E33:E40 G33:H39 H40 C41:C51 E41:E51 G41:H50 H51 C52:C54 E52:E54 G52:H53 H54 C55:C60 E55:E60 G55:H59 H60 C61:C62 E61:E62 G61:H61 H62 C63:C66 E63:E66 G63:H65 H66:H67 C67:C70 E67:E70 G68:H69 H70 C71:C73 E71:E73 G71:H72 H73:H74 C74:C80 E74:E80 G75:H79 H80 C81:C84 E81:E84 G81:H84">
+  <conditionalFormatting sqref="C1:C11 E1:E11 G1:H10 H11 C12:C14 E12:E14 G12:H13 H14 C15:C32 E15:E32 G15:H31 H32 C33:C40 E33:E40 G33:H39 H40 C41:C51 E41:E51 G41:H50 H51 C52:C54 E52:E54 G52:H53 H54 C55:C60 E55:E60 G55:H59 H60 C61:C62 E61:E62 G61:H61 H62 C63:C66 E63:E66 G63:H65 H66:H67 C67:C70 E67:E70 G68:H69 H70 C71:C73 E71:E73 G71:H72 H73:H74 C74:C80 E74:E80 G75:H79 H80 C81:C85 E81:E85 G81:H85">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -7867,6 +7976,8 @@
     <hyperlink ref="T83" r:id="rId124" location="" tooltip="" display="https://www.latercera.com/opinion/noticia/columna-de-daniel-matamala-cual-elefante/EOAKP2PXWJHSFDBAKRXGVVS5ZA/"/>
     <hyperlink ref="T84" r:id="rId125" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/formalizan-a-exdirector-general-de-la-pdi-hector-espinosa-fiscalia-le-imputa-apropiacion-de-dineros-de-gastos-reservados-de-la-institucion/IBGS7P3IPVGU3MQU4A7GJDH4UA/"/>
     <hyperlink ref="U84" r:id="rId126" location="" tooltip="" display="https://www.chvnoticias.cl/exclusivo-chv/todas-las-pruebas-fiscalia-hector-espinosa-pdi_20220828/"/>
+    <hyperlink ref="T85" r:id="rId127" location="" tooltip="" display="https://www.latercera.com/campuslt/noticia/luminarias-juzgado-de-garantia-de-iquique-condena-a-exconcejal-felipe-arenas-por-fraude-al-fisco-y-cohecho/OR3BBHZLARCULI7J5A22A66CSU/"/>
+    <hyperlink ref="U85" r:id="rId128" location="" tooltip="" display="https://iquiquetv.cl/2024/07/02/caso-luminarias-led-condenan-a-ex-concejal-felipe-arenas-por-cohecho-y-fraude-al-fisco/"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
actualizacion de casos y renv
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="478">
   <si>
     <t>Caso</t>
   </si>
@@ -194,6 +194,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://lavozdemaipu.cl/cathy-barriga-ultimo-informe-con-peras-y-manzanas/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.tvn.cl/programas/buenos-dias-a-todos/actualidad/caso-cathy-barriga-los-41-mil-millones-de-pesos-que-no-se-saben-donde</t>
+    </r>
+  </si>
+  <si>
     <t>Caso Penta</t>
   </si>
   <si>
@@ -792,7 +814,7 @@
     </r>
   </si>
   <si>
-    <t>Gobernador regional Araucanía (Luciano Rivas)</t>
+    <t>Caso Convenios: gobernador regional Araucanía (Luciano Rivas)</t>
   </si>
   <si>
     <t>Luciano Rivas</t>
@@ -821,6 +843,17 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t>https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.cnnchile.com/pais/caso-convenios-fundacion-la-araucania-sueldo_20240901/</t>
     </r>
   </si>
   <si>
@@ -1533,7 +1566,7 @@
     <t>Camila Polizzi, Diego Polanco</t>
   </si>
   <si>
-    <t>Fundación En tí</t>
+    <t>Fundación En ti</t>
   </si>
   <si>
     <t>estafa, falsificación de documento oficial, usurpación de identidad, lavado de activos</t>
@@ -3910,7 +3943,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="14">
-        <v>31000000000</v>
+        <v>41000000000</v>
       </c>
       <c r="C4" s="15">
         <v>2024</v>
@@ -3950,14 +3983,18 @@
       <c r="T4" t="s" s="20">
         <v>46</v>
       </c>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
+      <c r="U4" t="s" s="20">
+        <v>47</v>
+      </c>
+      <c r="V4" t="s" s="20">
+        <v>48</v>
+      </c>
       <c r="W4" s="19"/>
       <c r="X4" s="19"/>
     </row>
     <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="13">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="14">
         <v>30100000000</v>
@@ -3966,7 +4003,7 @@
         <v>2014</v>
       </c>
       <c r="D5" t="s" s="16">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s" s="16">
         <v>26</v>
@@ -3980,16 +4017,16 @@
       <c r="H5" s="17"/>
       <c r="I5" s="18"/>
       <c r="J5" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="19"/>
       <c r="O5" t="s" s="20">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P5" s="19"/>
       <c r="Q5" s="17"/>
@@ -4003,7 +4040,7 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="13">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6" s="14">
         <v>26800000000</v>
@@ -4020,7 +4057,7 @@
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
       <c r="J6" t="s" s="16">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
@@ -4039,7 +4076,7 @@
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="13">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B7" s="14">
         <v>19840000000</v>
@@ -4048,35 +4085,35 @@
         <v>2006</v>
       </c>
       <c r="D7" t="s" s="16">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F7" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" t="s" s="16">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="19"/>
       <c r="O7" t="s" s="20">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
       <c r="S7" t="s" s="16">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T7" t="s" s="20">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
@@ -4085,7 +4122,7 @@
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="13">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B8" s="14">
         <v>18400000000</v>
@@ -4094,7 +4131,7 @@
         <v>1989</v>
       </c>
       <c r="D8" t="s" s="16">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s" s="16">
         <v>26</v>
@@ -4109,16 +4146,16 @@
       <c r="M8" s="17"/>
       <c r="N8" s="19"/>
       <c r="O8" t="s" s="20">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="P8" s="19"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="17"/>
       <c r="S8" t="s" s="16">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="T8" t="s" s="20">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
@@ -4127,7 +4164,7 @@
     </row>
     <row r="9" ht="32.05" customHeight="1">
       <c r="A9" t="s" s="13">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B9" s="14">
         <v>12000000000</v>
@@ -4148,23 +4185,23 @@
       </c>
       <c r="I9" s="18"/>
       <c r="J9" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
       <c r="M9" t="s" s="16">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="N9" s="19"/>
       <c r="O9" t="s" s="20">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P9" s="19"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
       <c r="S9" s="17"/>
       <c r="T9" t="s" s="20">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="U9" s="19"/>
       <c r="V9" s="19"/>
@@ -4173,7 +4210,7 @@
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="13">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B10" s="14">
         <v>11000000000</v>
@@ -4182,13 +4219,13 @@
         <v>2018</v>
       </c>
       <c r="D10" t="s" s="16">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F10" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -4199,14 +4236,14 @@
       <c r="M10" s="17"/>
       <c r="N10" s="19"/>
       <c r="O10" t="s" s="20">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P10" s="19"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
       <c r="S10" s="17"/>
       <c r="T10" t="s" s="20">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
@@ -4215,7 +4252,7 @@
     </row>
     <row r="11" ht="32.05" customHeight="1">
       <c r="A11" t="s" s="13">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B11" s="14">
         <v>10210000000</v>
@@ -4224,13 +4261,13 @@
         <v>2021</v>
       </c>
       <c r="D11" t="s" s="16">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s" s="16">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F11" t="s" s="16">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G11" s="15">
         <v>2017</v>
@@ -4239,7 +4276,7 @@
         <v>2020</v>
       </c>
       <c r="I11" t="s" s="16">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J11" t="s" s="16">
         <v>29</v>
@@ -4251,16 +4288,16 @@
       <c r="M11" s="17"/>
       <c r="N11" s="19"/>
       <c r="O11" t="s" s="20">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="P11" t="s" s="20">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
       <c r="S11" s="17"/>
       <c r="T11" t="s" s="20">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
@@ -4269,7 +4306,7 @@
     </row>
     <row r="12" ht="32.05" customHeight="1">
       <c r="A12" t="s" s="13">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B12" s="14">
         <v>9000000000</v>
@@ -4278,7 +4315,7 @@
         <v>2017</v>
       </c>
       <c r="D12" t="s" s="16">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s" s="16">
         <v>26</v>
@@ -4289,7 +4326,7 @@
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" t="s" s="16">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J12" t="s" s="16">
         <v>29</v>
@@ -4301,14 +4338,14 @@
       <c r="M12" s="17"/>
       <c r="N12" s="19"/>
       <c r="O12" t="s" s="20">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="P12" s="19"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
       <c r="S12" s="17"/>
       <c r="T12" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
@@ -4317,7 +4354,7 @@
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="13">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B13" s="14">
         <v>8713407156</v>
@@ -4336,19 +4373,19 @@
       <c r="J13" s="17"/>
       <c r="K13" s="17"/>
       <c r="L13" t="s" s="16">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="19"/>
       <c r="O13" t="s" s="20">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
       <c r="S13" s="17"/>
       <c r="T13" t="s" s="20">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
@@ -4357,7 +4394,7 @@
     </row>
     <row r="14" ht="32.05" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B14" s="14">
         <v>8000000000</v>
@@ -4366,7 +4403,7 @@
         <v>2024</v>
       </c>
       <c r="D14" t="s" s="16">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E14" t="s" s="16">
         <v>26</v>
@@ -4377,7 +4414,7 @@
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" t="s" s="16">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J14" t="s" s="16">
         <v>29</v>
@@ -4387,17 +4424,17 @@
       <c r="M14" s="17"/>
       <c r="N14" s="19"/>
       <c r="O14" t="s" s="20">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
       <c r="S14" s="19"/>
       <c r="T14" t="s" s="20">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="U14" t="s" s="20">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
@@ -4405,7 +4442,7 @@
     </row>
     <row r="15" ht="44.05" customHeight="1">
       <c r="A15" t="s" s="13">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B15" s="14">
         <v>14300000000</v>
@@ -4414,7 +4451,7 @@
         <v>2019</v>
       </c>
       <c r="D15" t="s" s="16">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s" s="16">
         <v>37</v>
@@ -4430,22 +4467,22 @@
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" t="s" s="16">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="19"/>
       <c r="O15" t="s" s="20">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="P15" s="19"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
       <c r="T15" t="s" s="20">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="U15" t="s" s="20">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="V15" s="19"/>
       <c r="W15" s="19"/>
@@ -4453,7 +4490,7 @@
     </row>
     <row r="16" ht="32.05" customHeight="1">
       <c r="A16" t="s" s="13">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B16" s="14">
         <v>6000000000</v>
@@ -4462,13 +4499,13 @@
         <v>2018</v>
       </c>
       <c r="D16" t="s" s="16">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E16" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F16" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G16" s="15">
         <v>2008</v>
@@ -4477,7 +4514,7 @@
         <v>2021</v>
       </c>
       <c r="I16" t="s" s="16">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J16" t="s" s="16">
         <v>29</v>
@@ -4489,14 +4526,14 @@
       <c r="M16" s="17"/>
       <c r="N16" s="19"/>
       <c r="O16" t="s" s="20">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P16" s="19"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
       <c r="S16" s="17"/>
       <c r="T16" t="s" s="20">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="U16" s="17"/>
       <c r="V16" s="19"/>
@@ -4505,7 +4542,7 @@
     </row>
     <row r="17" ht="44.05" customHeight="1">
       <c r="A17" t="s" s="13">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B17" s="14">
         <v>4670000000</v>
@@ -4514,7 +4551,7 @@
         <v>2012</v>
       </c>
       <c r="D17" t="s" s="16">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E17" t="s" s="16">
         <v>26</v>
@@ -4530,36 +4567,36 @@
       </c>
       <c r="I17" s="17"/>
       <c r="J17" t="s" s="16">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="19"/>
       <c r="O17" t="s" s="20">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P17" s="19"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
       <c r="S17" t="s" s="16">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="T17" t="s" s="20">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="U17" t="s" s="20">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="V17" t="s" s="20">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="13">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B18" s="14">
         <v>4600000000</v>
@@ -4568,7 +4605,7 @@
         <v>2017</v>
       </c>
       <c r="D18" t="s" s="16">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E18" t="s" s="16">
         <v>26</v>
@@ -4583,7 +4620,7 @@
         <v>2020</v>
       </c>
       <c r="I18" t="s" s="16">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J18" t="s" s="16">
         <v>29</v>
@@ -4595,17 +4632,17 @@
       <c r="M18" s="17"/>
       <c r="N18" s="19"/>
       <c r="O18" t="s" s="20">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="P18" s="19"/>
       <c r="Q18" s="17"/>
       <c r="R18" s="17"/>
       <c r="S18" s="17"/>
       <c r="T18" t="s" s="20">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="U18" t="s" s="20">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="V18" s="19"/>
       <c r="W18" s="19"/>
@@ -4613,7 +4650,7 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B19" s="14">
         <v>4500000000</v>
@@ -4622,18 +4659,18 @@
         <v>2023</v>
       </c>
       <c r="D19" t="s" s="16">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F19" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
       <c r="I19" t="s" s="16">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J19" t="s" s="16">
         <v>29</v>
@@ -4645,7 +4682,7 @@
       <c r="M19" s="17"/>
       <c r="N19" s="19"/>
       <c r="O19" t="s" s="20">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="P19" s="19"/>
       <c r="Q19" s="17"/>
@@ -4654,22 +4691,22 @@
         <v>45</v>
       </c>
       <c r="T19" t="s" s="20">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="U19" t="s" s="20">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="V19" t="s" s="20">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="W19" t="s" s="20">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="X19" s="19"/>
     </row>
     <row r="20" ht="32.05" customHeight="1">
       <c r="A20" t="s" s="13">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B20" s="14">
         <v>4300000000</v>
@@ -4678,7 +4715,7 @@
         <v>2020</v>
       </c>
       <c r="D20" t="s" s="16">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s" s="16">
         <v>26</v>
@@ -4693,7 +4730,7 @@
         <v>2020</v>
       </c>
       <c r="I20" t="s" s="16">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J20" t="s" s="16">
         <v>29</v>
@@ -4703,14 +4740,14 @@
       <c r="M20" s="17"/>
       <c r="N20" s="19"/>
       <c r="O20" t="s" s="20">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="P20" s="19"/>
       <c r="Q20" s="17"/>
       <c r="R20" s="17"/>
       <c r="S20" s="17"/>
       <c r="T20" t="s" s="20">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
@@ -4719,7 +4756,7 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="13">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B21" s="14">
         <v>4000000000</v>
@@ -4728,13 +4765,13 @@
         <v>2024</v>
       </c>
       <c r="D21" t="s" s="16">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s" s="16">
         <v>37</v>
       </c>
       <c r="F21" t="s" s="16">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G21" s="15">
         <v>2012</v>
@@ -4743,7 +4780,7 @@
         <v>2021</v>
       </c>
       <c r="I21" t="s" s="16">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J21" t="s" s="16">
         <v>29</v>
@@ -4753,14 +4790,14 @@
       <c r="M21" s="17"/>
       <c r="N21" s="19"/>
       <c r="O21" t="s" s="20">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="P21" s="19"/>
       <c r="Q21" s="17"/>
       <c r="R21" s="17"/>
       <c r="S21" s="17"/>
       <c r="T21" t="s" s="20">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="U21" s="19"/>
       <c r="V21" s="19"/>
@@ -4769,7 +4806,7 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="13">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B22" s="14">
         <v>3000000000</v>
@@ -4786,26 +4823,26 @@
       <c r="H22" s="17"/>
       <c r="I22" s="18"/>
       <c r="J22" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K22" s="17"/>
       <c r="L22" t="s" s="16">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="19"/>
       <c r="O22" t="s" s="20">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="P22" s="19"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
       <c r="S22" s="17"/>
       <c r="T22" t="s" s="20">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U22" t="s" s="20">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
@@ -4813,7 +4850,7 @@
     </row>
     <row r="23" ht="20.35" customHeight="1">
       <c r="A23" t="s" s="21">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B23" s="22">
         <v>2500000000</v>
@@ -4829,7 +4866,7 @@
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
       <c r="I23" t="s" s="25">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J23" t="s" s="25">
         <v>13</v>
@@ -4838,7 +4875,7 @@
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
       <c r="N23" t="s" s="26">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
@@ -4846,10 +4883,10 @@
       <c r="R23" s="24"/>
       <c r="S23" s="24"/>
       <c r="T23" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="U23" t="s" s="26">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="V23" s="27"/>
       <c r="W23" s="27"/>
@@ -4857,7 +4894,7 @@
     </row>
     <row r="24" ht="20.35" customHeight="1">
       <c r="A24" t="s" s="21">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B24" s="22">
         <v>1100000000</v>
@@ -4866,13 +4903,13 @@
         <v>2023</v>
       </c>
       <c r="D24" t="s" s="25">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E24" t="s" s="25">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s" s="25">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="G24" s="23">
         <v>2023</v>
@@ -4881,7 +4918,7 @@
         <v>2024</v>
       </c>
       <c r="I24" t="s" s="25">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J24" t="s" s="25">
         <v>29</v>
@@ -4892,13 +4929,13 @@
       <c r="N24" s="27"/>
       <c r="O24" s="27"/>
       <c r="P24" t="s" s="26">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
       <c r="S24" s="24"/>
       <c r="T24" t="s" s="26">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="U24" s="27"/>
       <c r="V24" s="27"/>
@@ -4907,7 +4944,7 @@
     </row>
     <row r="25" ht="32.05" customHeight="1">
       <c r="A25" t="s" s="13">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B25" s="14">
         <v>2492000000</v>
@@ -4916,13 +4953,13 @@
         <v>2022</v>
       </c>
       <c r="D25" t="s" s="16">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E25" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F25" t="s" s="16">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G25" s="15">
         <v>2020</v>
@@ -4931,7 +4968,7 @@
         <v>2021</v>
       </c>
       <c r="I25" t="s" s="16">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J25" t="s" s="16">
         <v>29</v>
@@ -4941,29 +4978,29 @@
       <c r="M25" s="17"/>
       <c r="N25" s="19"/>
       <c r="O25" t="s" s="20">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="P25" s="19"/>
       <c r="Q25" s="17"/>
       <c r="R25" s="17"/>
       <c r="S25" s="17"/>
       <c r="T25" t="s" s="20">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="U25" t="s" s="20">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="V25" t="s" s="20">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="W25" t="s" s="20">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="X25" s="19"/>
     </row>
     <row r="26" ht="32.35" customHeight="1">
       <c r="A26" t="s" s="21">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B26" s="22">
         <v>2113000000</v>
@@ -4972,18 +5009,18 @@
         <v>2023</v>
       </c>
       <c r="D26" t="s" s="25">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E26" t="s" s="25">
         <v>26</v>
       </c>
       <c r="F26" t="s" s="25">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
       <c r="I26" t="s" s="25">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J26" t="s" s="25">
         <v>13</v>
@@ -4992,28 +5029,30 @@
       <c r="L26" s="24"/>
       <c r="M26" s="24"/>
       <c r="N26" t="s" s="26">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="O26" t="s" s="26">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="P26" s="27"/>
       <c r="Q26" s="24"/>
       <c r="R26" s="24"/>
       <c r="S26" s="24"/>
       <c r="T26" t="s" s="26">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="U26" t="s" s="26">
-        <v>168</v>
-      </c>
-      <c r="V26" s="27"/>
+        <v>170</v>
+      </c>
+      <c r="V26" t="s" s="26">
+        <v>171</v>
+      </c>
       <c r="W26" s="27"/>
       <c r="X26" s="27"/>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="13">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B27" s="14">
         <v>2000000000</v>
@@ -5022,13 +5061,13 @@
         <v>2023</v>
       </c>
       <c r="D27" t="s" s="16">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E27" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F27" t="s" s="16">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G27" s="15">
         <v>2018</v>
@@ -5037,7 +5076,7 @@
         <v>2019</v>
       </c>
       <c r="I27" t="s" s="16">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="J27" t="s" s="16">
         <v>29</v>
@@ -5047,17 +5086,17 @@
       <c r="M27" s="17"/>
       <c r="N27" s="19"/>
       <c r="O27" t="s" s="20">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="P27" s="19"/>
       <c r="Q27" s="17"/>
       <c r="R27" s="17"/>
       <c r="S27" s="17"/>
       <c r="T27" t="s" s="20">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="U27" t="s" s="20">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="V27" s="19"/>
       <c r="W27" s="19"/>
@@ -5065,7 +5104,7 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="13">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B28" s="14">
         <v>1700000000</v>
@@ -5084,25 +5123,25 @@
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K28" t="s" s="16">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" t="s" s="16">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N28" s="19"/>
       <c r="O28" t="s" s="20">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="P28" s="19"/>
       <c r="Q28" s="17"/>
       <c r="R28" s="17"/>
       <c r="S28" s="17"/>
       <c r="T28" t="s" s="20">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="U28" s="19"/>
       <c r="V28" s="19"/>
@@ -5111,7 +5150,7 @@
     </row>
     <row r="29" ht="32.05" customHeight="1">
       <c r="A29" t="s" s="13">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B29" s="14">
         <v>1673754000</v>
@@ -5120,7 +5159,7 @@
         <v>2019</v>
       </c>
       <c r="D29" t="s" s="16">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E29" t="s" s="16">
         <v>26</v>
@@ -5131,7 +5170,7 @@
       <c r="G29" s="17"/>
       <c r="H29" s="17"/>
       <c r="I29" t="s" s="16">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="J29" t="s" s="16">
         <v>29</v>
@@ -5141,17 +5180,17 @@
       <c r="M29" s="17"/>
       <c r="N29" s="19"/>
       <c r="O29" t="s" s="20">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="P29" s="19"/>
       <c r="Q29" s="17"/>
       <c r="R29" s="17"/>
       <c r="S29" s="17"/>
       <c r="T29" t="s" s="20">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="U29" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V29" s="19"/>
       <c r="W29" s="19"/>
@@ -5159,7 +5198,7 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="13">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B30" s="14">
         <v>1659000000</v>
@@ -5168,7 +5207,7 @@
         <v>2017</v>
       </c>
       <c r="D30" t="s" s="16">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E30" t="s" s="16">
         <v>37</v>
@@ -5180,27 +5219,27 @@
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K30" t="s" s="16">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="L30" t="s" s="16">
         <v>30</v>
       </c>
       <c r="M30" t="s" s="16">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N30" s="19"/>
       <c r="O30" t="s" s="20">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="P30" s="19"/>
       <c r="Q30" s="17"/>
       <c r="R30" s="17"/>
       <c r="S30" s="17"/>
       <c r="T30" t="s" s="20">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="U30" s="19"/>
       <c r="V30" s="19"/>
@@ -5209,7 +5248,7 @@
     </row>
     <row r="31" ht="32.35" customHeight="1">
       <c r="A31" t="s" s="28">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B31" s="29">
         <v>1600000000</v>
@@ -5225,7 +5264,7 @@
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
       <c r="I31" t="s" s="25">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J31" t="s" s="25">
         <v>13</v>
@@ -5234,7 +5273,7 @@
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" t="s" s="30">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="O31" s="27"/>
       <c r="P31" s="27"/>
@@ -5242,7 +5281,7 @@
       <c r="R31" s="24"/>
       <c r="S31" s="24"/>
       <c r="T31" t="s" s="26">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="U31" s="27"/>
       <c r="V31" s="27"/>
@@ -5251,7 +5290,7 @@
     </row>
     <row r="32" ht="44.05" customHeight="1">
       <c r="A32" t="s" s="13">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B32" s="14">
         <v>1600000000</v>
@@ -5260,13 +5299,13 @@
         <v>2020</v>
       </c>
       <c r="D32" t="s" s="16">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="E32" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F32" t="s" s="16">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G32" s="15">
         <v>2020</v>
@@ -5275,10 +5314,10 @@
         <v>2022</v>
       </c>
       <c r="I32" t="s" s="16">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J32" t="s" s="16">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K32" s="17"/>
       <c r="L32" t="s" s="16">
@@ -5287,18 +5326,18 @@
       <c r="M32" s="17"/>
       <c r="N32" s="19"/>
       <c r="O32" t="s" s="20">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="P32" t="s" s="20">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="Q32" s="17"/>
       <c r="R32" s="17"/>
       <c r="S32" t="s" s="16">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="T32" t="s" s="20">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="U32" s="19"/>
       <c r="V32" s="19"/>
@@ -5307,7 +5346,7 @@
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" t="s" s="13">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B33" s="14">
         <v>1253000000</v>
@@ -5317,10 +5356,10 @@
       </c>
       <c r="D33" s="17"/>
       <c r="E33" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F33" t="s" s="16">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G33" s="15">
         <v>1997</v>
@@ -5340,10 +5379,10 @@
       <c r="R33" s="17"/>
       <c r="S33" s="17"/>
       <c r="T33" t="s" s="20">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U33" t="s" s="20">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="V33" s="19"/>
       <c r="W33" s="19"/>
@@ -5351,7 +5390,7 @@
     </row>
     <row r="34" ht="32.35" customHeight="1">
       <c r="A34" t="s" s="28">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B34" s="29">
         <v>1200000000</v>
@@ -5365,7 +5404,7 @@
       <c r="G34" s="24"/>
       <c r="H34" s="24"/>
       <c r="I34" t="s" s="25">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J34" t="s" s="25">
         <v>13</v>
@@ -5374,7 +5413,7 @@
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" t="s" s="30">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="O34" s="27"/>
       <c r="P34" s="27"/>
@@ -5382,7 +5421,7 @@
       <c r="R34" s="24"/>
       <c r="S34" s="24"/>
       <c r="T34" t="s" s="26">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="U34" s="27"/>
       <c r="V34" s="27"/>
@@ -5391,7 +5430,7 @@
     </row>
     <row r="35" ht="20.35" customHeight="1">
       <c r="A35" t="s" s="28">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B35" s="29">
         <v>1200000000</v>
@@ -5407,7 +5446,7 @@
       <c r="G35" s="24"/>
       <c r="H35" s="24"/>
       <c r="I35" t="s" s="25">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="J35" t="s" s="25">
         <v>13</v>
@@ -5416,7 +5455,7 @@
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" t="s" s="26">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="O35" s="27"/>
       <c r="P35" s="27"/>
@@ -5424,10 +5463,10 @@
       <c r="R35" s="24"/>
       <c r="S35" s="24"/>
       <c r="T35" t="s" s="26">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="U35" t="s" s="26">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="V35" s="27"/>
       <c r="W35" s="27"/>
@@ -5435,7 +5474,7 @@
     </row>
     <row r="36" ht="32.05" customHeight="1">
       <c r="A36" t="s" s="13">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B36" s="14">
         <v>1100000000</v>
@@ -5444,7 +5483,7 @@
         <v>2022</v>
       </c>
       <c r="D36" t="s" s="16">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E36" t="s" s="16">
         <v>26</v>
@@ -5459,7 +5498,7 @@
         <v>2023</v>
       </c>
       <c r="I36" t="s" s="16">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J36" t="s" s="16">
         <v>29</v>
@@ -5471,14 +5510,14 @@
       <c r="M36" s="17"/>
       <c r="N36" s="19"/>
       <c r="O36" t="s" s="20">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="P36" s="19"/>
       <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
       <c r="S36" s="17"/>
       <c r="T36" t="s" s="20">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="U36" s="19"/>
       <c r="V36" s="19"/>
@@ -5487,7 +5526,7 @@
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="13">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B37" s="14">
         <v>1000000000</v>
@@ -5496,7 +5535,7 @@
         <v>2023</v>
       </c>
       <c r="D37" t="s" s="16">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="E37" t="s" s="16">
         <v>26</v>
@@ -5507,7 +5546,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="17"/>
       <c r="I37" t="s" s="16">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="J37" t="s" s="16">
         <v>29</v>
@@ -5519,14 +5558,14 @@
       <c r="M37" s="17"/>
       <c r="N37" s="19"/>
       <c r="O37" t="s" s="20">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="P37" s="19"/>
       <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
       <c r="S37" s="17"/>
       <c r="T37" t="s" s="20">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="U37" s="19"/>
       <c r="V37" s="19"/>
@@ -5535,7 +5574,7 @@
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="13">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B38" s="14">
         <v>946000000</v>
@@ -5545,10 +5584,10 @@
       </c>
       <c r="D38" s="17"/>
       <c r="E38" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F38" t="s" s="16">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G38" s="17"/>
       <c r="H38" s="17"/>
@@ -5564,7 +5603,7 @@
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" t="s" s="20">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U38" s="19"/>
       <c r="V38" s="19"/>
@@ -5573,7 +5612,7 @@
     </row>
     <row r="39" ht="44.05" customHeight="1">
       <c r="A39" t="s" s="13">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B39" s="14">
         <v>847807917</v>
@@ -5582,7 +5621,7 @@
         <v>2024</v>
       </c>
       <c r="D39" t="s" s="16">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
@@ -5600,7 +5639,7 @@
       <c r="R39" s="17"/>
       <c r="S39" s="17"/>
       <c r="T39" t="s" s="20">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="U39" s="19"/>
       <c r="V39" s="19"/>
@@ -5609,7 +5648,7 @@
     </row>
     <row r="40" ht="32.05" customHeight="1">
       <c r="A40" t="s" s="13">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="B40" s="14">
         <v>750000000</v>
@@ -5618,7 +5657,7 @@
         <v>2023</v>
       </c>
       <c r="D40" t="s" s="16">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="E40" t="s" s="16">
         <v>26</v>
@@ -5633,7 +5672,7 @@
         <v>2015</v>
       </c>
       <c r="I40" t="s" s="16">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="J40" t="s" s="16">
         <v>29</v>
@@ -5643,18 +5682,18 @@
       <c r="M40" s="17"/>
       <c r="N40" s="19"/>
       <c r="O40" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P40" t="s" s="20">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="Q40" s="17"/>
       <c r="R40" s="17"/>
       <c r="S40" t="s" s="20">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="T40" t="s" s="20">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="U40" s="19"/>
       <c r="V40" s="19"/>
@@ -5663,7 +5702,7 @@
     </row>
     <row r="41" ht="32.05" customHeight="1">
       <c r="A41" t="s" s="13">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B41" s="14">
         <v>680000000</v>
@@ -5672,18 +5711,18 @@
         <v>2018</v>
       </c>
       <c r="D41" t="s" s="16">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E41" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F41" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
       <c r="I41" t="s" s="16">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="J41" t="s" s="16">
         <v>29</v>
@@ -5695,27 +5734,27 @@
       <c r="M41" s="17"/>
       <c r="N41" s="19"/>
       <c r="O41" t="s" s="20">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="P41" s="19"/>
       <c r="Q41" s="17"/>
       <c r="R41" s="17"/>
       <c r="S41" s="17"/>
       <c r="T41" t="s" s="20">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="U41" t="s" s="20">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="V41" t="s" s="20">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="W41" s="19"/>
       <c r="X41" s="19"/>
     </row>
     <row r="42" ht="32.35" customHeight="1">
       <c r="A42" t="s" s="21">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="B42" s="22">
         <v>658000000</v>
@@ -5724,18 +5763,18 @@
         <v>2023</v>
       </c>
       <c r="D42" t="s" s="25">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="E42" t="s" s="25">
         <v>26</v>
       </c>
       <c r="F42" t="s" s="25">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="G42" s="24"/>
       <c r="H42" s="24"/>
       <c r="I42" t="s" s="25">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J42" t="s" s="25">
         <v>13</v>
@@ -5744,30 +5783,30 @@
       <c r="L42" s="24"/>
       <c r="M42" s="24"/>
       <c r="N42" t="s" s="26">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="O42" t="s" s="26">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="P42" s="27"/>
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
       <c r="S42" s="24"/>
       <c r="T42" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="U42" t="s" s="26">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="V42" t="s" s="26">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="W42" s="27"/>
       <c r="X42" s="27"/>
     </row>
     <row r="43" ht="20.35" customHeight="1">
       <c r="A43" t="s" s="28">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="B43" s="22">
         <v>577000000</v>
@@ -5783,7 +5822,7 @@
       <c r="G43" s="24"/>
       <c r="H43" s="24"/>
       <c r="I43" t="s" s="25">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="J43" t="s" s="25">
         <v>13</v>
@@ -5792,22 +5831,22 @@
       <c r="L43" s="24"/>
       <c r="M43" s="24"/>
       <c r="N43" t="s" s="26">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="O43" t="s" s="26">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P43" t="s" s="26">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
       <c r="S43" s="24"/>
       <c r="T43" t="s" s="26">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="U43" t="s" s="26">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="V43" s="27"/>
       <c r="W43" s="27"/>
@@ -5815,7 +5854,7 @@
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="13">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B44" s="14">
         <v>497000000</v>
@@ -5824,18 +5863,18 @@
         <v>2020</v>
       </c>
       <c r="D44" t="s" s="16">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E44" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F44" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" t="s" s="16">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="J44" t="s" s="16">
         <v>29</v>
@@ -5845,17 +5884,17 @@
       <c r="M44" s="17"/>
       <c r="N44" s="19"/>
       <c r="O44" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P44" s="19"/>
       <c r="Q44" s="17"/>
       <c r="R44" s="17"/>
       <c r="S44" s="17"/>
       <c r="T44" t="s" s="20">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="U44" t="s" s="20">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="V44" s="19"/>
       <c r="W44" s="19"/>
@@ -5863,7 +5902,7 @@
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="13">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B45" s="14">
         <v>465000000</v>
@@ -5872,13 +5911,13 @@
         <v>2019</v>
       </c>
       <c r="D45" t="s" s="16">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E45" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F45" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G45" s="17"/>
       <c r="H45" s="17"/>
@@ -5889,14 +5928,14 @@
       <c r="M45" s="17"/>
       <c r="N45" s="19"/>
       <c r="O45" t="s" s="20">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="P45" s="19"/>
       <c r="Q45" s="17"/>
       <c r="R45" s="17"/>
       <c r="S45" s="17"/>
       <c r="T45" t="s" s="20">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="U45" s="19"/>
       <c r="V45" s="19"/>
@@ -5905,7 +5944,7 @@
     </row>
     <row r="46" ht="32.35" customHeight="1">
       <c r="A46" t="s" s="21">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B46" s="22">
         <v>426000000</v>
@@ -5914,18 +5953,18 @@
         <v>2023</v>
       </c>
       <c r="D46" t="s" s="25">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E46" t="s" s="25">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F46" t="s" s="25">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G46" s="24"/>
       <c r="H46" s="24"/>
       <c r="I46" t="s" s="25">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="J46" t="s" s="25">
         <v>13</v>
@@ -5934,17 +5973,17 @@
       <c r="L46" s="24"/>
       <c r="M46" s="24"/>
       <c r="N46" t="s" s="26">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="O46" t="s" s="26">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P46" s="27"/>
       <c r="Q46" s="24"/>
       <c r="R46" s="24"/>
       <c r="S46" s="24"/>
       <c r="T46" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="U46" s="27"/>
       <c r="V46" s="27"/>
@@ -5953,7 +5992,7 @@
     </row>
     <row r="47" ht="44.35" customHeight="1">
       <c r="A47" t="s" s="28">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B47" s="29">
         <v>421000000</v>
@@ -5962,18 +6001,18 @@
         <v>2023</v>
       </c>
       <c r="D47" t="s" s="25">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="E47" t="s" s="25">
         <v>26</v>
       </c>
       <c r="F47" t="s" s="25">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
       <c r="I47" t="s" s="25">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J47" t="s" s="25">
         <v>13</v>
@@ -5982,30 +6021,30 @@
       <c r="L47" s="24"/>
       <c r="M47" s="24"/>
       <c r="N47" t="s" s="26">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="O47" t="s" s="26">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="P47" s="27"/>
       <c r="Q47" s="24"/>
       <c r="R47" s="24"/>
       <c r="S47" s="24"/>
       <c r="T47" t="s" s="26">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="U47" t="s" s="26">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="V47" t="s" s="26">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="W47" s="27"/>
       <c r="X47" s="27"/>
     </row>
     <row r="48" ht="44.05" customHeight="1">
       <c r="A48" t="s" s="13">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="B48" s="14">
         <v>400000000</v>
@@ -6014,33 +6053,33 @@
         <v>2023</v>
       </c>
       <c r="D48" t="s" s="16">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="E48" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F48" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G48" s="17"/>
       <c r="H48" s="17"/>
       <c r="I48" s="24"/>
       <c r="J48" t="s" s="16">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
       <c r="M48" s="17"/>
       <c r="N48" s="19"/>
       <c r="O48" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P48" s="19"/>
       <c r="Q48" s="17"/>
       <c r="R48" s="17"/>
       <c r="S48" s="17"/>
       <c r="T48" t="s" s="16">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="U48" s="19"/>
       <c r="V48" s="19"/>
@@ -6049,7 +6088,7 @@
     </row>
     <row r="49" ht="20.35" customHeight="1">
       <c r="A49" t="s" s="28">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B49" s="29">
         <v>356000000</v>
@@ -6062,12 +6101,12 @@
         <v>26</v>
       </c>
       <c r="F49" t="s" s="25">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
       <c r="I49" t="s" s="25">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="J49" t="s" s="25">
         <v>13</v>
@@ -6076,30 +6115,30 @@
       <c r="L49" s="24"/>
       <c r="M49" s="24"/>
       <c r="N49" t="s" s="26">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="O49" t="s" s="26">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="P49" s="27"/>
       <c r="Q49" s="24"/>
       <c r="R49" s="24"/>
       <c r="S49" s="24"/>
       <c r="T49" t="s" s="26">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="U49" t="s" s="26">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="V49" t="s" s="26">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="W49" s="27"/>
       <c r="X49" s="27"/>
     </row>
     <row r="50" ht="32.05" customHeight="1">
       <c r="A50" t="s" s="13">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="B50" s="14">
         <v>351000000</v>
@@ -6108,13 +6147,13 @@
         <v>2021</v>
       </c>
       <c r="D50" t="s" s="16">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E50" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F50" t="s" s="16">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G50" s="15">
         <v>2013</v>
@@ -6123,7 +6162,7 @@
         <v>2016</v>
       </c>
       <c r="I50" t="s" s="16">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="J50" t="s" s="16">
         <v>29</v>
@@ -6133,7 +6172,7 @@
       <c r="M50" s="17"/>
       <c r="N50" s="19"/>
       <c r="O50" t="s" s="20">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="P50" t="s" s="20">
         <v>16</v>
@@ -6141,13 +6180,13 @@
       <c r="Q50" s="17"/>
       <c r="R50" s="17"/>
       <c r="S50" t="s" s="16">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="T50" t="s" s="16">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="U50" t="s" s="20">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="V50" s="19"/>
       <c r="W50" s="19"/>
@@ -6155,7 +6194,7 @@
     </row>
     <row r="51" ht="32.05" customHeight="1">
       <c r="A51" t="s" s="13">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B51" s="14">
         <v>293093681</v>
@@ -6164,13 +6203,13 @@
         <v>2023</v>
       </c>
       <c r="D51" t="s" s="16">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E51" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F51" t="s" s="16">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
@@ -6181,14 +6220,14 @@
       <c r="M51" s="17"/>
       <c r="N51" s="19"/>
       <c r="O51" t="s" s="20">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="P51" s="19"/>
       <c r="Q51" s="17"/>
       <c r="R51" s="17"/>
       <c r="S51" s="19"/>
       <c r="T51" t="s" s="20">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="U51" s="19"/>
       <c r="V51" s="19"/>
@@ -6197,7 +6236,7 @@
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="13">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="B52" s="14">
         <v>290000000</v>
@@ -6206,7 +6245,7 @@
         <v>2006</v>
       </c>
       <c r="D52" t="s" s="16">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="E52" t="s" s="16">
         <v>37</v>
@@ -6216,21 +6255,21 @@
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
       <c r="J52" t="s" s="16">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
       <c r="M52" s="17"/>
       <c r="N52" s="19"/>
       <c r="O52" t="s" s="20">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="P52" s="19"/>
       <c r="Q52" s="17"/>
       <c r="R52" s="17"/>
       <c r="S52" s="17"/>
       <c r="T52" t="s" s="20">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="U52" s="19"/>
       <c r="V52" s="19"/>
@@ -6239,7 +6278,7 @@
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="13">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="B53" s="14">
         <v>289350646</v>
@@ -6248,7 +6287,7 @@
         <v>2018</v>
       </c>
       <c r="D53" t="s" s="16">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="E53" t="s" s="16">
         <v>26</v>
@@ -6259,7 +6298,7 @@
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
       <c r="I53" t="s" s="16">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="J53" t="s" s="16">
         <v>29</v>
@@ -6269,14 +6308,14 @@
       <c r="M53" s="17"/>
       <c r="N53" s="19"/>
       <c r="O53" t="s" s="20">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="P53" s="19"/>
       <c r="Q53" s="17"/>
       <c r="R53" s="17"/>
       <c r="S53" s="17"/>
       <c r="T53" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U53" s="19"/>
       <c r="V53" s="19"/>
@@ -6285,7 +6324,7 @@
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="13">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B54" s="14">
         <v>283000000</v>
@@ -6294,13 +6333,13 @@
         <v>2017</v>
       </c>
       <c r="D54" t="s" s="16">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E54" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F54" t="s" s="16">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G54" s="15">
         <v>2012</v>
@@ -6309,30 +6348,30 @@
         <v>2017</v>
       </c>
       <c r="I54" t="s" s="16">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="J54" t="s" s="16">
         <v>29</v>
       </c>
       <c r="K54" t="s" s="16">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="L54" t="s" s="16">
         <v>30</v>
       </c>
       <c r="M54" t="s" s="16">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N54" s="19"/>
       <c r="O54" t="s" s="20">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="P54" s="19"/>
       <c r="Q54" s="17"/>
       <c r="R54" s="17"/>
       <c r="S54" s="17"/>
       <c r="T54" t="s" s="20">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="U54" s="19"/>
       <c r="V54" s="19"/>
@@ -6341,7 +6380,7 @@
     </row>
     <row r="55" ht="20.35" customHeight="1">
       <c r="A55" t="s" s="21">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B55" s="22">
         <v>274000000</v>
@@ -6357,7 +6396,7 @@
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
       <c r="I55" t="s" s="25">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="J55" t="s" s="25">
         <v>13</v>
@@ -6366,7 +6405,7 @@
       <c r="L55" s="24"/>
       <c r="M55" s="24"/>
       <c r="N55" t="s" s="26">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="O55" s="27"/>
       <c r="P55" s="27"/>
@@ -6374,7 +6413,7 @@
       <c r="R55" s="24"/>
       <c r="S55" s="24"/>
       <c r="T55" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="U55" s="27"/>
       <c r="V55" s="27"/>
@@ -6383,7 +6422,7 @@
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="13">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="B56" s="14">
         <v>264254000</v>
@@ -6392,7 +6431,7 @@
         <v>2021</v>
       </c>
       <c r="D56" t="s" s="16">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="E56" t="s" s="16">
         <v>26</v>
@@ -6409,14 +6448,14 @@
       <c r="M56" s="17"/>
       <c r="N56" s="19"/>
       <c r="O56" t="s" s="20">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P56" s="19"/>
       <c r="Q56" s="17"/>
       <c r="R56" s="17"/>
       <c r="S56" s="17"/>
       <c r="T56" t="s" s="20">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="U56" s="19"/>
       <c r="V56" s="19"/>
@@ -6425,7 +6464,7 @@
     </row>
     <row r="57" ht="32.35" customHeight="1">
       <c r="A57" t="s" s="21">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B57" s="22">
         <v>250000000</v>
@@ -6434,18 +6473,18 @@
         <v>2023</v>
       </c>
       <c r="D57" t="s" s="25">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="E57" t="s" s="25">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F57" t="s" s="25">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G57" s="24"/>
       <c r="H57" s="24"/>
       <c r="I57" t="s" s="25">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="J57" t="s" s="25">
         <v>13</v>
@@ -6454,30 +6493,30 @@
       <c r="L57" s="24"/>
       <c r="M57" s="24"/>
       <c r="N57" t="s" s="26">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="O57" t="s" s="26">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="P57" s="27"/>
       <c r="Q57" s="24"/>
       <c r="R57" s="24"/>
       <c r="S57" s="24"/>
       <c r="T57" t="s" s="26">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="U57" t="s" s="26">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="V57" t="s" s="26">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="W57" s="27"/>
       <c r="X57" s="27"/>
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="13">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B58" s="14">
         <v>203000000</v>
@@ -6486,18 +6525,18 @@
         <v>2018</v>
       </c>
       <c r="D58" t="s" s="16">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="E58" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F58" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G58" s="17"/>
       <c r="H58" s="17"/>
       <c r="I58" t="s" s="16">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J58" t="s" s="16">
         <v>29</v>
@@ -6514,10 +6553,10 @@
       <c r="R58" s="17"/>
       <c r="S58" s="17"/>
       <c r="T58" t="s" s="20">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="U58" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V58" s="19"/>
       <c r="W58" s="19"/>
@@ -6525,7 +6564,7 @@
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="13">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B59" s="14">
         <v>200000000</v>
@@ -6534,7 +6573,7 @@
         <v>2022</v>
       </c>
       <c r="D59" t="s" s="16">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E59" t="s" s="16">
         <v>26</v>
@@ -6549,7 +6588,7 @@
         <v>2021</v>
       </c>
       <c r="I59" t="s" s="16">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="J59" t="s" s="16">
         <v>29</v>
@@ -6566,20 +6605,20 @@
       <c r="R59" s="17"/>
       <c r="S59" s="17"/>
       <c r="T59" t="s" s="20">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="U59" t="s" s="20">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="V59" t="s" s="20">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="W59" s="19"/>
       <c r="X59" s="19"/>
     </row>
     <row r="60" ht="32.05" customHeight="1">
       <c r="A60" t="s" s="13">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B60" s="14">
         <v>190000000</v>
@@ -6588,18 +6627,18 @@
         <v>2024</v>
       </c>
       <c r="D60" t="s" s="16">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="E60" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F60" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
       <c r="I60" t="s" s="16">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="J60" t="s" s="16">
         <v>29</v>
@@ -6609,17 +6648,17 @@
       <c r="M60" s="17"/>
       <c r="N60" s="19"/>
       <c r="O60" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P60" s="19"/>
       <c r="Q60" s="17"/>
       <c r="R60" s="17"/>
       <c r="S60" s="19"/>
       <c r="T60" t="s" s="20">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="U60" t="s" s="20">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="V60" s="19"/>
       <c r="W60" s="19"/>
@@ -6627,7 +6666,7 @@
     </row>
     <row r="61" ht="20.05" customHeight="1">
       <c r="A61" t="s" s="13">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B61" s="14">
         <v>188000000</v>
@@ -6636,18 +6675,18 @@
         <v>2021</v>
       </c>
       <c r="D61" t="s" s="16">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="E61" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F61" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G61" s="17"/>
       <c r="H61" s="17"/>
       <c r="I61" t="s" s="16">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="J61" t="s" s="16">
         <v>29</v>
@@ -6657,14 +6696,14 @@
       <c r="M61" s="17"/>
       <c r="N61" s="19"/>
       <c r="O61" t="s" s="20">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="P61" s="19"/>
       <c r="Q61" s="17"/>
       <c r="R61" s="17"/>
       <c r="S61" s="17"/>
       <c r="T61" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U61" s="19"/>
       <c r="V61" s="19"/>
@@ -6673,7 +6712,7 @@
     </row>
     <row r="62" ht="32.05" customHeight="1">
       <c r="A62" t="s" s="13">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B62" s="14">
         <v>176000000</v>
@@ -6682,13 +6721,13 @@
         <v>2024</v>
       </c>
       <c r="D62" t="s" s="16">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="E62" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F62" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G62" s="15">
         <v>2015</v>
@@ -6697,7 +6736,7 @@
         <v>2021</v>
       </c>
       <c r="I62" t="s" s="16">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="J62" t="s" s="16">
         <v>29</v>
@@ -6709,21 +6748,21 @@
       <c r="M62" s="17"/>
       <c r="N62" s="19"/>
       <c r="O62" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P62" t="s" s="20">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="Q62" s="17"/>
       <c r="R62" s="17"/>
       <c r="S62" t="s" s="16">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="T62" t="s" s="20">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="U62" t="s" s="20">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="V62" s="19"/>
       <c r="W62" s="19"/>
@@ -6731,7 +6770,7 @@
     </row>
     <row r="63" ht="20.05" customHeight="1">
       <c r="A63" t="s" s="13">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B63" s="14">
         <v>139739316</v>
@@ -6740,13 +6779,13 @@
         <v>2020</v>
       </c>
       <c r="D63" t="s" s="16">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E63" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F63" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G63" s="15">
         <v>2016</v>
@@ -6755,7 +6794,7 @@
         <v>2020</v>
       </c>
       <c r="I63" t="s" s="16">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="J63" t="s" s="16">
         <v>29</v>
@@ -6766,18 +6805,18 @@
       <c r="N63" s="19"/>
       <c r="O63" s="19"/>
       <c r="P63" t="s" s="20">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="Q63" t="s" s="16">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="R63" s="17"/>
       <c r="S63" s="17"/>
       <c r="T63" t="s" s="20">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="U63" t="s" s="20">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="V63" s="19"/>
       <c r="W63" s="19"/>
@@ -6785,7 +6824,7 @@
     </row>
     <row r="64" ht="20.35" customHeight="1">
       <c r="A64" t="s" s="21">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B64" s="22">
         <v>128000000</v>
@@ -6795,15 +6834,15 @@
       </c>
       <c r="D64" s="24"/>
       <c r="E64" t="s" s="25">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F64" t="s" s="25">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="G64" s="24"/>
       <c r="H64" s="24"/>
       <c r="I64" t="s" s="25">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="J64" t="s" s="25">
         <v>13</v>
@@ -6812,7 +6851,7 @@
       <c r="L64" s="24"/>
       <c r="M64" s="24"/>
       <c r="N64" t="s" s="26">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="O64" s="27"/>
       <c r="P64" s="27"/>
@@ -6820,10 +6859,10 @@
       <c r="R64" s="24"/>
       <c r="S64" s="24"/>
       <c r="T64" t="s" s="26">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="U64" t="s" s="26">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="V64" s="27"/>
       <c r="W64" s="27"/>
@@ -6831,7 +6870,7 @@
     </row>
     <row r="65" ht="32.05" customHeight="1">
       <c r="A65" t="s" s="13">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="B65" s="14">
         <v>104000000</v>
@@ -6840,7 +6879,7 @@
         <v>2024</v>
       </c>
       <c r="D65" t="s" s="16">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="E65" t="s" s="16">
         <v>26</v>
@@ -6858,24 +6897,24 @@
         <v>28</v>
       </c>
       <c r="J65" t="s" s="16">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K65" s="17"/>
       <c r="L65" s="17"/>
       <c r="M65" s="17"/>
       <c r="N65" s="19"/>
       <c r="O65" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P65" s="19"/>
       <c r="Q65" s="17"/>
       <c r="R65" s="17"/>
       <c r="S65" s="17"/>
       <c r="T65" t="s" s="20">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="U65" t="s" s="20">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="V65" s="19"/>
       <c r="W65" s="19"/>
@@ -6883,7 +6922,7 @@
     </row>
     <row r="66" ht="32.05" customHeight="1">
       <c r="A66" t="s" s="13">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="B66" s="14">
         <v>102000000</v>
@@ -6892,13 +6931,13 @@
         <v>2020</v>
       </c>
       <c r="D66" t="s" s="16">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="E66" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F66" t="s" s="16">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G66" s="15">
         <v>2016</v>
@@ -6907,7 +6946,7 @@
         <v>2020</v>
       </c>
       <c r="I66" t="s" s="16">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="J66" t="s" s="16">
         <v>29</v>
@@ -6919,16 +6958,16 @@
       <c r="M66" s="17"/>
       <c r="N66" s="19"/>
       <c r="O66" t="s" s="20">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="P66" t="s" s="20">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="Q66" s="17"/>
       <c r="R66" s="17"/>
       <c r="S66" s="17"/>
       <c r="T66" t="s" s="20">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
@@ -6937,7 +6976,7 @@
     </row>
     <row r="67" ht="32.05" customHeight="1">
       <c r="A67" t="s" s="13">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="B67" s="14">
         <v>80069002</v>
@@ -6946,13 +6985,13 @@
         <v>2023</v>
       </c>
       <c r="D67" t="s" s="16">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="E67" t="s" s="16">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F67" t="s" s="16">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G67" s="15">
         <v>2022</v>
@@ -6961,10 +7000,10 @@
         <v>2023</v>
       </c>
       <c r="I67" t="s" s="16">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="J67" t="s" s="16">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K67" t="s" s="16">
         <v>29</v>
@@ -6975,25 +7014,25 @@
       <c r="M67" s="17"/>
       <c r="N67" s="19"/>
       <c r="O67" t="s" s="20">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="P67" t="s" s="20">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="Q67" t="s" s="16">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="R67" t="s" s="16">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="S67" t="s" s="16">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="T67" t="s" s="20">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="U67" t="s" s="20">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="V67" s="19"/>
       <c r="W67" s="19"/>
@@ -7001,7 +7040,7 @@
     </row>
     <row r="68" ht="20.05" customHeight="1">
       <c r="A68" t="s" s="13">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B68" s="14">
         <v>66000000</v>
@@ -7010,7 +7049,7 @@
         <v>2018</v>
       </c>
       <c r="D68" t="s" s="16">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="E68" t="s" s="16">
         <v>26</v>
@@ -7022,21 +7061,21 @@
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" t="s" s="16">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="K68" s="17"/>
       <c r="L68" s="17"/>
       <c r="M68" s="17"/>
       <c r="N68" s="19"/>
       <c r="O68" t="s" s="20">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="P68" s="19"/>
       <c r="Q68" s="17"/>
       <c r="R68" s="17"/>
       <c r="S68" s="17"/>
       <c r="T68" t="s" s="20">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="U68" s="19"/>
       <c r="V68" s="19"/>
@@ -7045,7 +7084,7 @@
     </row>
     <row r="69" ht="20.05" customHeight="1">
       <c r="A69" t="s" s="13">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B69" s="14">
         <v>59595096</v>
@@ -7054,7 +7093,7 @@
         <v>2020</v>
       </c>
       <c r="D69" t="s" s="16">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="E69" t="s" s="16">
         <v>26</v>
@@ -7065,7 +7104,7 @@
       <c r="G69" s="17"/>
       <c r="H69" s="17"/>
       <c r="I69" t="s" s="16">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="J69" t="s" s="16">
         <v>29</v>
@@ -7080,7 +7119,7 @@
       <c r="R69" s="17"/>
       <c r="S69" s="17"/>
       <c r="T69" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U69" s="19"/>
       <c r="V69" s="19"/>
@@ -7089,7 +7128,7 @@
     </row>
     <row r="70" ht="20.05" customHeight="1">
       <c r="A70" t="s" s="13">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B70" s="14">
         <v>40000000</v>
@@ -7109,10 +7148,10 @@
         <v>2013</v>
       </c>
       <c r="I70" t="s" s="16">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="J70" t="s" s="16">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K70" s="17"/>
       <c r="L70" s="17"/>
@@ -7124,7 +7163,7 @@
       <c r="R70" s="17"/>
       <c r="S70" s="17"/>
       <c r="T70" t="s" s="20">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="U70" s="19"/>
       <c r="V70" s="19"/>
@@ -7133,7 +7172,7 @@
     </row>
     <row r="71" ht="32.05" customHeight="1">
       <c r="A71" t="s" s="13">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B71" s="14">
         <v>37550000</v>
@@ -7142,13 +7181,13 @@
         <v>2023</v>
       </c>
       <c r="D71" t="s" s="16">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E71" t="s" s="16">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F71" t="s" s="16">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G71" s="15">
         <v>2018</v>
@@ -7157,7 +7196,7 @@
         <v>2021</v>
       </c>
       <c r="I71" t="s" s="16">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J71" t="s" s="16">
         <v>29</v>
@@ -7167,14 +7206,14 @@
       <c r="M71" s="17"/>
       <c r="N71" s="19"/>
       <c r="O71" t="s" s="20">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="P71" s="19"/>
       <c r="Q71" s="17"/>
       <c r="R71" s="17"/>
       <c r="S71" s="17"/>
       <c r="T71" t="s" s="20">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="U71" s="19"/>
       <c r="V71" s="19"/>
@@ -7183,7 +7222,7 @@
     </row>
     <row r="72" ht="20.05" customHeight="1">
       <c r="A72" t="s" s="13">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B72" s="14">
         <v>35000000</v>
@@ -7192,13 +7231,13 @@
         <v>2002</v>
       </c>
       <c r="D72" t="s" s="16">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E72" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F72" t="s" s="16">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="G72" s="17"/>
       <c r="H72" s="17"/>
@@ -7209,19 +7248,19 @@
       <c r="M72" s="17"/>
       <c r="N72" s="19"/>
       <c r="O72" t="s" s="20">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="P72" s="19"/>
       <c r="Q72" s="17"/>
       <c r="R72" s="17"/>
       <c r="S72" t="s" s="16">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="T72" t="s" s="20">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U72" t="s" s="20">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="V72" s="19"/>
       <c r="W72" s="19"/>
@@ -7229,7 +7268,7 @@
     </row>
     <row r="73" ht="32.05" customHeight="1">
       <c r="A73" t="s" s="13">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B73" s="14">
         <v>31000000</v>
@@ -7238,13 +7277,13 @@
         <v>2019</v>
       </c>
       <c r="D73" t="s" s="16">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E73" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F73" t="s" s="16">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G73" s="15">
         <v>2017</v>
@@ -7253,7 +7292,7 @@
         <v>2019</v>
       </c>
       <c r="I73" t="s" s="16">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="J73" t="s" s="16">
         <v>29</v>
@@ -7265,22 +7304,22 @@
       <c r="M73" s="17"/>
       <c r="N73" s="19"/>
       <c r="O73" t="s" s="20">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="P73" t="s" s="20">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="Q73" t="s" s="16">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="R73" t="s" s="16">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="S73" t="s" s="16">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="T73" t="s" s="20">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="U73" s="19"/>
       <c r="V73" s="19"/>
@@ -7289,7 +7328,7 @@
     </row>
     <row r="74" ht="20.05" customHeight="1">
       <c r="A74" t="s" s="13">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="B74" s="14">
         <v>30000000</v>
@@ -7298,7 +7337,7 @@
         <v>2009</v>
       </c>
       <c r="D74" t="s" s="16">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="E74" t="s" s="16">
         <v>26</v>
@@ -7312,7 +7351,7 @@
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
       <c r="J74" t="s" s="16">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="K74" s="17"/>
       <c r="L74" s="17"/>
@@ -7324,7 +7363,7 @@
       <c r="R74" s="17"/>
       <c r="S74" s="17"/>
       <c r="T74" t="s" s="20">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="U74" s="19"/>
       <c r="V74" s="19"/>
@@ -7333,7 +7372,7 @@
     </row>
     <row r="75" ht="44.05" customHeight="1">
       <c r="A75" t="s" s="13">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B75" s="14">
         <v>24000000</v>
@@ -7342,13 +7381,13 @@
         <v>2022</v>
       </c>
       <c r="D75" t="s" s="16">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="E75" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F75" t="s" s="16">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G75" s="15">
         <v>2015</v>
@@ -7357,7 +7396,7 @@
         <v>2016</v>
       </c>
       <c r="I75" t="s" s="16">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="J75" t="s" s="16">
         <v>29</v>
@@ -7367,31 +7406,31 @@
       <c r="M75" s="17"/>
       <c r="N75" s="19"/>
       <c r="O75" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P75" t="s" s="20">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="Q75" s="17"/>
       <c r="R75" s="17"/>
       <c r="S75" t="s" s="16">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="T75" t="s" s="20">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="U75" t="s" s="20">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="V75" t="s" s="20">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="W75" s="19"/>
       <c r="X75" s="19"/>
     </row>
     <row r="76" ht="20.05" customHeight="1">
       <c r="A76" t="s" s="13">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B76" s="14">
         <v>23671000</v>
@@ -7400,13 +7439,13 @@
         <v>2008</v>
       </c>
       <c r="D76" t="s" s="16">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="E76" t="s" s="16">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F76" t="s" s="16">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G76" s="15">
         <v>2004</v>
@@ -7421,17 +7460,17 @@
       <c r="M76" s="17"/>
       <c r="N76" s="19"/>
       <c r="O76" t="s" s="20">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="P76" s="19"/>
       <c r="Q76" s="17"/>
       <c r="R76" s="17"/>
       <c r="S76" s="17"/>
       <c r="T76" t="s" s="20">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="U76" t="s" s="20">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="V76" s="19"/>
       <c r="W76" s="19"/>
@@ -7439,7 +7478,7 @@
     </row>
     <row r="77" ht="20.05" customHeight="1">
       <c r="A77" t="s" s="13">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B77" s="14">
         <v>22917478</v>
@@ -7448,7 +7487,7 @@
         <v>2013</v>
       </c>
       <c r="D77" t="s" s="16">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E77" t="s" s="16">
         <v>26</v>
@@ -7463,30 +7502,30 @@
         <v>2012</v>
       </c>
       <c r="I77" t="s" s="16">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="J77" t="s" s="16">
         <v>29</v>
       </c>
       <c r="K77" t="s" s="16">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="L77" t="s" s="16">
         <v>30</v>
       </c>
       <c r="M77" t="s" s="16">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="N77" s="19"/>
       <c r="O77" t="s" s="20">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="P77" s="19"/>
       <c r="Q77" s="17"/>
       <c r="R77" s="17"/>
       <c r="S77" s="17"/>
       <c r="T77" t="s" s="20">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="U77" s="19"/>
       <c r="V77" s="19"/>
@@ -7495,7 +7534,7 @@
     </row>
     <row r="78" ht="20.05" customHeight="1">
       <c r="A78" t="s" s="13">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B78" s="14">
         <v>20000000</v>
@@ -7504,13 +7543,13 @@
         <v>2023</v>
       </c>
       <c r="D78" t="s" s="16">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="E78" t="s" s="16">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F78" t="s" s="16">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="G78" s="15">
         <v>2023</v>
@@ -7519,7 +7558,7 @@
         <v>2024</v>
       </c>
       <c r="I78" t="s" s="16">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="J78" t="s" s="16">
         <v>29</v>
@@ -7533,19 +7572,19 @@
       <c r="M78" s="17"/>
       <c r="N78" s="19"/>
       <c r="O78" t="s" s="20">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="P78" t="s" s="20">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q78" s="17"/>
       <c r="R78" s="17"/>
       <c r="S78" s="17"/>
       <c r="T78" t="s" s="20">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="U78" t="s" s="20">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="V78" s="17"/>
       <c r="W78" s="19"/>
@@ -7553,7 +7592,7 @@
     </row>
     <row r="79" ht="20.05" customHeight="1">
       <c r="A79" t="s" s="13">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B79" s="14">
         <v>15700000</v>
@@ -7562,18 +7601,18 @@
         <v>2015</v>
       </c>
       <c r="D79" t="s" s="16">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="E79" t="s" s="16">
         <v>26</v>
       </c>
       <c r="F79" t="s" s="16">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G79" s="17"/>
       <c r="H79" s="17"/>
       <c r="I79" t="s" s="16">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="J79" t="s" s="16">
         <v>29</v>
@@ -7589,10 +7628,10 @@
       <c r="Q79" s="17"/>
       <c r="R79" s="17"/>
       <c r="S79" t="s" s="16">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="T79" t="s" s="20">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U79" s="19"/>
       <c r="V79" s="19"/>
@@ -7601,7 +7640,7 @@
     </row>
     <row r="80" ht="20.05" customHeight="1">
       <c r="A80" t="s" s="13">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B80" s="14">
         <v>10333332</v>
@@ -7610,7 +7649,7 @@
         <v>2024</v>
       </c>
       <c r="D80" t="s" s="16">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="E80" t="s" s="16">
         <v>26</v>
@@ -7625,7 +7664,7 @@
         <v>2024</v>
       </c>
       <c r="I80" t="s" s="16">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="J80" t="s" s="16">
         <v>29</v>
@@ -7637,19 +7676,19 @@
       <c r="M80" s="17"/>
       <c r="N80" s="19"/>
       <c r="O80" t="s" s="20">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="P80" t="s" s="20">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q80" s="17"/>
       <c r="R80" s="17"/>
       <c r="S80" s="17"/>
       <c r="T80" t="s" s="20">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="U80" t="s" s="20">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="V80" s="19"/>
       <c r="W80" s="19"/>
@@ -7657,7 +7696,7 @@
     </row>
     <row r="81" ht="32.35" customHeight="1">
       <c r="A81" t="s" s="28">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B81" s="22">
         <v>9000000</v>
@@ -7666,18 +7705,18 @@
         <v>2023</v>
       </c>
       <c r="D81" t="s" s="31">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="E81" t="s" s="25">
         <v>26</v>
       </c>
       <c r="F81" t="s" s="25">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G81" s="24"/>
       <c r="H81" s="24"/>
       <c r="I81" t="s" s="25">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="J81" t="s" s="25">
         <v>13</v>
@@ -7686,30 +7725,30 @@
       <c r="L81" s="24"/>
       <c r="M81" s="24"/>
       <c r="N81" t="s" s="26">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="O81" t="s" s="26">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="P81" s="27"/>
       <c r="Q81" s="24"/>
       <c r="R81" s="24"/>
       <c r="S81" s="24"/>
       <c r="T81" t="s" s="26">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="U81" t="s" s="26">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="V81" t="s" s="26">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="W81" s="27"/>
       <c r="X81" s="27"/>
     </row>
     <row r="82" ht="20.35" customHeight="1">
       <c r="A82" t="s" s="28">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B82" s="29">
         <v>1022000</v>
@@ -7725,7 +7764,7 @@
       <c r="G82" s="24"/>
       <c r="H82" s="24"/>
       <c r="I82" t="s" s="25">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="J82" t="s" s="25">
         <v>13</v>
@@ -7734,7 +7773,7 @@
       <c r="L82" s="24"/>
       <c r="M82" s="24"/>
       <c r="N82" t="s" s="26">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="O82" s="27"/>
       <c r="P82" s="27"/>
@@ -7742,10 +7781,10 @@
       <c r="R82" s="24"/>
       <c r="S82" s="24"/>
       <c r="T82" t="s" s="26">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="U82" t="s" s="26">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="V82" s="27"/>
       <c r="W82" s="27"/>
@@ -7753,7 +7792,7 @@
     </row>
     <row r="83" ht="44.35" customHeight="1">
       <c r="A83" t="s" s="28">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B83" s="29">
         <v>239000000</v>
@@ -7762,13 +7801,13 @@
         <v>2024</v>
       </c>
       <c r="D83" t="s" s="25">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="E83" t="s" s="25">
         <v>26</v>
       </c>
       <c r="F83" t="s" s="25">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G83" s="23">
         <v>2018</v>
@@ -7783,16 +7822,16 @@
       <c r="M83" s="24"/>
       <c r="N83" s="27"/>
       <c r="O83" t="s" s="26">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="P83" t="s" s="26">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="Q83" s="24"/>
       <c r="R83" s="24"/>
       <c r="S83" s="24"/>
       <c r="T83" t="s" s="26">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="U83" s="27"/>
       <c r="V83" s="27"/>
@@ -7801,7 +7840,7 @@
     </row>
     <row r="84" ht="32.35" customHeight="1">
       <c r="A84" t="s" s="28">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="B84" s="29">
         <v>146000000</v>
@@ -7810,7 +7849,7 @@
         <v>2021</v>
       </c>
       <c r="D84" t="s" s="25">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="E84" t="s" s="25">
         <v>37</v>
@@ -7824,24 +7863,24 @@
       </c>
       <c r="I84" s="24"/>
       <c r="J84" t="s" s="25">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="K84" s="24"/>
       <c r="L84" s="24"/>
       <c r="M84" s="24"/>
       <c r="N84" s="27"/>
       <c r="O84" t="s" s="26">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="P84" s="27"/>
       <c r="Q84" s="24"/>
       <c r="R84" s="24"/>
       <c r="S84" s="24"/>
       <c r="T84" t="s" s="26">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="U84" t="s" s="26">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="V84" s="27"/>
       <c r="W84" s="27"/>
@@ -7849,7 +7888,7 @@
     </row>
     <row r="85" ht="56.35" customHeight="1">
       <c r="A85" t="s" s="28">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B85" s="29">
         <v>500000000</v>
@@ -7858,7 +7897,7 @@
         <v>2024</v>
       </c>
       <c r="D85" t="s" s="25">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="E85" t="s" s="25">
         <v>26</v>
@@ -7873,41 +7912,41 @@
         <v>2018</v>
       </c>
       <c r="I85" t="s" s="25">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="J85" t="s" s="25">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="K85" t="s" s="25">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="L85" t="s" s="25">
         <v>30</v>
       </c>
       <c r="M85" t="s" s="25">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N85" s="27"/>
       <c r="O85" t="s" s="26">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="P85" t="s" s="26">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="Q85" t="s" s="25">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="R85" t="s" s="16">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="S85" t="s" s="25">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="T85" t="s" s="26">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="U85" t="s" s="26">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="V85" s="27"/>
       <c r="W85" s="27"/>
@@ -7915,14 +7954,14 @@
     </row>
     <row r="86" ht="32.35" customHeight="1">
       <c r="A86" t="s" s="28">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B86" s="29"/>
       <c r="C86" s="23">
         <v>2023</v>
       </c>
       <c r="D86" t="s" s="25">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="E86" t="s" s="25">
         <v>26</v>
@@ -7937,7 +7976,7 @@
         <v>2023</v>
       </c>
       <c r="I86" t="s" s="25">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="J86" t="s" s="25">
         <v>29</v>
@@ -7947,34 +7986,34 @@
       <c r="M86" s="24"/>
       <c r="N86" s="27"/>
       <c r="O86" t="s" s="26">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="P86" s="27"/>
       <c r="Q86" s="24"/>
       <c r="R86" s="17"/>
       <c r="S86" s="24"/>
       <c r="T86" t="s" s="26">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="U86" t="s" s="26">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="V86" t="s" s="26">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="W86" s="27"/>
       <c r="X86" s="27"/>
     </row>
     <row r="87" ht="32.35" customHeight="1">
       <c r="A87" t="s" s="28">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B87" s="29"/>
       <c r="C87" s="23">
         <v>2023</v>
       </c>
       <c r="D87" t="s" s="25">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="E87" t="s" s="25">
         <v>26</v>
@@ -7987,7 +8026,7 @@
         <v>2023</v>
       </c>
       <c r="I87" t="s" s="25">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="J87" t="s" s="25">
         <v>29</v>
@@ -7997,14 +8036,14 @@
       <c r="M87" s="24"/>
       <c r="N87" s="27"/>
       <c r="O87" t="s" s="26">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="P87" s="27"/>
       <c r="Q87" s="24"/>
       <c r="R87" s="17"/>
       <c r="S87" s="24"/>
       <c r="T87" t="s" s="26">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="U87" s="27"/>
       <c r="V87" s="27"/>
@@ -8013,27 +8052,27 @@
     </row>
     <row r="88" ht="32.35" customHeight="1">
       <c r="A88" t="s" s="28">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="B88" s="29"/>
       <c r="C88" s="23">
         <v>2023</v>
       </c>
       <c r="D88" t="s" s="25">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="E88" t="s" s="25">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F88" t="s" s="25">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G88" s="24"/>
       <c r="H88" s="23">
         <v>2023</v>
       </c>
       <c r="I88" t="s" s="25">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="J88" t="s" s="25">
         <v>29</v>
@@ -8048,7 +8087,7 @@
       <c r="R88" s="17"/>
       <c r="S88" s="24"/>
       <c r="T88" t="s" s="26">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="U88" s="27"/>
       <c r="V88" s="27"/>
@@ -8070,131 +8109,134 @@
     <hyperlink ref="V2" r:id="rId3" location="" tooltip="" display="https://www.fastcheck.cl/2023/05/16/misterio-sin-resolver-ocho-escandalos-de-corrupcion-municipal-pendientes-de-justicia/"/>
     <hyperlink ref="T3" r:id="rId4" location="" tooltip="" display="https://es.wikipedia.org/wiki/Pacogate#Investigación_y_sentencias"/>
     <hyperlink ref="T4" r:id="rId5" location="" tooltip="" display="https://radio.uchile.cl/2024/01/17/en-suspenso-prision-preventiva-para-cathy-barriga-tribunal-dictara-cautelar-este-jueves/"/>
-    <hyperlink ref="T7" r:id="rId6" location="" tooltip="" display="https://interferencia.cl/articulos/tres-graves-casos-de-corrupcion-en-que-latam-se-ha-visto-envuelta-en-su-historia-reciente"/>
-    <hyperlink ref="T8" r:id="rId7" location="" tooltip="" display="https://es.wikipedia.org/wiki/Pinocheques"/>
-    <hyperlink ref="T9" r:id="rId8" location="" tooltip="" display="https://www.chiletransparente.cl/caso-sqm/"/>
-    <hyperlink ref="T10" r:id="rId9" location="" tooltip="" display="https://www.ciperchile.cl/2018/04/02/los-negocios-ilicitos-de-juan-castro-el-ex-alcalde-de-talca-que-llego-al-senado/"/>
-    <hyperlink ref="T11" r:id="rId10" location="" tooltip="" display="https://www.meganoticias.cl/nacional/402950-malversacion-10-mil-millones-educacion-sergio-echeverria-exalcalde-san-joaquin-19-01-2023.html"/>
-    <hyperlink ref="T12" r:id="rId11" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T13" r:id="rId12" location="" tooltip="" display="https://www.aduana.cl/megafraude-tributario-investigacion-de-aduanas-fue-clave-para/aduana/2023-12-21/174405.html"/>
-    <hyperlink ref="T14" r:id="rId13" location="" tooltip="" display="https://www.latercera.com/la-tercera-pm/noticia/estafa-fraude-y-falsificacion-el-avance-en-la-investigacion-penal-en-las-condes-que-remece-a-la-administracion-penaloza/X7ZBPJAYLRA47LINUR5COTA5HY/"/>
-    <hyperlink ref="U14" r:id="rId14" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/las-investigaciones-que-envuelven-al-municipio-de-las-condes-y-a-su-alcaldesa-daniela-penaloza/GYYWEXRFXNGJVKFJPOEWRQUB7I/"/>
-    <hyperlink ref="T15" r:id="rId15" location="" tooltip="" display="https://es.wikipedia.org/wiki/Milicogate"/>
-    <hyperlink ref="U15" r:id="rId16" location="" tooltip="" display="https://www.latercera.com/la-tercera-domingo/noticia/el-metodo-rutherford-como-fueron-cayendo-uno-a-uno-los-comandantes-en-jefe-por-el-fraude-en-el-ejercito/IVKUSHEYJBDYHMSYZ4R3KZXQE4/"/>
-    <hyperlink ref="T16" r:id="rId17" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-metropolitana/2022/01/31/presentan-querella-contra-exalcaldesa-de-lampa-por-millonaria-deuda-de-cotizaciones.shtml"/>
-    <hyperlink ref="T17" r:id="rId18" location="" tooltip="" display="https://www.diarioconstitucional.cl/2021/04/17/detalles-del-caso-corpesca-tercer-tribunal-de-juicio-oral-en-lo-penal-de-santiago-condeno-al-exsenador-jaime-orpis-a-la-pena-unica-de-5-anos-y-un-dia-de-presidio-efectivo-en-calidad-de-autor-de-seis/"/>
-    <hyperlink ref="U17" r:id="rId19" location="" tooltip="" display="https://contracarga.cl/reportajes/caso-corpesca-explicado/"/>
-    <hyperlink ref="V17" r:id="rId20" location="" tooltip="" display="https://www.ciperchile.cl/2016/08/17/el-articulo-de-la-ley-de-pesca-que-le-ahorro-4-670-millones-a-corpesca/"/>
-    <hyperlink ref="T18" r:id="rId21" location="" tooltip="" display="https://www.elmostrador.cl/destacado/2023/02/06/los-2-500-millones-de-la-corporacion-municipal-de-la-florida-que-carter-no-termina-de-explicar/"/>
-    <hyperlink ref="U18" r:id="rId22" location="" tooltip="" display="https://www.biobiochile.cl/especial/bbcl-investiga/noticias/articulos/2023/01/27/detectan-diferencias-por-mas-de-4-600-millones-en-cuentas-bancarias-de-educacion-de-la-florida.shtml"/>
-    <hyperlink ref="T19" r:id="rId23" location="" tooltip="" display="https://www.latercera.com/la-tercera-sabado/noticia/cientos-de-depositos-en-efectivo-y-una-cuenta-con-2300-millones-las-pruebas-que-complican-al-tronco-torrealba/LH674LXDYVBR3J5IDIFUCMRIXE/"/>
-    <hyperlink ref="U19" r:id="rId24" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/20/caso-torrealba-detalles-de-gastos-de-campana-de-rn-que-fueron-financiados-con-dineros-de-vitacura/"/>
-    <hyperlink ref="V19" r:id="rId25" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2023/08/08/53-dias-tras-las-rejas-rechazan-solicitud-de-raul-torrealba-y-seguira-en-prision-preventiva/"/>
-    <hyperlink ref="W19" r:id="rId26" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/vitacura-contraloria-objeta-mas-de-4500-millones-a-administracion-de-alcalde-torrealba-en-dos-anos/GK3X6GQBOVB5BFGOV4N52T3PXI/"/>
-    <hyperlink ref="T20" r:id="rId27" location="" tooltip="" display="https://interferencia.cl/articulos/contraloria-realiza-sumario-en-estacion-central-por-deficit-de-4300-millones-detectado"/>
-    <hyperlink ref="T21" r:id="rId28" location="" tooltip="" display="https://www.elrancaguino.cl/2024/01/18/hasta-35-anos-de-carcel-y-el-pago-de-2-mil-millones-de-pesos-en-multas-arriesga-el-ex-alcalde-san-fernando-luis-berwart/"/>
-    <hyperlink ref="T22" r:id="rId29" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U22" r:id="rId30" location="" tooltip="" display="https://www.df.cl/aniversario/caso-inverlink-el-escandalo-que-amenazo-la-estabilidad-del-mercado"/>
-    <hyperlink ref="T23" r:id="rId31" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="U23" r:id="rId32" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/07/06/1100220/fundacion-el-desarrollo-de-organizaciones.html"/>
-    <hyperlink ref="T24" r:id="rId33" location="" tooltip="" display="https://www.meganoticias.cl/amp/nacional/442953-mantencion-de-areas-verdes-alcalde-de-arica-firmo-trato-directo-por-1100-millones-con-empresa-creada-14-dias-antes.html"/>
-    <hyperlink ref="T25" r:id="rId34" location="" tooltip="" display="https://www.latercera.com/earlyaccess/noticia/las-millonarias-transacciones-que-complican-al-alcalde-de-rancagua/GY4SPWLFPJDODKTTXDN7FR74B4/"/>
-    <hyperlink ref="U25" r:id="rId35" location="" tooltip="" display="https://radio.uchile.cl/2023/03/04/tras-allanamiento-a-alcalde-de-rancagua-expertos-en-transparencia-llaman-a-fortalecer-los-mecanismos-para-perseguir-la-corrupcion/"/>
-    <hyperlink ref="V25" r:id="rId36" location="" tooltip="" display="https://www.meganoticias.cl/nacional/442934-alcalde-rancagua-formalizacion-abril-delitos-corrupcion-juan-ramon-godoy-21-03-2024.html"/>
-    <hyperlink ref="W25" r:id="rId37" location="" tooltip="" display="https://www.cde.cl/cde-interpone-querella-criminal-contra-el-alcalde-de-rancagua-por-delitos-asociados-a-hechos-de-corrupcion/"/>
-    <hyperlink ref="U26" r:id="rId38" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml"/>
-    <hyperlink ref="T27" r:id="rId39" location="" tooltip="" display="https://www.cnnchile.com/pais/destitucion-alcalde-rinconada-contraloria-irregularidades_20230606/"/>
-    <hyperlink ref="U27" r:id="rId40" location="" tooltip="" display="https://munirinconada.cl/alcalde-juan-galdames-se-refiere-a-juicio-de-cuentas-que-ordena-la-restitucion-de-300-millones/"/>
-    <hyperlink ref="T28" r:id="rId41" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
-    <hyperlink ref="T29" r:id="rId42" location="" tooltip="" display="https://www.ovejeronoticias.cl/2023/12/puerto-natales-ex-alcalde-udi-fernando-paredes-continua-con-reclusion-domiciliaria-total/"/>
-    <hyperlink ref="U29" r:id="rId43" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T30" r:id="rId44" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
-    <hyperlink ref="T31" r:id="rId45" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T32" r:id="rId46" location="" tooltip="" display="https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022"/>
-    <hyperlink ref="T33" r:id="rId47" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U33" r:id="rId48" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
-    <hyperlink ref="T34" r:id="rId49" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T35" r:id="rId50" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="U35" r:id="rId51" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
-    <hyperlink ref="T36" r:id="rId52" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
-    <hyperlink ref="T37" r:id="rId53" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
-    <hyperlink ref="T38" r:id="rId54" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="T39" r:id="rId55" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/03/19/milicogate-dictan-procesamiento-contra-general-y-coroneles-r-por-presunto-fraude-de-519-millones.shtml"/>
-    <hyperlink ref="T41" r:id="rId56" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
-    <hyperlink ref="U41" r:id="rId57" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
-    <hyperlink ref="V41" r:id="rId58" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
-    <hyperlink ref="T42" r:id="rId59" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="U42" r:id="rId60" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
-    <hyperlink ref="V42" r:id="rId61" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/12/29/caso-manicure/"/>
-    <hyperlink ref="T43" r:id="rId62" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/11/pdi-allano-gobernacion-del-maule-en-medio-de-investigaciones-por-traspasos-a-urbanismo-social.shtml"/>
-    <hyperlink ref="U43" r:id="rId63" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/12/caso-convenios-jefe-de-control-interno-del-gore-maule-declaro-por-traspasos-a-urbanismo-social.shtml"/>
-    <hyperlink ref="T44" r:id="rId64" location="" tooltip="" display="https://www.eldesconcierto.cl/reportajes/2024/01/23/municipio-se-querella-por-multa-de-500-millones-acusan-a-exalcalde-de-melipilla-por-fraude-al-fisco.html"/>
-    <hyperlink ref="U44" r:id="rId65" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/municipalidad-de-melipilla-presenta-querella-por-fraude-al-fisco-contra-el-exalcalde-ivan-campos/P6XRT2X73NAHJIEMIZWPRX6VEU/"/>
-    <hyperlink ref="T45" r:id="rId66" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2019/05/05/las-vueltas-de-la-vida-rn-elige-a-claudio-eguiluz-condenado-por-caso-sqm-como-su-presidente-regional-en-el-biobio/"/>
-    <hyperlink ref="T46" r:id="rId67" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="T47" r:id="rId68" location="" tooltip="" display="https://radionuevomundo.cl/2023/07/18/gobernador-rivas-suma-al-caso-fundacion-local-traspasos-arbitrarios-a-coihue-y-a-universidades-de-la-araucania/"/>
-    <hyperlink ref="U47" r:id="rId69" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
-    <hyperlink ref="V47" r:id="rId70" location="" tooltip="" display="https://resumen.cl/articulos/la-derecha-de-la-araucania-en-el-caso-fundaciones-las-irregularidades-de-espacio-coigue-que-llevaron-al-ministerio-de-justicia-a-solicitar-su-cierre"/>
-    <hyperlink ref="T48" r:id="rId71" location="" tooltip="" display="https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/"/>
-    <hyperlink ref="T49" r:id="rId72" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml"/>
-    <hyperlink ref="U49" r:id="rId73" location="" tooltip="" display="https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana"/>
-    <hyperlink ref="V49" r:id="rId74" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-biobio/detienen-a-lider-de-empresa-en-allanamiento-por-caso-convenios-pdi/2024-03-13/123002.html"/>
-    <hyperlink ref="T50" r:id="rId75" location="" tooltip="" display="http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739"/>
-    <hyperlink ref="U50" r:id="rId76" location="" tooltip="" display="https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica"/>
-    <hyperlink ref="T51" r:id="rId77" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
-    <hyperlink ref="T52" r:id="rId78" location="" tooltip="" display="https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/"/>
-    <hyperlink ref="T53" r:id="rId79" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T55" r:id="rId80" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="T56" r:id="rId81" location="" tooltip="" display="https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/"/>
-    <hyperlink ref="T57" r:id="rId82" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
-    <hyperlink ref="U57" r:id="rId83" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
-    <hyperlink ref="V57" r:id="rId84" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="T58" r:id="rId85" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
-    <hyperlink ref="U58" r:id="rId86" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T59" r:id="rId87" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
-    <hyperlink ref="U59" r:id="rId88" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
-    <hyperlink ref="V59" r:id="rId89" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
-    <hyperlink ref="T60" r:id="rId90" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
-    <hyperlink ref="U60" r:id="rId91" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml"/>
-    <hyperlink ref="T61" r:id="rId92" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T62" r:id="rId93" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
-    <hyperlink ref="U62" r:id="rId94" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
-    <hyperlink ref="T63" r:id="rId95" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html"/>
-    <hyperlink ref="T64" r:id="rId96" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
-    <hyperlink ref="U64" r:id="rId97" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
-    <hyperlink ref="T65" r:id="rId98" location="" tooltip="" display="https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/"/>
-    <hyperlink ref="U65" r:id="rId99" location="" tooltip="" display="https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html"/>
-    <hyperlink ref="T66" r:id="rId100" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
-    <hyperlink ref="T67" r:id="rId101" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
-    <hyperlink ref="U67" r:id="rId102" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
-    <hyperlink ref="T68" r:id="rId103" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
-    <hyperlink ref="T69" r:id="rId104" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T70" r:id="rId105" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
-    <hyperlink ref="T71" r:id="rId106" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
-    <hyperlink ref="T72" r:id="rId107" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U72" r:id="rId108" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
-    <hyperlink ref="T73" r:id="rId109" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
-    <hyperlink ref="T75" r:id="rId110" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
-    <hyperlink ref="U75" r:id="rId111" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
-    <hyperlink ref="V75" r:id="rId112" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
-    <hyperlink ref="T76" r:id="rId113" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U76" r:id="rId114" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
-    <hyperlink ref="T77" r:id="rId115" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
-    <hyperlink ref="T78" r:id="rId116" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
-    <hyperlink ref="U78" r:id="rId117" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/04/02/fiscalia-formalizara-a-daniel-jadue-por-cohecho-administracion-desleal-fraude-al-fisco-y-estafa.shtml"/>
-    <hyperlink ref="T79" r:id="rId118" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T81" r:id="rId119" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="U81" r:id="rId120" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
-    <hyperlink ref="V81" r:id="rId121" location="" tooltip="" display="https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/"/>
-    <hyperlink ref="T82" r:id="rId122" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
-    <hyperlink ref="U82" r:id="rId123" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
-    <hyperlink ref="T83" r:id="rId124" location="" tooltip="" display="https://www.latercera.com/opinion/noticia/columna-de-daniel-matamala-cual-elefante/EOAKP2PXWJHSFDBAKRXGVVS5ZA/"/>
-    <hyperlink ref="T84" r:id="rId125" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/formalizan-a-exdirector-general-de-la-pdi-hector-espinosa-fiscalia-le-imputa-apropiacion-de-dineros-de-gastos-reservados-de-la-institucion/IBGS7P3IPVGU3MQU4A7GJDH4UA/"/>
-    <hyperlink ref="U84" r:id="rId126" location="" tooltip="" display="https://www.chvnoticias.cl/exclusivo-chv/todas-las-pruebas-fiscalia-hector-espinosa-pdi_20220828/"/>
-    <hyperlink ref="T85" r:id="rId127" location="" tooltip="" display="https://www.latercera.com/campuslt/noticia/luminarias-juzgado-de-garantia-de-iquique-condena-a-exconcejal-felipe-arenas-por-fraude-al-fisco-y-cohecho/OR3BBHZLARCULI7J5A22A66CSU/"/>
-    <hyperlink ref="U85" r:id="rId128" location="" tooltip="" display="https://iquiquetv.cl/2024/07/02/caso-luminarias-led-condenan-a-ex-concejal-felipe-arenas-por-cohecho-y-fraude-al-fisco/"/>
-    <hyperlink ref="V86" r:id="rId129" location="" tooltip="" display="https://www.meganoticias.cl/nacional/415393-cuentas-corrientes-empresario-acusado-pagar-sobornos-involucra-fraude-70-municipios-28-05-2023.html"/>
-    <hyperlink ref="T88" r:id="rId130" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
+    <hyperlink ref="U4" r:id="rId6" location="" tooltip="" display="https://lavozdemaipu.cl/cathy-barriga-ultimo-informe-con-peras-y-manzanas/"/>
+    <hyperlink ref="V4" r:id="rId7" location="" tooltip="" display="https://www.tvn.cl/programas/buenos-dias-a-todos/actualidad/caso-cathy-barriga-los-41-mil-millones-de-pesos-que-no-se-saben-donde"/>
+    <hyperlink ref="T7" r:id="rId8" location="" tooltip="" display="https://interferencia.cl/articulos/tres-graves-casos-de-corrupcion-en-que-latam-se-ha-visto-envuelta-en-su-historia-reciente"/>
+    <hyperlink ref="T8" r:id="rId9" location="" tooltip="" display="https://es.wikipedia.org/wiki/Pinocheques"/>
+    <hyperlink ref="T9" r:id="rId10" location="" tooltip="" display="https://www.chiletransparente.cl/caso-sqm/"/>
+    <hyperlink ref="T10" r:id="rId11" location="" tooltip="" display="https://www.ciperchile.cl/2018/04/02/los-negocios-ilicitos-de-juan-castro-el-ex-alcalde-de-talca-que-llego-al-senado/"/>
+    <hyperlink ref="T11" r:id="rId12" location="" tooltip="" display="https://www.meganoticias.cl/nacional/402950-malversacion-10-mil-millones-educacion-sergio-echeverria-exalcalde-san-joaquin-19-01-2023.html"/>
+    <hyperlink ref="T12" r:id="rId13" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T13" r:id="rId14" location="" tooltip="" display="https://www.aduana.cl/megafraude-tributario-investigacion-de-aduanas-fue-clave-para/aduana/2023-12-21/174405.html"/>
+    <hyperlink ref="T14" r:id="rId15" location="" tooltip="" display="https://www.latercera.com/la-tercera-pm/noticia/estafa-fraude-y-falsificacion-el-avance-en-la-investigacion-penal-en-las-condes-que-remece-a-la-administracion-penaloza/X7ZBPJAYLRA47LINUR5COTA5HY/"/>
+    <hyperlink ref="U14" r:id="rId16" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/las-investigaciones-que-envuelven-al-municipio-de-las-condes-y-a-su-alcaldesa-daniela-penaloza/GYYWEXRFXNGJVKFJPOEWRQUB7I/"/>
+    <hyperlink ref="T15" r:id="rId17" location="" tooltip="" display="https://es.wikipedia.org/wiki/Milicogate"/>
+    <hyperlink ref="U15" r:id="rId18" location="" tooltip="" display="https://www.latercera.com/la-tercera-domingo/noticia/el-metodo-rutherford-como-fueron-cayendo-uno-a-uno-los-comandantes-en-jefe-por-el-fraude-en-el-ejercito/IVKUSHEYJBDYHMSYZ4R3KZXQE4/"/>
+    <hyperlink ref="T16" r:id="rId19" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-metropolitana/2022/01/31/presentan-querella-contra-exalcaldesa-de-lampa-por-millonaria-deuda-de-cotizaciones.shtml"/>
+    <hyperlink ref="T17" r:id="rId20" location="" tooltip="" display="https://www.diarioconstitucional.cl/2021/04/17/detalles-del-caso-corpesca-tercer-tribunal-de-juicio-oral-en-lo-penal-de-santiago-condeno-al-exsenador-jaime-orpis-a-la-pena-unica-de-5-anos-y-un-dia-de-presidio-efectivo-en-calidad-de-autor-de-seis/"/>
+    <hyperlink ref="U17" r:id="rId21" location="" tooltip="" display="https://contracarga.cl/reportajes/caso-corpesca-explicado/"/>
+    <hyperlink ref="V17" r:id="rId22" location="" tooltip="" display="https://www.ciperchile.cl/2016/08/17/el-articulo-de-la-ley-de-pesca-que-le-ahorro-4-670-millones-a-corpesca/"/>
+    <hyperlink ref="T18" r:id="rId23" location="" tooltip="" display="https://www.elmostrador.cl/destacado/2023/02/06/los-2-500-millones-de-la-corporacion-municipal-de-la-florida-que-carter-no-termina-de-explicar/"/>
+    <hyperlink ref="U18" r:id="rId24" location="" tooltip="" display="https://www.biobiochile.cl/especial/bbcl-investiga/noticias/articulos/2023/01/27/detectan-diferencias-por-mas-de-4-600-millones-en-cuentas-bancarias-de-educacion-de-la-florida.shtml"/>
+    <hyperlink ref="T19" r:id="rId25" location="" tooltip="" display="https://www.latercera.com/la-tercera-sabado/noticia/cientos-de-depositos-en-efectivo-y-una-cuenta-con-2300-millones-las-pruebas-que-complican-al-tronco-torrealba/LH674LXDYVBR3J5IDIFUCMRIXE/"/>
+    <hyperlink ref="U19" r:id="rId26" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/20/caso-torrealba-detalles-de-gastos-de-campana-de-rn-que-fueron-financiados-con-dineros-de-vitacura/"/>
+    <hyperlink ref="V19" r:id="rId27" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2023/08/08/53-dias-tras-las-rejas-rechazan-solicitud-de-raul-torrealba-y-seguira-en-prision-preventiva/"/>
+    <hyperlink ref="W19" r:id="rId28" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/vitacura-contraloria-objeta-mas-de-4500-millones-a-administracion-de-alcalde-torrealba-en-dos-anos/GK3X6GQBOVB5BFGOV4N52T3PXI/"/>
+    <hyperlink ref="T20" r:id="rId29" location="" tooltip="" display="https://interferencia.cl/articulos/contraloria-realiza-sumario-en-estacion-central-por-deficit-de-4300-millones-detectado"/>
+    <hyperlink ref="T21" r:id="rId30" location="" tooltip="" display="https://www.elrancaguino.cl/2024/01/18/hasta-35-anos-de-carcel-y-el-pago-de-2-mil-millones-de-pesos-en-multas-arriesga-el-ex-alcalde-san-fernando-luis-berwart/"/>
+    <hyperlink ref="T22" r:id="rId31" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U22" r:id="rId32" location="" tooltip="" display="https://www.df.cl/aniversario/caso-inverlink-el-escandalo-que-amenazo-la-estabilidad-del-mercado"/>
+    <hyperlink ref="T23" r:id="rId33" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="U23" r:id="rId34" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/07/06/1100220/fundacion-el-desarrollo-de-organizaciones.html"/>
+    <hyperlink ref="T24" r:id="rId35" location="" tooltip="" display="https://www.meganoticias.cl/amp/nacional/442953-mantencion-de-areas-verdes-alcalde-de-arica-firmo-trato-directo-por-1100-millones-con-empresa-creada-14-dias-antes.html"/>
+    <hyperlink ref="T25" r:id="rId36" location="" tooltip="" display="https://www.latercera.com/earlyaccess/noticia/las-millonarias-transacciones-que-complican-al-alcalde-de-rancagua/GY4SPWLFPJDODKTTXDN7FR74B4/"/>
+    <hyperlink ref="U25" r:id="rId37" location="" tooltip="" display="https://radio.uchile.cl/2023/03/04/tras-allanamiento-a-alcalde-de-rancagua-expertos-en-transparencia-llaman-a-fortalecer-los-mecanismos-para-perseguir-la-corrupcion/"/>
+    <hyperlink ref="V25" r:id="rId38" location="" tooltip="" display="https://www.meganoticias.cl/nacional/442934-alcalde-rancagua-formalizacion-abril-delitos-corrupcion-juan-ramon-godoy-21-03-2024.html"/>
+    <hyperlink ref="W25" r:id="rId39" location="" tooltip="" display="https://www.cde.cl/cde-interpone-querella-criminal-contra-el-alcalde-de-rancagua-por-delitos-asociados-a-hechos-de-corrupcion/"/>
+    <hyperlink ref="U26" r:id="rId40" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-la-araucania/2024/01/07/imputado-en-arista-caso-convenios-gobernador-de-la-araucania-luciano-rivas-confirma-su-repostulacion.shtml"/>
+    <hyperlink ref="V26" r:id="rId41" location="" tooltip="" display="https://www.cnnchile.com/pais/caso-convenios-fundacion-la-araucania-sueldo_20240901/"/>
+    <hyperlink ref="T27" r:id="rId42" location="" tooltip="" display="https://www.cnnchile.com/pais/destitucion-alcalde-rinconada-contraloria-irregularidades_20230606/"/>
+    <hyperlink ref="U27" r:id="rId43" location="" tooltip="" display="https://munirinconada.cl/alcalde-juan-galdames-se-refiere-a-juicio-de-cuentas-que-ordena-la-restitucion-de-300-millones/"/>
+    <hyperlink ref="T28" r:id="rId44" location="" tooltip="" display="https://www.chiletransparente.cl/caso-larrainvial/"/>
+    <hyperlink ref="T29" r:id="rId45" location="" tooltip="" display="https://www.ovejeronoticias.cl/2023/12/puerto-natales-ex-alcalde-udi-fernando-paredes-continua-con-reclusion-domiciliaria-total/"/>
+    <hyperlink ref="U29" r:id="rId46" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T30" r:id="rId47" location="" tooltip="" display="https://www.chiletransparente.cl/caso-luminarias/"/>
+    <hyperlink ref="T31" r:id="rId48" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T32" r:id="rId49" location="" tooltip="" display="https://www.t13.cl/noticia/politica/decretan-suspension-condicional-causa-malversacion-fondos-fundador-rd-21-12-2022"/>
+    <hyperlink ref="T33" r:id="rId50" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U33" r:id="rId51" location="" tooltip="" display="https://es.wikipedia.org/wiki/Corrupción_en_Chile#El_caso_MOP-GATE"/>
+    <hyperlink ref="T34" r:id="rId52" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T35" r:id="rId53" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="U35" r:id="rId54" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/08/04/fundacion-kimun-el-incumplido-contrato-por-1-200-millones/"/>
+    <hyperlink ref="T36" r:id="rId55" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/12/10/justicia-admite-querella-contra-alcaldesa-de-rio-bueno-por-malversacion-de-caudales-y-fraude-al-fisco.shtml"/>
+    <hyperlink ref="T37" r:id="rId56" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/judicial/denuncias-de-corrupcion/detenido-el-alcalde-de-algarrobo-se-entrego-frente-a-un-motel/2023-11-23/072824.html"/>
+    <hyperlink ref="T38" r:id="rId57" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="T39" r:id="rId58" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/03/19/milicogate-dictan-procesamiento-contra-general-y-coroneles-r-por-presunto-fraude-de-519-millones.shtml"/>
+    <hyperlink ref="T41" r:id="rId59" location="" tooltip="" display="https://www.meganoticias.cl/nacional/403342-contraloria-cifra-en-680-millones-posible-fraude-al-fisco-bajo-el-mandato-del-exintendente-guevara.html"/>
+    <hyperlink ref="U41" r:id="rId60" location="" tooltip="" display="https://cronicas.americatransparente.org/los-otros-programas-vita-41-mil-millones-transferidos-a-entidades-privadas-de-lo-barnechea/"/>
+    <hyperlink ref="V41" r:id="rId61" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/politica/contraloria-envio-a-fiscalia-caso-de-millonarios-contratos-con/2023-01-23/152629.html"/>
+    <hyperlink ref="T42" r:id="rId62" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="U42" r:id="rId63" location="" tooltip="" display="https://radio.uchile.cl/2023/11/18/cde-se-querello-contra-fundaciones-en-la-araucania-por-fraude-al-gore/"/>
+    <hyperlink ref="V42" r:id="rId64" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2023/12/29/caso-manicure/"/>
+    <hyperlink ref="T43" r:id="rId65" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/11/pdi-allano-gobernacion-del-maule-en-medio-de-investigaciones-por-traspasos-a-urbanismo-social.shtml"/>
+    <hyperlink ref="U43" r:id="rId66" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-maule/2024/03/12/caso-convenios-jefe-de-control-interno-del-gore-maule-declaro-por-traspasos-a-urbanismo-social.shtml"/>
+    <hyperlink ref="T44" r:id="rId67" location="" tooltip="" display="https://www.eldesconcierto.cl/reportajes/2024/01/23/municipio-se-querella-por-multa-de-500-millones-acusan-a-exalcalde-de-melipilla-por-fraude-al-fisco.html"/>
+    <hyperlink ref="U44" r:id="rId68" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/municipalidad-de-melipilla-presenta-querella-por-fraude-al-fisco-contra-el-exalcalde-ivan-campos/P6XRT2X73NAHJIEMIZWPRX6VEU/"/>
+    <hyperlink ref="T45" r:id="rId69" location="" tooltip="" display="https://www.elmostrador.cl/noticias/pais/2019/05/05/las-vueltas-de-la-vida-rn-elige-a-claudio-eguiluz-condenado-por-caso-sqm-como-su-presidente-regional-en-el-biobio/"/>
+    <hyperlink ref="T46" r:id="rId70" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="T47" r:id="rId71" location="" tooltip="" display="https://radionuevomundo.cl/2023/07/18/gobernador-rivas-suma-al-caso-fundacion-local-traspasos-arbitrarios-a-coihue-y-a-universidades-de-la-araucania/"/>
+    <hyperlink ref="U47" r:id="rId72" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
+    <hyperlink ref="V47" r:id="rId73" location="" tooltip="" display="https://resumen.cl/articulos/la-derecha-de-la-araucania-en-el-caso-fundaciones-las-irregularidades-de-espacio-coigue-que-llevaron-al-ministerio-de-justicia-a-solicitar-su-cierre"/>
+    <hyperlink ref="T48" r:id="rId74" location="" tooltip="" display="https://www.elmostrador.cl/dia/2023/03/31/exsubsecretaria-martorell-declaro-como-imputada-por-corrupcion-en-caso-motorola/"/>
+    <hyperlink ref="T49" r:id="rId75" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-del-bio-bio/2024/03/13/caso-convenios-allanan-empresa-que-facturo-356-millones-en-convenios-del-gore-bio-bio-y-bonhomia.shtml"/>
+    <hyperlink ref="U49" r:id="rId76" location="" tooltip="" display="https://resumen.cl/articulos/fundacion-contrato-con-dineros-del-gore-biobio-a-empresas-de-coordinador-de-programa-y-a-firma-donde-trabaja-su-hermano-y-su-madre-excandidata-republicana"/>
+    <hyperlink ref="V49" r:id="rId77" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-biobio/detienen-a-lider-de-empresa-en-allanamiento-por-caso-convenios-pdi/2024-03-13/123002.html"/>
+    <hyperlink ref="T50" r:id="rId78" location="" tooltip="" display="http://www.fiscaliadechile.cl/Fiscalia/sala_prensa/noticias_regional_det.do?id=22739"/>
+    <hyperlink ref="U50" r:id="rId79" location="" tooltip="" display="https://resumen.cl/articulos/exalcalde-pasara-10-anos-en-carcel-por-apropiarse-de-351-millones-de-la-municipalidad-y-de-empresa-electrica"/>
+    <hyperlink ref="T51" r:id="rId80" location="" tooltip="" display="https://www.24horas.cl/actualidad/politica/que-se-le-acusa-a-karina-oliva-emitir-boletas-falsas-defraudar-290-millones"/>
+    <hyperlink ref="T52" r:id="rId81" location="" tooltip="" display="https://www.fastcheck.cl/2021/11/18/yasna-provoste-se-robo-600-millones-de-dolares-del-ministerio-de-educacion-falso/"/>
+    <hyperlink ref="T53" r:id="rId82" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T55" r:id="rId83" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="T56" r:id="rId84" location="" tooltip="" display="https://radio.uchile.cl/2021/04/16/a-la-carcel-ex-senador-udi-jaime-orpis-es-condenado-a-prision-por-cohecho-y-fraude-al-fisco/"/>
+    <hyperlink ref="T57" r:id="rId85" location="" tooltip="" display="https://radio.uchile.cl/2023/11/28/755094/"/>
+    <hyperlink ref="U57" r:id="rId86" location="" tooltip="" display="https://elpais.com/chile/2023-08-05/caso-lenceria-la-telenovelesca-arista-de-la-trama-de-corrupcion-que-hace-temblar-la-politica-chilena.html"/>
+    <hyperlink ref="V57" r:id="rId87" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="T58" r:id="rId88" location="" tooltip="" display="https://www.ciperchile.cl/2023/05/10/caso-itelecom-detectan-66-pagos-en-efectivo-a-principal-asesor-de-german-codina-por-203-millones/"/>
+    <hyperlink ref="U58" r:id="rId89" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T59" r:id="rId90" location="" tooltip="" display="https://eltipografo.cl/2022/08/presentan-nueva-querella-por-fraude-al-fisco-contra-ex-alcalde-de-mostazal-sergio-medel-a"/>
+    <hyperlink ref="U59" r:id="rId91" location="" tooltip="" display="https://eltipografo.cl/2023/03/deficit-de-8-mil-millones-en-el-municipio-y-querellas-por-fraude-al-fisco-enfrenta-ex-alcalde-de-mostazal"/>
+    <hyperlink ref="V59" r:id="rId92" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-ohiggins/2022/08/11/municipio-prepara-querellas-tras-millonarias-irregularidades-en-san-francisco-de-mostazal.shtml"/>
+    <hyperlink ref="T60" r:id="rId93" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/29/quien-es-daniel-agusto-perez-el-exalcalde-formalizado-por-fraude-al-fisco/"/>
+    <hyperlink ref="U60" r:id="rId94" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-antofagasta/2024/01/24/son-11-casos-de-karen-rojo-formalizaron-a-exdelegado-de-pinera-en-antofagasta-por-fraude-al-fisco.shtml"/>
+    <hyperlink ref="T61" r:id="rId95" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T62" r:id="rId96" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/exalcalde-de-nunoa-andres-zarhi-queda-con-arresto-domiciliario-nocturno-tras-formalizacion-por-fraude-al-fisco/64LJ53FVUJA4BIGCC4DMKIJWRU/"/>
+    <hyperlink ref="U62" r:id="rId97" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/27/1123065/decretan-arresto-domiciliario-nocturno-andreszarhi.html"/>
+    <hyperlink ref="T63" r:id="rId98" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-del-maule/contraloria-ordeno-sumarios-contra-municipio-de-linares-rincon-acusa/2022-06-22/174906.html"/>
+    <hyperlink ref="T64" r:id="rId99" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/caso-convenios-ministerio-publico-indaga-traspasos-a-fundaciones-por-mas-de-14-mil-millones-en-ocho-regiones/XUWDKEDIWNDXTOU3RCMSIVQZE4/"/>
+    <hyperlink ref="U64" r:id="rId100" location="" tooltip="" display="https://www.meganoticias.cl/nacional/420687-nexos-politicos-gore-arica-fundacion-comprometidos-280-millones-25-7-2023.html"/>
+    <hyperlink ref="T65" r:id="rId101" location="" tooltip="" display="https://www.theclinic.cl/2024/02/27/pdi-acorrala-al-circulo-de-virginia-reginato-udi-acusa-a-exadministrador-municipal-de-millonarios-gastos-en-restaurantes-y-licorerias/"/>
+    <hyperlink ref="U65" r:id="rId102" location="" tooltip="" display="https://www.soychile.cl/valparaiso/sociedad/2024/01/22/844669/formalizacion-vina-boisier-fisco-reacciones.html"/>
+    <hyperlink ref="T66" r:id="rId103" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
+    <hyperlink ref="T67" r:id="rId104" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
+    <hyperlink ref="U67" r:id="rId105" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
+    <hyperlink ref="T68" r:id="rId106" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
+    <hyperlink ref="T69" r:id="rId107" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T70" r:id="rId108" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
+    <hyperlink ref="T71" r:id="rId109" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
+    <hyperlink ref="T72" r:id="rId110" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U72" r:id="rId111" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
+    <hyperlink ref="T73" r:id="rId112" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
+    <hyperlink ref="T75" r:id="rId113" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
+    <hyperlink ref="U75" r:id="rId114" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
+    <hyperlink ref="V75" r:id="rId115" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
+    <hyperlink ref="T76" r:id="rId116" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U76" r:id="rId117" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
+    <hyperlink ref="T77" r:id="rId118" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
+    <hyperlink ref="T78" r:id="rId119" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
+    <hyperlink ref="U78" r:id="rId120" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/04/02/fiscalia-formalizara-a-daniel-jadue-por-cohecho-administracion-desleal-fraude-al-fisco-y-estafa.shtml"/>
+    <hyperlink ref="T79" r:id="rId121" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T81" r:id="rId122" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="U81" r:id="rId123" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
+    <hyperlink ref="V81" r:id="rId124" location="" tooltip="" display="https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/"/>
+    <hyperlink ref="T82" r:id="rId125" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
+    <hyperlink ref="U82" r:id="rId126" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
+    <hyperlink ref="T83" r:id="rId127" location="" tooltip="" display="https://www.latercera.com/opinion/noticia/columna-de-daniel-matamala-cual-elefante/EOAKP2PXWJHSFDBAKRXGVVS5ZA/"/>
+    <hyperlink ref="T84" r:id="rId128" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/formalizan-a-exdirector-general-de-la-pdi-hector-espinosa-fiscalia-le-imputa-apropiacion-de-dineros-de-gastos-reservados-de-la-institucion/IBGS7P3IPVGU3MQU4A7GJDH4UA/"/>
+    <hyperlink ref="U84" r:id="rId129" location="" tooltip="" display="https://www.chvnoticias.cl/exclusivo-chv/todas-las-pruebas-fiscalia-hector-espinosa-pdi_20220828/"/>
+    <hyperlink ref="T85" r:id="rId130" location="" tooltip="" display="https://www.latercera.com/campuslt/noticia/luminarias-juzgado-de-garantia-de-iquique-condena-a-exconcejal-felipe-arenas-por-fraude-al-fisco-y-cohecho/OR3BBHZLARCULI7J5A22A66CSU/"/>
+    <hyperlink ref="U85" r:id="rId131" location="" tooltip="" display="https://iquiquetv.cl/2024/07/02/caso-luminarias-led-condenan-a-ex-concejal-felipe-arenas-por-cohecho-y-fraude-al-fisco/"/>
+    <hyperlink ref="V86" r:id="rId132" location="" tooltip="" display="https://www.meganoticias.cl/nacional/415393-cuentas-corrientes-empresario-acusado-pagar-sobornos-involucra-fraude-70-municipios-28-05-2023.html"/>
+    <hyperlink ref="T88" r:id="rId133" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
gráfico nuevo en app
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="510">
   <si>
     <t>Caso</t>
   </si>
@@ -2500,6 +2500,88 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t>https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html</t>
+    </r>
+  </si>
+  <si>
+    <t>Caso Convenios (Fundación ProCultura)</t>
+  </si>
+  <si>
+    <t>Alberto Larraín</t>
+  </si>
+  <si>
+    <t>Fundación ProCultura</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.latercera.com/earlyaccess/noticia/pintar-fachadas-turismo-creativo-y-ayuda-contra-el-suicidio-los-diversos-rubros-de-procultura-la-fundacion-con-mas-convenios-en-la-mira-de-fiscalia/PE7YFQCVMBAOTPHJPTUBEHVPUU/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.ex-ante.cl/perfil-lo-que-hay-que-saber-de-alberto-larrain-sus-vinculos-politicos-y-las-indagaciones-a-la-fundacion-procultura-que-creo/</t>
+    </r>
+  </si>
+  <si>
+    <t>Daniel Jadue, Farmacias Populares</t>
+  </si>
+  <si>
+    <t>cohecho, administración desleal, fraude al Fisco, estafa</t>
+  </si>
+  <si>
+    <t>arresto domiciliario</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.latercera.com/nacional/noticia/mas-de-200-millones-para-sanar-deudas-de-achifarp-y-pagos-a-funcionarios-fantasma-los-hitos-que-marcaron-el-primer-dia-de-formalizacion-del-alcalde-de-recoleta/YGFDCRRVJNFSXAA7KWM3YEIIUQ/</t>
+    </r>
+  </si>
+  <si>
+    <t>Alcalde de de La Higuera (Yerko Galleguillos)</t>
+  </si>
+  <si>
+    <t>Yerko Galleguillos</t>
+  </si>
+  <si>
+    <t>La Higuera</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.elcomunal.cl/comunales/2024/03/25/15-demandas-1-querella-y-17-solicitudes-de-arresto-por-deudas-de-1500-millones-del-municipio-de-la-higuera-sacuden-a-yerko-galleguillos/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://www.elcomunal.cl/comunales/2024/10/04/contraloria-detecta-graves-irregularidades-en-municipalidad-de-la-higuera-y-envia-antecedentes-a-fiscalia/</t>
     </r>
   </si>
 </sst>
@@ -2696,7 +2778,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2792,6 +2874,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3869,7 +3954,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:X90"/>
+  <dimension ref="A1:X94"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -8368,8 +8453,184 @@
       <c r="W90" s="27"/>
       <c r="X90" s="27"/>
     </row>
+    <row r="91" ht="20.35" customHeight="1">
+      <c r="A91" t="s" s="21">
+        <v>496</v>
+      </c>
+      <c r="B91" s="22">
+        <v>500000000</v>
+      </c>
+      <c r="C91" s="23">
+        <v>2023</v>
+      </c>
+      <c r="D91" t="s" s="25">
+        <v>497</v>
+      </c>
+      <c r="E91" t="s" s="25">
+        <v>163</v>
+      </c>
+      <c r="F91" s="26"/>
+      <c r="G91" s="26"/>
+      <c r="H91" s="26"/>
+      <c r="I91" s="26"/>
+      <c r="J91" t="s" s="25">
+        <v>13</v>
+      </c>
+      <c r="K91" s="26"/>
+      <c r="L91" s="26"/>
+      <c r="M91" s="26"/>
+      <c r="N91" t="s" s="28">
+        <v>498</v>
+      </c>
+      <c r="O91" s="27"/>
+      <c r="P91" t="s" s="28">
+        <v>91</v>
+      </c>
+      <c r="Q91" s="26"/>
+      <c r="R91" s="17"/>
+      <c r="S91" s="26"/>
+      <c r="T91" t="s" s="28">
+        <v>499</v>
+      </c>
+      <c r="U91" t="s" s="28">
+        <v>500</v>
+      </c>
+      <c r="V91" s="27"/>
+      <c r="W91" s="27"/>
+      <c r="X91" s="27"/>
+    </row>
+    <row r="92" ht="20.35" customHeight="1">
+      <c r="A92" t="s" s="21">
+        <v>501</v>
+      </c>
+      <c r="B92" s="22">
+        <v>200000000</v>
+      </c>
+      <c r="C92" s="23">
+        <v>2024</v>
+      </c>
+      <c r="D92" t="s" s="25">
+        <v>458</v>
+      </c>
+      <c r="E92" t="s" s="25">
+        <v>163</v>
+      </c>
+      <c r="F92" t="s" s="25">
+        <v>459</v>
+      </c>
+      <c r="G92" s="23">
+        <v>2019</v>
+      </c>
+      <c r="H92" s="23">
+        <v>2024</v>
+      </c>
+      <c r="I92" t="s" s="25">
+        <v>420</v>
+      </c>
+      <c r="J92" t="s" s="16">
+        <v>29</v>
+      </c>
+      <c r="K92" s="26"/>
+      <c r="L92" s="26"/>
+      <c r="M92" s="26"/>
+      <c r="N92" s="27"/>
+      <c r="O92" t="s" s="28">
+        <v>502</v>
+      </c>
+      <c r="P92" s="27"/>
+      <c r="Q92" s="26"/>
+      <c r="R92" s="17"/>
+      <c r="S92" t="s" s="25">
+        <v>503</v>
+      </c>
+      <c r="T92" t="s" s="28">
+        <v>504</v>
+      </c>
+      <c r="U92" s="27"/>
+      <c r="V92" s="27"/>
+      <c r="W92" s="27"/>
+      <c r="X92" s="27"/>
+    </row>
+    <row r="93" ht="32.35" customHeight="1">
+      <c r="A93" t="s" s="21">
+        <v>505</v>
+      </c>
+      <c r="B93" s="22">
+        <v>1700000000</v>
+      </c>
+      <c r="C93" s="23">
+        <v>2024</v>
+      </c>
+      <c r="D93" t="s" s="25">
+        <v>506</v>
+      </c>
+      <c r="E93" t="s" s="25">
+        <v>26</v>
+      </c>
+      <c r="F93" t="s" s="25">
+        <v>27</v>
+      </c>
+      <c r="G93" s="23">
+        <v>2022</v>
+      </c>
+      <c r="H93" s="23">
+        <v>2024</v>
+      </c>
+      <c r="I93" t="s" s="25">
+        <v>507</v>
+      </c>
+      <c r="J93" t="s" s="25">
+        <v>29</v>
+      </c>
+      <c r="K93" s="26"/>
+      <c r="L93" s="26"/>
+      <c r="M93" s="26"/>
+      <c r="N93" s="27"/>
+      <c r="O93" t="s" s="28">
+        <v>189</v>
+      </c>
+      <c r="P93" s="27"/>
+      <c r="Q93" s="26"/>
+      <c r="R93" s="17"/>
+      <c r="S93" s="26"/>
+      <c r="T93" t="s" s="28">
+        <v>508</v>
+      </c>
+      <c r="U93" t="s" s="28">
+        <v>509</v>
+      </c>
+      <c r="V93" s="27"/>
+      <c r="W93" s="27"/>
+      <c r="X93" s="27"/>
+    </row>
+    <row r="94" ht="20.35" customHeight="1">
+      <c r="A94" s="32"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="26"/>
+      <c r="D94" s="26"/>
+      <c r="E94" s="26"/>
+      <c r="F94" s="26"/>
+      <c r="G94" s="26"/>
+      <c r="H94" s="26"/>
+      <c r="I94" s="26"/>
+      <c r="J94" s="26"/>
+      <c r="K94" s="26"/>
+      <c r="L94" s="26"/>
+      <c r="M94" s="26"/>
+      <c r="N94" s="27"/>
+      <c r="O94" s="27"/>
+      <c r="P94" s="27"/>
+      <c r="Q94" s="26"/>
+      <c r="R94" s="17"/>
+      <c r="S94" s="26"/>
+      <c r="T94" s="27"/>
+      <c r="U94" s="27"/>
+      <c r="V94" s="27"/>
+      <c r="W94" s="27"/>
+      <c r="X94" s="27"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C12 E1:E12 G1:H11 H12 C13:C15 E13:E15 G13:H14 H15 C16:C32 E16:E32 G16:H31 H32 C33:C42 E33:E42 G33:H41 H42 C43:C54 E43:E54 G43:H53 H54 C55:C57 E55:E57 G55:H56 H57 C58:C64 E58:E64 G58:H63 H64 C65:C66 E65:E66 G65:H65 H66 C67:C71 E67:E71 G67:H70 H71:H72 C72:C75 E72:E75 G73:H74 H75 C76:C78 E76:E78 G76:H77 H78:H79 C79:C85 E79:E85 G80:H84 H85 C86:C90 E86:E90 G86:H90">
+  <conditionalFormatting sqref="C1:C12 E1:E12 G1:H11 H12 C13:C15 E13:E15 G13:H14 H15 C16:C32 E16:E32 G16:H31 H32 C33:C42 E33:E42 G33:H41 H42 C43:C54 E43:E54 G43:H53 H54 C55:C57 E55:E57 G55:H56 H57 C58:C64 E58:E64 G58:H63 H64 C65:C66 E65:E66 G65:H65 H66 C67:C71 E67:E71 G67:H70 H71:H72 C72:C75 E72:E75 G73:H74 H75 C76:C78 E76:E78 G76:H77 H78:H79 C79:C85 E79:E85 G80:H84 H85 C86:C94 E86:E94 G86:H94">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -8521,6 +8782,11 @@
     <hyperlink ref="U87" r:id="rId141" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
     <hyperlink ref="V88" r:id="rId142" location="" tooltip="" display="https://www.meganoticias.cl/nacional/415393-cuentas-corrientes-empresario-acusado-pagar-sobornos-involucra-fraude-70-municipios-28-05-2023.html"/>
     <hyperlink ref="T90" r:id="rId143" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
+    <hyperlink ref="T91" r:id="rId144" location="" tooltip="" display="https://www.latercera.com/earlyaccess/noticia/pintar-fachadas-turismo-creativo-y-ayuda-contra-el-suicidio-los-diversos-rubros-de-procultura-la-fundacion-con-mas-convenios-en-la-mira-de-fiscalia/PE7YFQCVMBAOTPHJPTUBEHVPUU/"/>
+    <hyperlink ref="U91" r:id="rId145" location="" tooltip="" display="https://www.ex-ante.cl/perfil-lo-que-hay-que-saber-de-alberto-larrain-sus-vinculos-politicos-y-las-indagaciones-a-la-fundacion-procultura-que-creo/"/>
+    <hyperlink ref="T92" r:id="rId146" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/mas-de-200-millones-para-sanar-deudas-de-achifarp-y-pagos-a-funcionarios-fantasma-los-hitos-que-marcaron-el-primer-dia-de-formalizacion-del-alcalde-de-recoleta/YGFDCRRVJNFSXAA7KWM3YEIIUQ/"/>
+    <hyperlink ref="T93" r:id="rId147" location="" tooltip="" display="https://www.elcomunal.cl/comunales/2024/03/25/15-demandas-1-querella-y-17-solicitudes-de-arresto-por-deudas-de-1500-millones-del-municipio-de-la-higuera-sacuden-a-yerko-galleguillos/"/>
+    <hyperlink ref="U93" r:id="rId148" location="" tooltip="" display="https://www.elcomunal.cl/comunales/2024/10/04/contraloria-detecta-graves-irregularidades-en-municipalidad-de-la-higuera-y-envia-antecedentes-a-fiscalia/"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
correccion bug scroll, enlace de fuente malo, datos perdidos en tabla
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -2331,23 +2331,7 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve"> El Tribunal,el marco del caso denominado</t>
-    </r>
+    <t>https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/</t>
   </si>
   <si>
     <t>Caso Cuentas Corrientes, Municipalidad de Río Bueno</t>
@@ -10044,51 +10028,50 @@
     <hyperlink ref="U78" r:id="rId131" location="" tooltip="" display="https://www.elsancarlino.cl/2024/06/contraloria-detecta-dos-nuevos.html"/>
     <hyperlink ref="T79" r:id="rId132" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-atacama/2020/08/01/alcalde-suplente-tierra-amarilla-quedo-prision-preventiva-tras-formalizacion-fraudes.shtml"/>
     <hyperlink ref="T80" r:id="rId133" location="" tooltip="" display="https://www.diarioconstitucional.cl/2023/06/20/ex-administrador-municipal-que-aprobo-el-financiamiento-para-que-alcalde-concejales-y-funcionarios-publicos-de-tierra-amarilla-emprendieran-viaje-turistico-a-la-habana-y-varadero-incurre-en-el-delit/"/>
-    <hyperlink ref="U80" r:id="rId134" location="" tooltip="" display="https://www.cde.cl/cde-valora-condena-a-exadministrador-municipal-de-tierra-amarilla-en-caso-concejales-on-tour/#:~:text=(23.03.2023)"/>
-    <hyperlink ref="T81" r:id="rId135" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2024/02/15/cuentas-corrientes-rio-bueno-debera-restituir-76-millones-por-pagos-improcedentes-a-gestion-global.shtml"/>
-    <hyperlink ref="U81" r:id="rId136" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/09/24/caso-cuentas-corrientes-exalcalde-de-rio-bueno-declara-en-fiscalia-por-contratacion-de-gestion-global.shtml"/>
-    <hyperlink ref="T82" r:id="rId137" location="" tooltip="" display="https://www.canal9.cl/episodios/noticias/2024/07/26/alcalde-de-coronel-y-concejal-araya-seran-formalizados-por-caso-puerto-coronel"/>
-    <hyperlink ref="U82" r:id="rId138" location="" tooltip="" display="https://www.cooperativa.cl/noticias/pais/region-del-biobio/formalizaran-por-delitos-de-corrupcion-al-alcalde-de-coronel-y-a-otras/2024-07-26/084551.html"/>
-    <hyperlink ref="V82" r:id="rId139" location="" tooltip="" display="https://www.meganoticias.cl/nacional/459252-querella-alcalde-coronel-boris-chamorro-cohecho-pago-coimas-17-09-2024.html"/>
-    <hyperlink ref="W82" r:id="rId140" location="" tooltip="" display="https://sabes.cl/2024/09/17/cde-se-suma-al-caso-puerto-coronel-se-querella-contra-alcalde-boris-chamorro-por-delitos-ligados-a-corrupcion/"/>
-    <hyperlink ref="T83" r:id="rId141" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
-    <hyperlink ref="T84" r:id="rId142" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T85" r:id="rId143" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/contraloria-detecta-dos-nuevos-municipios-involucrados-en-el-caso-cuentas-corrientes-y-deriva-antecedentes-a-la-fiscalia/5C3ZRUU3WFF4BFYSN4BG4GD7QE/"/>
-    <hyperlink ref="T86" r:id="rId144" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
-    <hyperlink ref="T87" r:id="rId145" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
-    <hyperlink ref="T88" r:id="rId146" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U88" r:id="rId147" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
-    <hyperlink ref="T89" r:id="rId148" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
-    <hyperlink ref="T91" r:id="rId149" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
-    <hyperlink ref="U91" r:id="rId150" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
-    <hyperlink ref="V91" r:id="rId151" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
-    <hyperlink ref="T92" r:id="rId152" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
-    <hyperlink ref="U92" r:id="rId153" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
-    <hyperlink ref="T93" r:id="rId154" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
-    <hyperlink ref="T94" r:id="rId155" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-lagos/2023/09/13/causa-por-corrupcion-y-lavado-de-activos-fiscal-explica-allanamiento-en-municipio-de-puerto-montt.shtml"/>
-    <hyperlink ref="U94" r:id="rId156" location="" tooltip="" display="https://www.diariodepuertomontt.cl/noticia/politica/2024/08/ter-ordena-la-remocion-del-alcalde-de-puerto-montt"/>
-    <hyperlink ref="V94" r:id="rId157" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/08/23/1140650/remueven-alcalde-de-puerto-montt.html"/>
-    <hyperlink ref="W94" r:id="rId158" location="" tooltip="" display="https://www.24horas.cl/regiones/zona-sur/los-lagos/alcalde-de-puerto-montt-destituido-notable-abandono-deberes"/>
-    <hyperlink ref="T95" r:id="rId159" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
-    <hyperlink ref="U95" r:id="rId160" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/04/02/fiscalia-formalizara-a-daniel-jadue-por-cohecho-administracion-desleal-fraude-al-fisco-y-estafa.shtml"/>
-    <hyperlink ref="T96" r:id="rId161" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
-    <hyperlink ref="T98" r:id="rId162" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
-    <hyperlink ref="U98" r:id="rId163" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
-    <hyperlink ref="V98" r:id="rId164" location="" tooltip="" display="https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/"/>
-    <hyperlink ref="T99" r:id="rId165" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/07/10/1136142/suprema-revoca-prision-preventiva.html"/>
-    <hyperlink ref="U99" r:id="rId166" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/06/07/1133101/cronologia-delitos-fiscal-puerto-natales.html"/>
-    <hyperlink ref="T100" r:id="rId167" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
-    <hyperlink ref="U100" r:id="rId168" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
-    <hyperlink ref="V101" r:id="rId169" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/10/15/cuentas-corrientes-tesorero-municipal-acusado-de-cohecho-logra-salida-alternativa-tras-donar-200-mil.shtml"/>
-    <hyperlink ref="W101" r:id="rId170" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/25/causa-por-corrupcion-mantienen-prision-preventiva-para-alcalde-de-san-ignacio-y-un-operador-politico.shtml"/>
-    <hyperlink ref="U102" r:id="rId171" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
-    <hyperlink ref="T103" r:id="rId172" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
-    <hyperlink ref="U103" r:id="rId173" location="" tooltip="" display="https://radio.uchile.cl/2024/02/13/caso-cuentas-corrientes-detienen-a-alcalde-de-bulnes-por-delitos-economicos/"/>
-    <hyperlink ref="T104" r:id="rId174" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/19/ex-udi-y-exasesor-de-sauerbaum-quien-es-el-operador-politico-investigado-por-corrupcion-en-nuble.shtml"/>
-    <hyperlink ref="U104" r:id="rId175" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/25/causa-por-corrupcion-mantienen-prision-preventiva-para-alcalde-de-san-ignacio-y-un-operador-politico.shtml"/>
-    <hyperlink ref="T105" r:id="rId176" location="" tooltip="" display="https://www.elciudadano.com/reportaje-investigacion/fue-funcionario-de-confianza-de-felipe-alessandri-fiscalia-investiga-a-diputado-republicano-agustin-romero-por-fraude-al-fisco/03/07/"/>
-    <hyperlink ref="U105" r:id="rId177" location="" tooltip="" display="https://www.cooperativa.cl/noticias/pais/judicial/justicia-designo-a-ministra-de-fuero-para-cobrar-pago-de-horas-extras-a/2023-11-27/155546.html"/>
-    <hyperlink ref="V105" r:id="rId178" location="" tooltip="" display="https://interferencia.cl/articulos/corte-designa-ministra-de-fuero-para-cobrar-11-millones-que-diputado-republicano-recibio"/>
+    <hyperlink ref="T81" r:id="rId134" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2024/02/15/cuentas-corrientes-rio-bueno-debera-restituir-76-millones-por-pagos-improcedentes-a-gestion-global.shtml"/>
+    <hyperlink ref="U81" r:id="rId135" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-rios/2023/09/24/caso-cuentas-corrientes-exalcalde-de-rio-bueno-declara-en-fiscalia-por-contratacion-de-gestion-global.shtml"/>
+    <hyperlink ref="T82" r:id="rId136" location="" tooltip="" display="https://www.canal9.cl/episodios/noticias/2024/07/26/alcalde-de-coronel-y-concejal-araya-seran-formalizados-por-caso-puerto-coronel"/>
+    <hyperlink ref="U82" r:id="rId137" location="" tooltip="" display="https://www.cooperativa.cl/noticias/pais/region-del-biobio/formalizaran-por-delitos-de-corrupcion-al-alcalde-de-coronel-y-a-otras/2024-07-26/084551.html"/>
+    <hyperlink ref="V82" r:id="rId138" location="" tooltip="" display="https://www.meganoticias.cl/nacional/459252-querella-alcalde-coronel-boris-chamorro-cohecho-pago-coimas-17-09-2024.html"/>
+    <hyperlink ref="W82" r:id="rId139" location="" tooltip="" display="https://sabes.cl/2024/09/17/cde-se-suma-al-caso-puerto-coronel-se-querella-contra-alcalde-boris-chamorro-por-delitos-ligados-a-corrupcion/"/>
+    <hyperlink ref="T83" r:id="rId140" location="" tooltip="" display="https://www.latercera.com/politica/noticia/caso-penta-ex-subsecretario-pablo-wagner-condenado-delitos-tributarios-absuelto-cohecho/233126/"/>
+    <hyperlink ref="T84" r:id="rId141" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T85" r:id="rId142" location="" tooltip="" display="https://www.latercera.com/nacional/noticia/contraloria-detecta-dos-nuevos-municipios-involucrados-en-el-caso-cuentas-corrientes-y-deriva-antecedentes-a-la-fiscalia/5C3ZRUU3WFF4BFYSN4BG4GD7QE/"/>
+    <hyperlink ref="T86" r:id="rId143" location="" tooltip="" display="https://www.chiletransparente.cl/caso-ceresita/"/>
+    <hyperlink ref="T87" r:id="rId144" location="" tooltip="" display="https://www.diarioviregion.cl/index.php/noticias/27551-ex-alcalde-de-san-fernando-juan-paulo-molina-condenado-por-fraude-al-fisco-reiterado"/>
+    <hyperlink ref="T88" r:id="rId145" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U88" r:id="rId146" location="" tooltip="" display="https://es.wikipedia.org/wiki/Caso_Coimas"/>
+    <hyperlink ref="T89" r:id="rId147" location="" tooltip="" display="https://www.latercera.com/reportajes/noticia/la-excesiva-demora-contraloria-salvo-josefa-errazuriz/613135/"/>
+    <hyperlink ref="T91" r:id="rId148" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/ex-alcaldesa-karen-rojo-condenada-a-cinco-anos-de-carcel-por-fraude-al/2022-03-24/135330.html"/>
+    <hyperlink ref="U91" r:id="rId149" location="" tooltip="" display="https://cooperativa.cl/noticias/pais/region-de-antofagasta/suprema-rechazo-recurso-de-nulidad-y-karen-rojo-debera-cumplir-pena-en/2022-03-23/155942.html"/>
+    <hyperlink ref="V91" r:id="rId150" location="" tooltip="" display="https://chile.as.com/actualidad/detencion-de-karen-rojo-a-que-partido-pertenecia-cuanto-dinero-robo-y-por-que-estaba-en-holanda-n/"/>
+    <hyperlink ref="T92" r:id="rId151" location="" tooltip="" display="https://www.biobiochile.cl/noticias/2015/01/24/cinco-casos-de-corrupcion-que-mancharon-la-politica-antes-de-penta-en-los-ultimos-15-anos.shtml"/>
+    <hyperlink ref="U92" r:id="rId152" location="" tooltip="" display="https://www.emol.com/noticias/nacional/2014/10/23/686503/caso-efe-corte-ratifica-condena-en-contra-de-luis-ajenjo-por-fraude-al-fisco.html"/>
+    <hyperlink ref="T93" r:id="rId153" location="" tooltip="" display="https://www.eldinamo.cl/pais/2013/08/28/sol-letelier-uso-23-millones-de-pesos-de-recoleta-para-su-campana-municipal/"/>
+    <hyperlink ref="T94" r:id="rId154" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-los-lagos/2023/09/13/causa-por-corrupcion-y-lavado-de-activos-fiscal-explica-allanamiento-en-municipio-de-puerto-montt.shtml"/>
+    <hyperlink ref="U94" r:id="rId155" location="" tooltip="" display="https://www.diariodepuertomontt.cl/noticia/politica/2024/08/ter-ordena-la-remocion-del-alcalde-de-puerto-montt"/>
+    <hyperlink ref="V94" r:id="rId156" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/08/23/1140650/remueven-alcalde-de-puerto-montt.html"/>
+    <hyperlink ref="W94" r:id="rId157" location="" tooltip="" display="https://www.24horas.cl/regiones/zona-sur/los-lagos/alcalde-de-puerto-montt-destituido-notable-abandono-deberes"/>
+    <hyperlink ref="T95" r:id="rId158" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2023/11/15/1112897/daniel-jadue-declaracion-farmacias-populares.html"/>
+    <hyperlink ref="U95" r:id="rId159" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/chile/2024/04/02/fiscalia-formalizara-a-daniel-jadue-por-cohecho-administracion-desleal-fraude-al-fisco-y-estafa.shtml"/>
+    <hyperlink ref="T96" r:id="rId160" location="" tooltip="" display="https://www.elciudadano.com/politica/los-18-emblematicos-alcaldes-corruptos-de-la-derecha-historias-de-un-tsunami-delictual/06/22/"/>
+    <hyperlink ref="T98" r:id="rId161" location="" tooltip="" display="https://www.malaespinacheck.cl/pais/2024/01/03/los-14-detenidos-en-todo-chile-por-el-caso-convenios/"/>
+    <hyperlink ref="U98" r:id="rId162" location="" tooltip="" display="https://www.elciudadano.com/actualidad/el-entramado-de-ilicitos-de-platas-que-exploto-en-el-gore-araucania-y-que-repercute-en-renovacion-nacional/12/29/"/>
+    <hyperlink ref="V98" r:id="rId163" location="" tooltip="" display="https://elperiodico.cl/contraloria-corrobora-participacion-de-exfuncionaria-del-gore-araucania-en-comision-que-aprobo-proyecto-de-fundacion-que-posteriormente-la-contrato/"/>
+    <hyperlink ref="T99" r:id="rId164" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/07/10/1136142/suprema-revoca-prision-preventiva.html"/>
+    <hyperlink ref="U99" r:id="rId165" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/06/07/1133101/cronologia-delitos-fiscal-puerto-natales.html"/>
+    <hyperlink ref="T100" r:id="rId166" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/20/1122268/contraloria-caso-convenios-minvu-serviu.html"/>
+    <hyperlink ref="U100" r:id="rId167" location="" tooltip="" display="https://www.ex-ante.cl/confidencial-las-47-fundaciones-indagadas-por-justicia-en-el-caso-convenios/"/>
+    <hyperlink ref="V101" r:id="rId168" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/10/15/cuentas-corrientes-tesorero-municipal-acusado-de-cohecho-logra-salida-alternativa-tras-donar-200-mil.shtml"/>
+    <hyperlink ref="W101" r:id="rId169" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/25/causa-por-corrupcion-mantienen-prision-preventiva-para-alcalde-de-san-ignacio-y-un-operador-politico.shtml"/>
+    <hyperlink ref="U102" r:id="rId170" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
+    <hyperlink ref="T103" r:id="rId171" location="" tooltip="" display="https://www.emol.com/noticias/Nacional/2024/02/15/1121826/caso-cuentas-corrientes.html"/>
+    <hyperlink ref="U103" r:id="rId172" location="" tooltip="" display="https://radio.uchile.cl/2024/02/13/caso-cuentas-corrientes-detienen-a-alcalde-de-bulnes-por-delitos-economicos/"/>
+    <hyperlink ref="T104" r:id="rId173" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/19/ex-udi-y-exasesor-de-sauerbaum-quien-es-el-operador-politico-investigado-por-corrupcion-en-nuble.shtml"/>
+    <hyperlink ref="U104" r:id="rId174" location="" tooltip="" display="https://www.biobiochile.cl/noticias/nacional/region-de-nuble/2023/04/25/causa-por-corrupcion-mantienen-prision-preventiva-para-alcalde-de-san-ignacio-y-un-operador-politico.shtml"/>
+    <hyperlink ref="T105" r:id="rId175" location="" tooltip="" display="https://www.elciudadano.com/reportaje-investigacion/fue-funcionario-de-confianza-de-felipe-alessandri-fiscalia-investiga-a-diputado-republicano-agustin-romero-por-fraude-al-fisco/03/07/"/>
+    <hyperlink ref="U105" r:id="rId176" location="" tooltip="" display="https://www.cooperativa.cl/noticias/pais/judicial/justicia-designo-a-ministra-de-fuero-para-cobrar-pago-de-horas-extras-a/2023-11-27/155546.html"/>
+    <hyperlink ref="V105" r:id="rId177" location="" tooltip="" display="https://interferencia.cl/articulos/corte-designa-ministra-de-fuero-para-cobrar-11-millones-que-diputado-republicano-recibio"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
mantención gráficos, datos nuevos
</commit_message>
<xml_diff>
--- a/datos/casos_corrupcion_chile.xlsx
+++ b/datos/casos_corrupcion_chile.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="712">
   <si>
     <t>Caso</t>
   </si>
@@ -3736,6 +3736,26 @@
         <rFont val="Helvetica"/>
       </rPr>
       <t>https://www.ciperchile.cl/2025/12/19/contraloria-revisa-trabajo-de-cecilia-perez-en-la-florida-solicita-devolucion-de-18-millones-por-labores-no-acreditadas/</t>
+    </r>
+  </si>
+  <si>
+    <t>Contratación irregular de Francisco Orrego</t>
+  </si>
+  <si>
+    <t>Francisco Orrego</t>
+  </si>
+  <si>
+    <t>Contratación Irregular</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t>https://contrapoderchile.cl/contraloria-confirma-que-francisco-orrego-devolvio-9-millones-a-la-municipalidad-de-la-florida-por-contratacion-irregular/</t>
     </r>
   </si>
 </sst>
@@ -5108,7 +5128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Y128"/>
+  <dimension ref="A1:Y129"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
@@ -11735,8 +11755,59 @@
       <c r="X128" s="26"/>
       <c r="Y128" s="26"/>
     </row>
+    <row r="129" ht="56.35" customHeight="1">
+      <c r="A129" t="s" s="13">
+        <v>708</v>
+      </c>
+      <c r="B129" s="14">
+        <v>9120775</v>
+      </c>
+      <c r="C129" s="15">
+        <v>2025</v>
+      </c>
+      <c r="D129" t="s" s="17">
+        <v>709</v>
+      </c>
+      <c r="E129" t="s" s="17">
+        <v>27</v>
+      </c>
+      <c r="F129" t="s" s="17">
+        <v>57</v>
+      </c>
+      <c r="G129" s="15">
+        <v>2025</v>
+      </c>
+      <c r="H129" s="15">
+        <v>2025</v>
+      </c>
+      <c r="I129" t="s" s="17">
+        <v>132</v>
+      </c>
+      <c r="J129" t="s" s="17">
+        <v>230</v>
+      </c>
+      <c r="K129" s="16"/>
+      <c r="L129" s="16"/>
+      <c r="M129" s="16"/>
+      <c r="N129" s="25"/>
+      <c r="O129" s="26"/>
+      <c r="P129" t="s" s="27">
+        <v>710</v>
+      </c>
+      <c r="Q129" s="27"/>
+      <c r="R129" s="25"/>
+      <c r="S129" s="26"/>
+      <c r="T129" s="26"/>
+      <c r="U129" t="s" s="24">
+        <v>711</v>
+      </c>
+      <c r="V129" s="26"/>
+      <c r="W129" s="26"/>
+      <c r="X129" s="26"/>
+      <c r="Y129" s="26"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C3 E1:E3 G1:H2 H3 C4:C12 E4:E12 G4:H11 H12 C13:C25 E13:E25 G13:H24 H25 C26:C37 E26:E37 G26:H36 H37 C38:C40 E38:E40 G38:H39 H40 C41:C44 E41:E44 G41:H43 H44 C45:C47 E45:E47 G45:H46 H47 C48:C71 E48:E71 G48:H70 H71 C72:C78 E72:E78 G72:H77 H78 C79:C82 E79:E82 G79:H81 H82 C83:C97 E83:E97 G83:H96 H97 C98:C106 E98:E106 G98:H105 H106:H107 C107:C117 E107:E117 G108:H116 H117 C118:C128 E118:E128 G118:H128">
+  <conditionalFormatting sqref="C1:C3 E1:E3 G1:H2 H3 C4:C12 E4:E12 G4:H11 H12 C13:C25 E13:E25 G13:H24 H25 C26:C37 E26:E37 G26:H36 H37 C38:C40 E38:E40 G38:H39 H40 C41:C44 E41:E44 G41:H43 H44 C45:C47 E45:E47 G45:H46 H47 C48:C71 E48:E71 G48:H70 H71 C72:C78 E72:E78 G72:H77 H78 C79:C82 E79:E82 G79:H81 H82 C83:C97 E83:E97 G83:H96 H97 C98:C106 E98:E106 G98:H105 H106:H107 C107:C117 E107:E117 G108:H116 H117 C118:C129 E118:E129 G118:H129">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal" stopIfTrue="1">
       <formula>"Izquierda"</formula>
     </cfRule>
@@ -11967,6 +12038,7 @@
     <hyperlink ref="U127" r:id="rId220" location="" tooltip="" display="https://contrapoderchile.cl/concejala-de-la-florida-rn-fue-contratada-en-el-municipio-de-santiago-y-ha-recibido-mas-de-8-millones-en-horas-extras/"/>
     <hyperlink ref="U128" r:id="rId221" location="" tooltip="" display="https://www.adnradio.cl/2025/12/19/golpe-a-la-gestion-carter-contraloria-pide-devolver-fondos-pagados-a-cecilia-perez-su-exmarido-y-su-cunada-en-la-florida/"/>
     <hyperlink ref="V128" r:id="rId222" location="" tooltip="" display="https://www.ciperchile.cl/2025/12/19/contraloria-revisa-trabajo-de-cecilia-perez-en-la-florida-solicita-devolucion-de-18-millones-por-labores-no-acreditadas/"/>
+    <hyperlink ref="U129" r:id="rId223" location="" tooltip="" display="https://contrapoderchile.cl/contraloria-confirma-que-francisco-orrego-devolvio-9-millones-a-la-municipalidad-de-la-florida-por-contratacion-irregular/"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>